<commit_message>
script final Marco de cooperación
</commit_message>
<xml_diff>
--- a/logos.xlsx
+++ b/logos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rinco\Documents\MarcoDeCooperacionColombia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB27C49-5D2D-4EFC-BED1-4FD1D541BFC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A28AB62-964F-4381-8C58-C11AFF28C4D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16200" yWindow="-2505" windowWidth="16200" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Agencia</t>
   </si>
@@ -42,9 +42,6 @@
     <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAFoAAABaCAYAAAA4qEECAAAUx0lEQVR4nO2dCXhU5bnHf2fWTJbJnskGIQsJhgRkR1BZBUUprnXhsUVRtFe9Veu1vXhVpGpbba9XrVUUl6rVWhQQuFUBWUVAQjAsIWxJyA7Zl0lmn/t83yQ0YABjZ064lP/z5HmYOTPvOec937zf+/7fBS5AHSiBPIvu3k8/ACYDznP8eeqBda7XZt0WqBPoAiW4E4mAJcDn8BcSAylcE+CLP9dXcncE9FoDregLuKBodXFB0SrhgqJVQqC9Dr/A7fHidXvA7QWP1ydSo4BWQdFq0GoC6qX6BeeUol1uDxqNgkbxKc7l8oDLQ4TZSHZCGJmWMMwGjdR3q8NFcV07+6taqG+2g1aDTq85IQcPJ16fCzgnFO3xePE43GQmmWmyuTjeYgOnmzRLGLeO7UdGbAg1zTYKK1uYONRCVYuNtYW1zMixcNdlA6hqsvH+1jIKy5pRDBpGpUZid7jZXdoEei06bd+v+D5VtDQJLg96rYYnrs8mSK9lwbJCtF546KosLk6JYGleJc+tKsLp9BCi15KTbObK3HjwKjy7qohj9e38aGQSC2YNYl9lK8+u2E9NXTsf3Duab8ubmf/xPlrtLhRd35qYQIfga4CpPR0Tq9io1TBjiIUbhicyJNnMuF9vkLvzUzfmUNXYwe9WFWEOMXLnhBQuy4jG5fGSGBEkTYtBq8Hm8vBxXgWfFdSQHh/G+Iwo0uJCmff6DlITwtj++ES+3F/L53uP8eZXZTg6TdNpsNb12qwrAqaLQAk+E7xiT3O4eeqWwQxPiSA5Mojff3FYbnQv3TmClIggfv7uLm4e3597Jqay5UAdv1paSGVNGzeOSWb9wXoqGtsZnx7FfVPTee6mHHaXt/Dokj3MGd+ft+4dzby381m46gA3j0xi7mUpRIYYePrjfSihhsCurtNAG0jhmpG3/gRI6/6e8Bncbg9jB0bz2NWZbDhQR5vDhc3pZviASLYdaaDO6mDxncMxm/TMeyOPDQfruWFkEreM68eU7FgyLGGYgnSU13fwwfYKLs+M4ZL0KK4aEs/Ml7cSYtRxZa6FDqebcJOBLUcaufvSFMpabOwrb0aj7XGTLPbk/fW9gOkiUIJPB7fLQ1Z8GFcPicfm9EiTkRkXytE6K+ZgPR9vKKHN5sLjAaNOw7RcC4vnDpc/g+eXFbKjuFF+Nm/fcWnD35k7gs2H69le0kiESU9ihInffLKP/tEmKurb0Shehiab5WY6e2w/cvtH4HJ61L7tPghYnB5uG5NEuElHv0gT/aOCeWxZIelxobzzdRnZWTFMzY5j1IJ1JEeYWDx3BI8u2cufvizmymGJTBtsYdawBCbnWvjkmwr+Z+0R6X0s2lhKY7uTJfeMJi3JzH+vOcIlGdEsXHUQm8NNeLAeRVG4YUSi8P9Uv21VFS1jDY3CiJRIzEE6VhceZ39NG6FGHYpG4VBJI/dNSePV9cWMHhhNrdXB3LfyeebabJY+MJYB8WHsq27h27JmZl82gB0LJjPv8hQWbyqR9vq6V7azt6qFR2Zksm3PMenWDU8Jl17HG5tLiQ01Mig+RPoAXjVvXG1Fe71eGUSEGLSImKR/dDDVTR3y38JHDo8ykWgOYtOheh6ensGTywv5pqSRK3MsxJmN7K1sZkxqFMP6hfPe1nISw4PkCheBTHSogfTYEG5d9A0jUyIxBOuluyeim6gQPROyYqlq7sASFkRwiF56PWpCXUW7vWQnhlFS387UQXFEhuh566ujpEQHs/NoE7lJYeyubCEhIkj62APjQvjm8UlSiZekRfGXu0bK4CQtLoTnbhxMdIiB2FADP78inTFpkQxKDONQWQvljR3Sfm8+WIclPIgXVh9h9IAIpmfHUdFkY3RqpPTfz1tF4/YwPiOao/XtuL1elu+qJiXKhCXUSGp0MBOzYlEULzNzLUQE61kwK5vubu/85YVMXvAls/64Ta5SpdsxYX5GpERgDjNQXGuVXkdcmFHKTjQbeXdbOcda7FQ2dTC0f4SPN1ER6ira6/MkxM//+S8OMWpAhHwvMljHL6YP5LoRiYxNi+aiJDNDkszotQobD9bJrx4+biUm1MicKzLIP9rM1iMNJ4luandi0muYP3OQ5EWuHZ7IzyanEWLUSpOVGhPMK+uLmXpRLFabS9XbRnVFa2DX0SbGpkVi1GkZmRJB0bE2Wu1u7v9LAQtXFLFufy2NbU6CDTrpsg20hPJpQQ2xYQYenprOvElp0vyIzbQ7kiJNhAXp+d0Xh9hwsI53tpTx8Ed75Eb4dUkjw/tHYOkkp3aUNEjmT02oGxnqNNS0OaRP+8i0DOqtTtodHho7nNKkuDwe7pkwgKQIk1zNQhVL8ioZkhzOt2UtfFV0nJgIE188NI7kSNMJse9tK5fmQjyU5mY7Q/uF8/amUgYnhFHTaifOHERdq4NHpg0k72gTVuFH9xy0BAzqns0DGXEhLMmvkqurqLqVqdmxfH2kkd/eOJj37hrJgOhgqWSBQfFhvLmhRHIYMWEGXvz7Qcrq24kM1lPTYqfd4fOHC8qbsdrcvPxlMVFmowyAxK9hTFoUxcesXD88UW627U43a/Yf55K0SMkOqgnVN8OIIJ30Jl5ZX4JRr2HKRbHsLGmgxeZkW3GD9Da6YAk3Mrh/BLPfyGPJjkrWPjGJB6els+5AHZ/tPYbd5ZEKn391FpkJoWzLr+ShKwfy1eF6GdILL2RncT0TMqPxeL0s2lTClEGxVDR0cNJOqgJUVbSi10gmbVyab4WKVTYgJph+McGsLKhh0YYS7no7n47OEFmE1G/dMUy6Y78W4XdJoww6Zg6J545x/eXKjgk1yJsQYfYvbsyRq//JT/bxs0lplNZZiQoPkoyf8HSmZ1twuNxsPlCHxnAemw6tViOzIYKJu/biBLLiQ2mxubhqsEX6tzeMSuav28p4fHmh/Hy91cHvPz9MZLCBNf95OdMGx31Hpk6jyNBbmJHf35zLk58WEaTXcPXQBA4dtzIuM0bSq7PH9JN++0N/2ydfa1Re0erTpDqF/TWtvLiumBuGJUjv47OCaqbnxku/evHdo7DanPxpXTFX5FposNp5flURcREmLu5nZt7ENJlBEUoLM/ouX9CseypbeHndEe68LAVzUAbvf13GtJw4CipaJKey7NtqSuvacYo0Vx8kAFQnlTQaDaXHrcSHGVm6q5qtxQ14NRpGDYiUYXjJcSvZieHc904+d7yex79NSmfPs9O4f0qa9BxKaq28v72cMmFnO5FX2sQDf97Fo3/by5jUSDYV1UqFigBG+OlPriyiuskmN+DDla2no0kDCtX5aMGgddhc0h2bPyNThtfFte1ys7rz0hT+tL6YY60OfvPjXFbvOcaTy/dL+yo8iJ9emsJlA6Mx6LSszKvEo0BRTSs3v7aDnMQwXp0znNfXFUuC6sFpGdIbEZ7GHZf0l3Z67tv5NNldaHv2oQPKR/dZKstldxMfZeLR6QOZkWvBi5e02FDa7C4e/LCAqvoOnrwum9KGDt7bcpSdpY001rez8Me52D3w9JI9DM+MYUxmNJOyYqVdfmZlEbNHJzMmM4a4UIOMQsXf3qpWbl+cR1mdFZ3htNby/EtlyRMbtRxrtvG3nZVsLa5HqyiSjUu3hPLM9YMlBz3lt5u4Zlgi149I5O4JqbR3OEmINBEVamBUeqQ0C+X17SxeX8z2Q/U8N3uo/OzGA3XyWHO7U7pxf9leJv1v7emVHHCobjq6Q3jM1nanTFOJoCLYqJNkU4TJwAOT00i1hLJxfy17yptl9kUUy1Q226hrc0j+Qmxuq/Kr6fDAszfncPvYfjIBm51glhyHCMlX7KqW/Dbd6kVOg/PTdHTB1VmBNG9CqiwZaLO7KamzStcuPSaUYSnhcmNb8W0NCeFB1LbYiQjRy42tttXB5ZnRNFqdfLSzkr3lzVjCjAyMDyMkSMtTK4ooKG5AY9SdKfvdhfPTdJy4AK0Gj8bL6+uOSBpz7uUDiA7Rk5tklorNP9rEit010pv4cHs5i9aXYNApPDw9U7J9izaVMi49ivsnplLbapfeiHhIL689QkFxI9ogvdpBYM/32feXgPxJa0x6Pt1Vxc6yJq7IjpVR4YHqVqwOF3+4eSgLlheyamclmmADTq+X335aSG2bnceuyeInb+TJjElOv3AarA62HG6guqEdnencqXjrc9NxKlyCkBeETyfnkWgJkZntvEP16LpRo6I2xO1wM3FwLEU1bdTUtvusvli+P6wM7Pw2HadCKkjbeVkKVDXbqWqwnaRkeUjxeS4bCmtlude5tHp7wrl9dV4fl3GmkFlnCKjj5DdcKERXCRcUrRIuKFolBFrRxnPmTs+OgF5roDfDvM6H6c9qla7dz59JP03ntQYMgVb0rwGRrvZXIYVwP5o7rzvUjw9QyGv3k6zTniCQeBGYADj8cA6lc+Xd3klUPe0nuQIGYD0wx0/yvoNAK7p/558/EQZEB0Cuv+WdhEArusdG9q4uLF/tbLcaOBk+ayTRdAZ4erLPIkPjsbl98gzaHmWIpCx2lyzkkYHOyeV3AW26Vz0yFEoWxP1PxvaT1UZxoUbJxgmOWRBKn+89TmWt9Tsh95ngdnuJDw9i4ewsTAYtz/z9IPsrWk6KGkWngShu/K8ZmawsqJZZGzUTAeor2uWRlaN/uCnnxHuiaKarNa2mxcYvPtrLB1vL0Bm/3+V5PV5ZizdnfIoM2UUx5IwXtsiH2sVDi85bkS2/cUQi9VY7724s9VlmldAnAYv4mQuIiv+B89eQMX81o57ewCvriok3B/HmnGGMyojC5fj+ToWQ2dZZJTp9cBx3Xj4AzylVo65ORtCucm00fR0ZVjfbOVzeTGl9B3nFDdz/1k7e3nJUNnbeOjJZ2IReyROr98CxNllM8/S12fSLD+2TxqCe0KeKlsyc4I7F5iTMhE7L3/cck8diw4N6XR8n6qNF3bToVxGprt9cny3r/bxqN6z0gHOH61B8RZDCvgrIYvEf0GciWi1eWn1YlomJMrCZI5Nw90Hh+anoU0U73T53yyX+Wh30t4Ry36RUeWxN4fFel26JxyI6ZIsrWmRHgcBzN2QTFW5UvZXiVPQp8S9qpSddnIDRqGVsSgR3T0yVtR1/3lrGp/lVMnvdW0gzYdTxwheHuW5Yomzf+OWMLH75zs6+vNW+VfSlGVGs+49LT7w+Wt/Brz7ZxwtrjuBWlB/c/aDRKtg6nDyyZA9rHhrP/ZNSeXNTCR298GL8jT5V9Nr9tbz65RH0ei1lTR3sr2qlqdmOYtSerj7ue0EsasWkY9Pe47y6sZSfT0njiR8N4pU1R+TXlT5ou+9TRVc22Vi6pUz+1OXy1fovySpVadCycMV+Zg6xcMuoZHaWNPkegl/O0Dv0vXtn0kvl6gz+nxSj1WloEI1JH++Vkadoy1C6BUxq4rxPZYlKpWU7KvnomwrZ4A8/yGv8p9EnitZ2BiImvf9KBbqm0gSfUn4gT6VR+M+lhdS12eV7opRXbahuo0WRuCjbEq0OGw/VofjBXAiZrXYnH35TweFaq3zdXapOr5WdAre/lS8L2TcfrJeNS2qiT0rC5NAqwUdrFamEXmI6kAW81P1rko+2u+XqPV1RjcvRWWqm6xzddrIJWe16bdZ0/2rgHwj0iu7xjiUl2gu++RQoPS0QWSh5FpknPYDv2umALvFAK9rWmdfz9/bj9rNcxY/5xx4RaEXf25nj81dIJhRSBuwANvhRrljNrX6S1SMCrejrAJFKsftBVlcW/KXOKeu3+XEVCsqwAPijn+R9B4FW9E3AeD/LXCn68YG7/Sx38/9nRXec9ErBl/EQheanyVQjW+Nc0vpqjNqeGnxcPWWsuwrTfdHIKaZbo/Fl189Mu3ac6eA/C1X9aJGYzUkyMyzJzJaSRtkU372LVQ4R8yLblcOCdKwpqqXV5jpro4/QbZCYbJMeRXy4kcgwo881UZB5RNGNWyAIqyabj7DqgxZldRVtd3PL6GQem5HJXe/u4s11rWhM/1C0yFqL/6fjxVuHyIb8QY9/SbO19eyKdnlIjAlm+f1jMZ+GlBIDs97cXMofvjgsZ5rqVI4OVY8MHZ0ZaOcZMh52l1v2C/aG/BGPwqDTyHZnMbBQTLURPxYx8u2q7Dh+dHGCTNiKUW23LdqB3e2VvLVaOCdbK4R+fwjBJhQrRrH9dXOpnKIgbYfby2trDjNtSALvzh3BtcMSmD8zi8fFQFitTjXK9Lxi77yd1KsSpJNpMJFZ1wXr0Rr1rN5ZyQMf7pYP8N+npDEgPlSaHLXwL1HxLxa2JtTAsvwqdol25yA9V1wUh1fFuUr/Mq0Vwk0UpJKY2yQgxk6oOaD0X6uHxeuVxZQCoSq3zamu6K7440ybXcAyTYpywv1rc5zP49gUsHfWwpkk8X6yRmXAotWg7/Jx/egSyDNpFDnJUUCMU1YzS6vyilY41urjl+LNxu/aSI+XkGDfiAgR0cnqUD9doQjPB8aHykkIYiyFmI2HikGL6sPfDtb42MhJg2LljXq6e1gOF8OSzXKWnagKrW22fZ85G2eEtyuz4vWycNZFcirvxzur5GwPrR9zlmeDygMGteSXNrG7ooWJWTHMuTQFT7sDV7sTV5tdzh0VyhAQg7hFfXRv5tMpXWmyDiceIbPDKQscxaTd9+8ZLcP/krp2HltaKD+sJuOhamQoyBwxIUyUfS27bwxv3zGcyYNi+bq4gdgQAz8d319ONV+1u4Z3vjoq2bvvC0XxVSCJer4HZw7C5fUSaTL4BnTnWOS8000H67jv/QJJMul6IdsfUD0EF70pn31bzTUvb+OJa7K4/ZJ+8k9ATI95amURz39+CJu7F8SP4qviF4MLU6KCef6mHF9uyu2R9Xwf5VXwSV4V/7vnGE6nW3Ul01dchzZIx9o9NawrqpWzScWwQTGGraS+g1bx/2QZdL1i18RnRXnZpc9tlsSSt7PuS7CBVrsbR4ePvlYEB95HYyf6RNGKHMemk+xc8XErxV2ulqy90/9guWLO6amejDAp4sH29VilQCvadKaDskRA12sV6DlNP9VZMihnQ/A/8+WzIdCKXg0IcsFfSVRhT6o6vbYVfmzCFA9OZNYDA+D/AOPXEpdYYzx+AAAAAElFTkSuQmCC</t>
   </si>
   <si>
-    <t>HCHR</t>
-  </si>
-  <si>
     <t>ONUDI</t>
   </si>
   <si>
@@ -69,46 +66,55 @@
     <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAFoAAABaCAYAAAA4qEECAAARQUlEQVR4nO2cC5RWVRXH/wwzwACDSEggEiaECpqGaUqAKSQJZqJBlqmpaJhlZIseVpbaC8tHWfnI0rS0Byb5SggVNB+kohI+IFCxUFAQlHFmGB7TOqzfZR0P+9zv3vt9U63W919r1szce8+59+yzz36foyqqqKKKKqqooooqqqgiNzrogOv+G1SrkdRP0gB++kjqJakj9ztIapb0qqTVklZIWinptf/At42S9GFJTca9Nkm/k/Rs3k5rK/NtmfA2SQdJGiHpvZKGQODuJRq7wa2X9E9JiyU9LOkBSYskbW6H73xR0hhJwyP3j+DnzTydtjdHN0j6kKRJkkZLenuF+nXEf0rSnyXNlPS3CvWbwK2u2TCEhd9K+nieDtuL0IMknSrpE5J2b48XeHBEv1/S1ZJultRSoX4dU9wtaVjk/rmSvpe1s0oT2hH1HEknS+pRyY4zwnH5xZJuqJBYcQxzj6R3GPdc/+O4XxI1FRpgZ0lflvSIpM/lJPJaSUtY/i9wzcm/JyU9n1MWOu77paT5kg7LOQYLyyUdi44I4fTbNZJ6Z+moEhz9fkmXSjoww7MtEPBBSQvQ3i9jTTgO+Zqkb0t6QtJ7JHVlIM4yebekQ/gZnOFdTqT8WNI3Jb1e5hjHS/pTxHj4jaRPluqgXEI7Lr5AUqcSzy1AgdwpaWnKc9+gPzcZ+0eeqWdSHad9JIMO+LukKRVQmGdL+lHk3nGS/pjWuKjo6Cnp95K+n0Lk13nmcEkHS7qsBJGF/Wz97cPZ1/dJmgbXnyZpYYpM3hc5ekquEe4ItzpiXHkJNImiCKEHSvoLJlsaHpL0MUn3ljnANKxHJr+P98XQjecuKPN9jqufNq47mnw9rWFeQg+VNDfFvnye2d2E/TxLUt+c78iLnSX9Ao9uq6TbeL+Fb6Qs/yzYgBiy+j8rxRTMRei9kLExReQch5GSvihpoqQ1yFDHaceVMbg0jEexniSpUdIJko5mkv8RaZcma7PgIUzIEF3SVkxWQu+G1h1o3HPa/auIkpe4dgee4P0oq5lw2sgyBujjQOT/HTDAo5IOReEKmTyKd1pwxL6ojPd/J6JvJiLGdkAWQndjUEOMe824ot837j0Dsaez1I6C8HNRTP2NNsmS3MoE+uiLp3knVswknrkAwi8Mnl/NwK+IjGs6Nn8RNGJxheiAx7gDsgSVrsB2DfGGpI+iGGPYl7b+e8bw4xyRx+BGFyz6l6R38kx3Ajf9kHtOJxxgOEIduH4gzlKILZI+A0OcY9y/BIaYW4DYsxj7B4PrR/G9j771Q9Pt6DMl/cy43oL8nZPS9mxiAc7p2IJbfBVLfTJipCHHwJqRjzOZoJMx7ZxX2irpWyViD46oXzCurySq+JJxrxRGYmqGpugN6I3tSCP0PoQkuxn3Pu7JwxD1TM6nuO6U1ZcIbfpwomA/HJPBiJJ98AIdt/8VIjyHp7iIUKmP4YithKtuxiqwXGaH6yWdaFy/DSVaBE6UHRm0c7HsvQm5bkOM0B2xf0cZ986TdGHkg3oRGB/L/xfyEzO3QoQueFZ8mXa1MMexuPYhuqAoLVF4GrZ2XjglPM9o85boXkwZTokQ+bYUIvfk/liUxWQmJSuR/e+JeYUxzCArshYv9C6SCiFa4Og1xr3vFoyXz2fVhnDxj7pwYD52kXS+cX2VpKmRlzk3/CayJy5ANEHSHwp8dBYXPIa7UKD/IgD1x0j2xkXkPm9cfzsBqCK4ymgzlEnfBovQ0yIzOz1FYVyGk/AGSvK+gh9cLhai9V8lqmgRwOHGSBDo1DTvLgW3SnrFuH1s8kdI6L5YGiGcpv915D0n0cYR+RiUWFEk2ZEthh2dFU8y6Wuwuy3uFeJxVXDNWTBfKfBOp3xvN65PoM8d7OipxA5CdCN6FS7nGtxeh3V0fKzRPiuSmLbLaFxeRj8bEWG9UUh7GdG9zeiSEJPx/PJmumeyInwMRow94lsdDaSCBpQxwP8XXBaxudPQwOTsGjzjLKKLfI6eYBB5K05JS8DNW8in7Qf3zOFaXgXWnmhjxY1hRT4LI/lj3kosJjQlj8cBypOZ2YBuOj64PioktGXIzzOM8QS3Q+grUaD/qzgPK2odIYMQA5kA3zHrS2TwppxjuscgtJvE7okydJz8AaPhLyIdjmQFOAX4w3YicMcMz2Rp92OU3iFYJCFWUMMR4mMF3v0IK9uHEyWDE0KPJSbhYzUFKhamcO1G7NZKYmdMrydSVpOFOoj6pPd9wiK4lr/PiLS1LKrR+BR5sNQwgZ043Tsh9Dijs7tZbiF64YU5/KrCRBZOz0TiHlbELYaBhD2H4Xj4nH09HuqYSHj2XmxvHztji+dBUyROvY3Q9ZFg9Z2RF4yE2E+HocAK4QGW4KqUZKiFZTgOr1Jv4S/hZ4n4dYXYIdYbQS8VrA2xzMJtouNdRiVOS0qyM5Hld7dDkeFuhCwvIabySkau6sGqvI52CyCSz9WJHLZ0kSIVR+8rYElZKbRdawnOhx7iMq9qKERSZZmWdS6COs+SCTE+RV+IiTnNuH463C2IL8KyNZh2PhYY7Yfg9IRiJQ1WmGKXGggdYrHxIULM7MHfuWuES2AcRPZXSeKGn53SdDfi435YdBMu+Gc9JlqKONk9UoOxLCKnB+UchxUZbEhER4jFkU56UefcZMQJysU5yPwnvX42UXI1DuVoYQoZlvO8e6/hke3nJYTX8tOTMYRYh6kXIkv5mQ8r6dClBo4IsTzSST3B8+a8hdglMAyZ+kNs8wSdMCFXwp0hupIT/DXZlWbur+TaMm81NNF3h4iN3haxGPKGJCxLbZs7atmKMfm8MfJ3ufgs3DYLuepjGQnir8P1k/DwPoe83YXUWSPcVI8YacVrnUHY9xVPFJ3LZPi6aQsx5BAfJY6RxYHaGkse1EaC4xd7s5+gDTe1Bi1/Z87siY8OEPAs5ODJKLSNhmJ2XP1zImonYGMfSTZnMmaZy2Tv6YmEQRDmelbJVNzwzty3wg0xDE/ZZpEVbbWIghAjSnRQR/FiOUiKcU6BC6/m/w1en5vhEqekbiHJ+1PMz8QmTsKyB3oFl4OQrUsw9xJOfrRgtlv00ZlV1Ibn2howo/vWnYzkQVOtYSduIQ31ekYbso0s9B7B9YWUyvoc2oZOmODJ+EPhvCRjvDX4nRDpIvJzM+B8l2R4nGolBQnXOmorlgRKstzStH7or82MYbXxzFFGhdTrVgFNK9E4q5MYfmSYYPMjLvQIPjKReacEXLwniuw6Clv6IhoeJnMyF859BBGScNVBxnt+k2MMeRFjwjAe7fCKlTOsybAlLURYbyHqGiwkHNqdpfiaJ+u78aF/w/PcGNixNd4K6e1ZKP3Jovg4qB3i4zt5VldsU5JlLq+sMRRaJyOSVwqWWTTYUz4+ViGe+hiOQ280fCJG1nllYvKzyoQNknrA/Q3m2CvCXeWgD5O3JjBDfVgMtqTG2CHaIWLQp2GJMWEDIjboahRSg7Etoj8cm4ReVwQccoD3d0fycQomIEH3iDtfDhIiLo94zl0iJuJTNRFPJi8nrDDER+fIPpQmr2o+3GA0kAEkXucLAUeHg0i8RYvQilQklYOkv7ByNcFgg7mc+Hu6JlI6FVoQpdASeXkszDif32El5h6IiyRe8A+4PFHa16I4F+GA3ATnvls2YhNQBF2wkET5sYWRRmWBqx1cUcN2iBAW+5eCtVdljF8W5WEOSvEDwdaLfRAtidf5PCZVIsoegNuv5vdizzu0MDxSPlEEIxB1L6Xs8LIyQq5cbHNNZPPL0AL7W+4x5PSQQK4meAIbuEeQMH0zqGNbjAeZTFYTinINLrTg5g0op/CnNlJAXwQn0+bWwBxN0CdSr7gtDu7qOsYaxeSNaO2VRsMYOjDT4UYil8ezqoWc+/0TJvo92MMJQf0J6xoo7G78X8/vHhHvNsEbFdgfvgfiKslGWZmlKYQKfKzHL9hmRz9jVOx0T9lQGUNbpLDRBYEsc/FK5NdQ76SATcaqCK2iN3lXcv0N5HXspxKb8KczwbempO+sfYxzk5q8WmTOEmOJj/Hc26z4A4Un9d7zTsbOwmTzxVGrZyLNQF7/LxXgiAnt5Im3PpRgdAye6R6xcLZn15OSMMuFXoQyCesUSuHmMuvv/l/wHMp9W4w8MUXmGoQeRprriZwD/0mE0M+jAH0rpA35egT/L8dMTJO5aajDpOyMIl1exjbsFlZ1L0SrZVUlqTFLzF7tJSK2E/pBAu++R9iRCFleQs/Hzgw1cCuyuNVocznB/1oCUUWLcurhpL6EU68s2I+w8cfz91lEGC3cYRB6TVjllcz22siMTYrYwWnYSpA+xJ7sM7HwJbLqA8l2F93W3NmT8+WcFzWCvZXdmKwYkU/0JsPH5WGS1l9WM40GQyO2YSnMjpQHTIskFZopDlyBXLs1UlFUCuVszUgwknhyTxyrWAGn+74fGNdfsmq7fULPidQvfLrgB39FO+YV66iz2Ml4/kW2ZbxMDGR2wW0O5eDDELkX4vR4YwwJrorkB8+zErQ+oddF9nUcHYmxlsKiyOb0vSObREWpwXiIPgxxlicr0ujFuy1dEEOytXgWnHwfRDcz2mzTm2Bcn+cVVL4FHbXrMf7/q/Fw/GVXi2KM1eKl4WFSO6HM3ReCzDfarqJi6f1EwyYTTXzUcKx64FWOo8z2U5iktaTMhuOp9oOp1hvm6v7I4NMZ92/h5FgR+mQYJRRNjRgPZlWTtaFznhelStAEcZ4rQVgLzhH6a8Rkm5qyc6qBLQ7JvpCXyZTfAvGOQ3/kUZzLydz8nrDuZyjlrfeKcGaktB+D/rA83TPTrByL0BMjIuQao+YiK6ZGThloY6DXpPRzHDUdiQm10cvctHFm0uOEEl4jiduTuMM8rJ29mXA//Ov3M5tSX6v+LsHhTLJ1AtoOe79DWISuJTgU7uvYRHw3FvQuhcsj1UbCdr40pf2FwVE6D7HE7yJmncjlWji1LxPoB3m6sCqPQszsyfUmRE7aBtSJ1IJbhwQ8TCF/auWW5TVtjpwSUBcxZ7JiGhxh4RLCAKHNPgw5nhD5z3DWCKKCS4P9iA2e7AxFVQuZ82/CRCfgjHVFlPwqEruexiRYRF6Or1GyPC7mnt4SiVIdbuyly4otGPixoyfOZgknFs5EPMzRuO+TsUgqcRhWMzV9IyiGbGLp3+elx3pD/Esj5WArsEwyebExQieH/VmYETlCMgveJA5yV+TZw8iiXAWX7YwjdXDBveWl0IxMH4VpuQ+McA7fEZO7LzDpz2R9UVrAZQ52ZYjeBEyKel4JsWNby3ZBvtYSR5gU2WddSSwkoL8AU/DilMzMIoJgVmYqilKRremRbbzjYmcHZUQz+7RLnVY7GgtobOaei+G9iIhSRee38y2xE8iiKEXoZSnnc5wfCajkwblE9GIc24Cs/gvc9vkSheF5Nur3RzTMpu8zUw503cp4P5Jzm8V2ZDmbtA7Nb2UQ1pAZearIyz0MhqOsDZchmthhdT9m3rN4k41YEMsx73xnqAvZkSGUih3K79RjLsFi9oUXOeBqO7IeAjsMe9GqyVuKEitaDuvjVMyvPMq2Fa/xVVzskRD2cSyCPnBqv5ylbo2YnDMiWe9cyHPa7hkp7vKD1DTE6tHy4G3Yrp8usHO1EmjFGZqRV+GlIQwqpeGxlLTNAK7PLJBjDNGMrXwjgZ0BhC3bG2soFZ5KzKKQLI4h7/nRXSmUMY+F5ISwE8vYchF754eIqB2W9QTyjNiASLyZI0ErvdNsO4oc1L07isjazSWckdhJXOWiD5M8GmWWbLjMmrZaSwTyMe90rxcztCsbRU9EPyLluPVOJEZjhYCVQhcmexDKsz/yvYfnTDUS0VuJYnwOwpat3KqooooqqqiiiiqqqKKKdoakfwNvYv72Ht4zuwAAAABJRU5ErkJggg==</t>
   </si>
   <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAFoAAABaCAYAAAA4qEECAAAdPUlEQVR4nO2dC7TN1fbH59nncByvo/I6XuVNhUhe1ZVUtyLJTUmiFJJCualLD0Vv1S0ukm7inxTKRXlcrzzKq0h5pCiS1+GgPI6Lc+5Y9/+Zjdlq7X324aTGuHeOscfe+7fX7/dba675+M451/rthMS+s+V3RqeJSF0RqS8itUWkqogUF5EiIpJEV7NF5LiI/Cgi6SLylYh8JiKfiMgqEdn7extUUhxtTgWVFZHWvM4TkXwisllEvhCR90XkOxjqGHuXiBQSkeEiUlJEyotIDRG5RUQeEpF/wezJvLb9Hgb4azHaMepoHO3+ICK9RKS5iOwXkRki8qKIfCoiO6Kc80cRKcgE+FRKRM4XkVYicr+IPCEi80TkJRH5MM5+VxeR9SJyLP7h5kyRPL7WtSLyZ9Q8Fl3KwGcwuJswEd1E5IMYTBba54vy207Ov1NEqolIO467SVkoIlfk0C9njiqKyBwRuVtE0nLPhjDlBaOdVnQSkeVIjhtoRpS2Z4nIBNo4c9AA6ZuOysdD2bxyIqdRM0WkjYhcICJfYkqmYWpClCUiUzFLQ7D7z+IjTopOltEXIimjReRsEblGRNZGaXs7HXdScrGIdMAGnwglcE6yiNTCZMSidSJyh4g0FJFEEVkhIn1jtB9P+xKYoCUicsnJMOpkUEdnERnGYB21FZGJgXaFReQVJOtBpD4eOgP0UY9JrCAixUTkTJj1PQjFTZwbxGBse3oc1+5AP1aijd9HaefG8yc+H+bzHO67MzfMyi2jm3IDp3rvmeNDReSeQPvyqKJzXjeABmJRcSbkeiTVSe4mJHIzTGzJJDj7flBEytD2bDR0jYhM4hWLGW7ixmDLrxORpYE2DtUsY3IF2Oh40IIxPR6v04yX0cnYrWNIzhJmVVD/Bsy4perMvvPgjnH7YlzfDbYP8O4HJucfmBr/vCcY5L3e8aLgbmfzrxKRFJzgcPoQokQk+3ak9YNAm4YglxS+uzFdifbsimNs/6F4bHQBpON6PHF/w2TnwDoGmFxFRBYgDZfF6EgJnI5rVwlzVFNE7gOVhM7Lz8snN0GLsL2tYE5P7LGDjKUD5xw3Y3qfifZpGWNUas6rHe8T4VFMiofRw1CVASKSChRTuhP7VtYcc45plohkImXRoJ6akgaYi8sZbE6qmMUrFl2AMxOCm94wrH2Uc4oAKd8Cp1tqDVrpao71x+kvgdkDc+hPjox26nQbM/8ODk8xrJOW10XkOQPN8qH2O4jwNiOZqeaaThpHishrnNtIRObm1FEoxbwKxmj3TgBVOH8xlvummOPOFN6M432c/tc2vx8FVb0qIl04dhFOeDLf3USeG6vjsWy0w8eLkbj1qLSzT01QJYeH38Z+q8oNY3LOEZHdHHuDTvwBm/gBJuMGbHA0SuTezbCTlUAdZ+AkMzAtm3Bk83m3EekrniRuQSh2cf+76e8lJlR/He06l+unIDCzQSgtGPv9mMdPOM/Z+kEisieE86OF4NUY1Hl8XwEiKAEG/grg34LvAobuDrbeba7lOjcKSUkhX9Ewht0uS4R4A/fbgNprkNORyR2BlNbEOd0L8yfym2POX4CX5Zjo8kx8cczWNwiO7W9XxjsaAXL+5ykReQG0dStjbg9q2cPkN0Nj3PWmxMPoyuQLDhunsxrGX80krCLKewsHVJSOuQ59FLjmvTA2AvNCTE7F9nWGSX9lMrd67S7C7s70jpcBbXTj5Qb9KGbBOe+vReR0GPU5k5UVyMkcRcq/pO1oJu4WzMsy+vkIQrMKO10RrbgX+/21vWjIRj/O4KyDW8aJXTAfjskbDcQaiNd/NHA9d4/J2OHhMC/Va3M1k3kFPuF8BuczWfADIQHZhv1tgMNuAvRsBf69DdMh4O69pGLfDeROvsbu/g3BOIwEb2WCBnOvJEyKGJ+xDen/BRMsNQIBrEYd9MRPUblHOLYbuLcTDXCOsUeUjN0z2OwbSXFugOmKRgYw2FEMfGrgGpaOxpEZnAnDR4HHB6HOc1F1IWBJJME1KHCNITD8Wb6vx0QpJm8D7F0KUoowYWswo3ViMboPjQ+Y31zCp5/BkluRQI3yHjM21KdLyOa1NommjkjaJCSmO9cbGAPaJaCaTYkAq3HtyjGQk3NIfxeRb4F6n8Pc87jfStO2L+rvUw/MR02OryEu0BRtC2z6evp4DFgr+KYgo9M4MRNmH6az+QxUWk6bdXwvj6T2D3QyGS14GrxpqRNBzV2odjR45/Dwy6CTeXxuhGl5ifNWM2GNA+dvob9bQBFbEJTpOEdNI0wDvvmQcRH3fdzrU3vGJYzf8emIiBwyZvFKa5IsoxuACpJxHnuAQs1o9xp2r7mx312x1XMCg+zNjZxp8KkP93kbe+fb7HNQ9fdwwgNwgvWYvPE4psZoWwrXmm6QktJt9P8yNEvN3wGSSx2x6ZEoGb2HybOfxffCxAF/wUEeQcMOIJzlaVfVnPMzRtfjPQkPvhlmlOeid4AdOwPvNA89PIAbHQp5ALPhOmKpIcy9gzD2W89m90SKtiC9HbHhWwmcErCtWfiPKfSpAd7+A5x0EhrQAlMxB7v6ENIsSOBYmHQfr9O9/i4GgSgen8aEuQn/PyT3KAjtuBHCJLD/LxhdwXwuRycEiXka6PYkCCIL6S4VJTXahdLU297xJLDn35A+QSrWwMwXKW21JZgIoY4Ek4+2tANNuZc+L8HENCVA0bFmEcj4+RJ3/+3YZZ+GIf35gKZjEYApwNlWCFSyARHKx18wOtVrkEYE9BSY9kGM/VjaXEdU5OdyI+RAXmKGLXWjIw94xzsiCb0ZUKz6XrZ33cLmc0tSm3thss1PZ6E9aqpCad0X0DQfPk4G5qkfGEIfriEiXcEkp4Hxf9E3y2j7uRJRWDcY3Yvj7wLPBJs3I9DZRtxwvHc8GbV9hDyypRuMmjmJH8dk/EF+SYm8BKY8xefGONgq+JdeqPsd5gqZSF8BNMZ3fhPwCf59t8NMTTWsxmwImj0X6d7hMfonFKXMTUDVlcqCD9siyQJzNCApBdyaF2BEW9TWL7C2QV3f8I4Xx+NrpaYKzulppKU+Kc6HkfTO/P4BfVvOeYUwbT1J1HfCuT3L8aIwrAP+p4ypnihlcI+2gXHNQLiUHsIkCX18FVtvzVo6fUmI4ISqMEtK6j1fNMf6G7BeEwewJtCh5iarZckl198MSPMgrvtJ4JwEqjfzsLUfgNvzE25Xxt6/DvM1K5eGc7+UY3+hTXGg6WU48S6Be04Go/t+YB5ap3ntrZ62XI/T/cEcWwNqKxmhElLdk849OBRVrVnYJaUaSIdf7S7NBC32jp/BwN/yjvfCPLUDm4byzA15f4yB7vNsaGGCis6Bc1uZpHwbgqJ5HDuA2pf0zlnCRJX3jq8B7p7N9xQ07knTpofxHzsxsy7lWjvCzaoTFKiXL8rsCOpxB1Kgs1wd9fOpOt73K+/4BTgxW/W+B7XeRBbtghhRXg1SklcTlQ0imMgtdcGWt2Rys8xEKm1kEmp6x/fDH2V0fq7X3whpHWOjZ6P1LiaoEwH412UmNFJKM4tHupOlamXwcrkoi1wqc/yAd7wKTkavfyE2PsPAw5BdVMqCwW2xe4OQ0F0xzglRImOohL9ZGogoj8DQqoHzvzVrQn4Eo1fEH+xFOzQeGMW7S2BViMDQJhwcy6CqgRnfBmn0QcqVTjdmowSME0yHX3l2Tu5qpLU5an4WwcEuOtY14OmPGru9CidmQ/l0zE3IT8SiY9jnd9CwKoG235vKt6VtBhtnIZxPgdD+DM9qEDh9yGfH34KacaqILVnO4KphC3tz4ftMfkNQj90wfCHBx3VImW9S3LGrzPfXTdknjYnUzKDNyk1HYpaRjfMLwEK0lxk4HovGI5lH6esZgbbpgbSA4JfsqqUV5Doak8BahP2fiuZofTUhydT7umA3J2AvX8QMTMQpfmlucJAcwnXYZWVgKnmSScaxaWhv6RZC5qIggvuYcBvKN0VaZqABl3kLG4uQ7Dknl4yuysQmcu6ZBhMLfqghY57knVvTWxL8Oe8vwzPnsP8JOkpECx1lJpnI6Saw6lTw6RBKNn+CAZvMDY6TZrTgXCWgEq8fafNTYsVQOhN4HoxM5x4j0aybmeQhfL6cQq6lBNBNYSY8JJkhaoK2ZCAUxQwWV6oMslnA9yz6l99b+LiW3+oTDY+gTyvwaRqE7UrCywod7Y4UDWPmNCG+G3VTOgxSSDM1M5+KRInsBPM0nLzENM8sTcCZXoFktces+Ov0fmCyJuLAbvUmPhplM7bJOK/swDK18+iDfzzFW26xAcdZAec6DoHINNH0f9pFvEClG+o8BNVWRq3x6nw7kdQNJt8bzwpPJcXnewjZfZpCWnQZzmpUzKv9f7uQDQ+RBkG1iQ5D6KmMV7BVKu5F0IeNwy4NDP4HAqK8c853VQSPrg7lTCRpF5Gckh+AbKTtdCDSXaHKbwzSYGA50ZtP67jeEyaL6FMaWvE0WDbepbVf0X4OKh9CLeX84ipUMrCIcr75rAt02pmYw/Hq6wied4NpfD2Nmplj/uKPtaZAm4CTujNKyjREGqZOAPIVDjTqR653mJeTUZhZlXv28KQsFu0kif8ktrlKQIiKk8v5MnCd8p4JLcD5mjyqigDanIhDTEcjJhhQ0kqGGv3N5CKqmTbrGXCaMRk7sFPxDFoLpIvQno7e76mU+ccw4UuAiMVNYl7X/xXG48dDFqY2Y8L9Fa614InP6AjOzWpAa4RNzW9+mFzJtPnPOpIIs/qqqYSkEWBoPmEB6tLBnPwtXvtC+TmtxbnlRFXoeDb5h0dMRJVKSLuOiKsxNvh1vPlr9GkEjNoQY4eBpR1ebbIzMMzfaXA5jvdH73gapkMZXRhEtM+ki4/h2zS/MpmceJsIs/KNydRFiNk1OTKDGW5ppNyB/Y9N5biB6ZC/sCVEjc36tkng0aGgl9l0TjNj+8gdn4svENCFMqhjFMdlaR+T0YJjVfANIwJtW0cRlvqMWyX9XOCv4u1sGK05kv0EfC7lfGWElGBdCqBagi/DRQ8z8DIwxgYH0+hsftRZNWBmHPv8Mrw27VH/T4k07wicsxsTl8nk34iHrxzYWmGjxX/htEuaIOpRSlCfeufVxff4gYoAEj4zkl4H7avKdb5BOLUk2AOz6+qsRSPMwtOYDlWFanRqDTa0DpHO2ebGM1D3i0ijqgbsisN8RLyU6CGizQoxdmRF6HQVnGIRmDzEBEs7cKAbzXn5wb5FSGq1wQz2CdyjBxPgpxEiXNeO6xzv/QvudSaR4pu0cddcHcH+6VKsdXSiGJ3X1Z71ebepw11ApK4mclIaijbYRSqWipn8cSo2dwn36QpDynnnZINAPkYD3iPKs1XrLAaWaRx8Ntr5d4ToRT77hYZS3noNS/UQAlvQqMi7msBtTOYcArGCOHOn6QsjJswcis15n9lONOigLu9+OD0MuFTCO74M2PMFJml7oPM3k92ayYTcw+AbMUlLiFI1XZnNBO3W8hDefoHJB5dGAFqTgRuLw7wV6DkGhmkRI8Vk7wagwaF1zLcTL1hsreaqFu8FMIkdmPDRTJA7tiAJT/4NMzQRFXkJ+6tBgMKVNAao0juLEPQeszBF6UEY7sJZXUZgV/xUhZmveWq8G8lqxvG59G8Fk5OKmXuDMLkdpmc0eZqDpHebEJwUYv3f6UjZVsOwmgjL3WhS0wCTi5IEs2WvfCbtcJY5djvm61WTX3eatyeCmr3OwZLYoVpAqx1m5ZJwcZtPyCIf0gdps/QJN3SD/gEY5+cOUgNFAqV5IJ1GoIPTsYHJvHfHZn/KpI402T7Nr1dFdcuZsP9dc8+LcMLTmahQ1eZO+v8u30+jLxpkFWEyXsG0/N04c+eInxcTcQ03Cfsy3LgUklDQlPcLwWxb/nmTCXk40Mk+dESXsfY2MHIMZuoRvLy/QkgpCWEoYvCpLZxeRjLnIy+oikbppk5YAh4ciuIci1DtfgotKo0zTfC2ZxwDLY3E1yn9VQMkZfRuoialspiFVByI5hsUv9Y3axyOoXr3Bbb+HiSF2QvPX5Bzh6IxLU0UuopBWGpCRyfxW2j3UyFv0DnRAJOX2YwZvDnK4vj+wLmRfH8eXiUaDcmAP30987KS/LSIVwwdh71SqgBOTTbFVsXMi2irAcx0Oj8m0Fm1rX812NWuElqJE34Fe/0hkWkCwUhumBgPJTK2TqQ074piMmqwiKcH0twOYVmAtquWL2ZV1BPm3HRw/k8JMb/qfA+1NKW62GDric8ETRRDMpW64VxCS3ingrPrmDV3lo7T0XqE8W9wj1CB9GRpI8wZjT0NRYcJmMT3Td76ZZzyXm8pwmokXgO2DJaK7bH89ZeE1WEmRpvjvVBZVa2KMOZT1FnD2h2ghUFe5s/Z9I+p1fVAS0KRnzCQ7oS3w01FOi9Js2uTyWtUD1x7EJOs/eyPPdc8R2Xe14POtFy3mX2Ka0EdP8UWdiFKFiqQikHfhI1JAt4sp2M1zE0uRBJnERRMxXFMhVm7ydcuMT4gg0T+BQD7UL55J9oylP5UY4JLsk4vH4txdpFTmJQLE5PJhI+jXjkfwdBVWH8yKdod+CsNrjTi1G0T+8yysllMzHf0bXw0RguQ6j2CkIHY16EwV/PAGoar3a6Dqij86UcQMJtAxdncu809xuPgxmCfe0cxJ0r7mWSt65XGEb1s2lzHBNwS46EpSn1hsiAU2Yy7IbZ3AnBRk2M3GyhnxyxAzwNowDMcG4LD/1nq17fRGxnQh2Dp6WbTTRnD6CTvuRzdvOvcjBm4yHMSSp9x3QnM/rQoWyNClGwWRCrNRDqjYXKlBThcS7r2ezavoYZpid625tVIuC6XmME4nkHzxiBU/fwNTaElWA8CmRbCwD3Alpaol2LJpaaycLG3kP0oVeD3aXd24D5HwKi6uXM6atwxh4p2tCfQlMnhsRFTqB6FnnSzFJv8NqtRlTe1TIh9gCDsbsxPN4oR67AAS9CoyQjQzyjE6HTC0VQ88nyzpqI2qzcfhDlanUjBppU3JuYwWFsTRtdEYcCX5Aca4mAfA3HMAl5dwiSGKtwFuWdTnJIWALabyViJWbk2ykNTOiJUz5ntE1plusrwaCGaVI60wkhw/jSYW4OCSPfQIGPtBX8CFVCayWr52dxgM9hysPn9Nmxnf68OqQvQX+A91vOTkhmoht8VOHaEUFijOV1Olsz1toCHp2Ca6sCUSYF9NIJwPIdk3mcSTZ3JWVyGCdUyWVsQ03Fgbz98g0apewELoeXHOT4YZUTA/s6huDnX2/qbycB0U1FrLxC4HNyagfotjHVjQ0VhdllMSicc3ijM2jaYHG+BVtCAYWhJJ7OVoy/2tg1Vny+Z1KVMei0YfKOXBtjDOQui3C/Hx0jcGdhu2xxmT0O6enO8AJPyHLZ7Ouqq9E+kbCnSPzbKAkOffsCUzAQtrEBix3Hs81wwuTLB0Eyi1LqGyU/A5PUgr57wZx8w9GH63s5j8lry+VGZLHE+GKUPztAvT7Vg0PlMdKU2bhCQaIJX1M2gzRUEDitBAXUlfor2BJpYVIsQ/zOc3hXemAYbM/m0KbweJnB6lBSvj9VfAwj4JbFfULyPYxuFXfa3TBQxcGkKzLsbiLSRSXAS5G9hWMRKnhsJRBYiEd0ClZUTpdIk/OfgjGsx6U086XvBZO420N+HMYu6N9F/Ks0igpx7va0UUSneh1flw0YtZQZ74bBOM222YEqOEdbW9daL9PS2Z1iqhyNthU3eQBCxCDu53WDkJ0Ebvc35hWBsVaLVS8m7HMaEjQpskxby4z3N92ZIub/W4xjO/2Ny93Ppc338To5PCsvN49jq4Z0fI0IqinQ0BsDXAMsWw25eTHRpM3UPmKcFhCg/MO9qGFYFph7B7GTAzAjqWoj7FUetM0kdfMyajcVRQvwIk36XOfYo0jybQOUL7O8KTJyG3wUYx6Ugkbh2HeT2uXfXUzWZTOJpsTebWoNrjCeeBNyzzH6DjsbzgL5ClIrOwqQUZzKSgHUHwcZbwbDfxOEYa1B8uJLvGcDREQjTUbPuWakCMO+P5DYyQS6h9XlBOpEnObaGgRFU+item0nC7OKVhbo7RlyJaaiDufkOOz7ePKzk16R8BFudeBUFXSwlAbYVc1eCySyLKTqDY6WMA16OJIc2S+UpowWGjfRWKIXoOMzeyCRkMQhFGdnAvneZPF1xVAwJLoFUH+X8TWYBS2EcaTmi2GNI504Ytx8Gd4C5tvCagWkoyjVC2yh8OkKFZeAJbOc4qWeTFiDc7BllVX8sykA954E49iLpTYwj042TRzELB2GI4uam2NIk7Liu3ctiUtbhtBajQeUJ5y8Ggfj7C6PRARDVc3E88jMq5cWj54uBFloi4aVNdi0bBu0ASaxi4B8RCCSTh+gMirFp268Z3Nvc437yyPuYmIpcpx/vtXHW/kMEDxE6v2SeP1qYfEV9HLnmugsxUXsxh3N5bZKTpLx6xn8B1PRHVLkU3zMxBzu9tGFlMHOHKA/Dfplw+AgBzkDs5WNm28ctpDdL0X4Akn4t9j+Exz8mohwfZWGkv1StLt9jPZ8vLsorRhcDW6cwiDUeYxOxzRdQ4LwqypMYv8MUTcYP/A2YtxSGr/bal8Ju6uaiB8gJl2ZCrovS33TC8BmYmAzzvI2SoKZrwfHPBPav55ry8l8rkpGqnjjBTURNjslnwOjQyn6lN5DiXUzaM1zzecxDrIzfnUxKhELCXZiYjmQOcyryHkJyC3KN/WzQzGnvTNz0a/w9iKYQr4+jbRao41lsYX4GdwsoootXKI5Fl8LkkubhgEtAFh35fn4O19jOhL8cZb3gCdOv+T8sNVFdl9dVCKWO5luc4lRvV9MEnOKPYNV4FrVbqoXZqQRa6GqeqKD73i8mMClnHt2zBvTz0a/1Hy6n6g9vCvLKQk19HFoHhtSEQdfm4gm8PlUhhavLCPqSncvN9rw8p7z8e5BYdAgvnxEF7F8Ck3V51okyWYCFLQwkqyXhh12dUvq9/LPQS3j9lFzuV4xGG/ERV5Jf/k2lWU6h6fivp1NlOv7r6X+MPkX0P0afIsorZ3gVwcDKwL+yuSRPJQKTpYThCexv8akG2DudWqR1YuVIup9Hv9dRrV7nXaOltx8ymyLE8kAIrxThvObko9NZwBN6VPMJUV4xuh3R17gAo12xtjFh+VKYPpysne+J61IT3EItThmti8b93V8P0d4+aLtzjBzHBPpjy09nUgds5rXtRcDUOS/+EzGvGK3PygjV57SoqquFDpJ7nsqKoHGmrSai7D7s1iYMn89C+SNg5TbmAd+6P1D7MBepTEAb2vIqR7R6yPSjFswfQeWlDrn2P3LPRnHuN49KvwWO1uChAKvq03TnkkfZRJO6uUh3O2Wb7/2R5gHkrb8xl5hnVoUKWH0+2tWenEpPmLydXImukX6Lqs8AJiynP9jJkX5LZ6hF3cHmeUk2Q5eN3T8LaXogEHg8SZ4i2TwQUcnfWPSVeZ6I7pHRzUmDA/+ntYx2g+P5L6yc6Ldk9FqqJtmkJEcE0qi6V+TrKIn6bFOxjqecpmH5aUyO2vwcVxqdLOUVo9UcxAp1/XxDItJyA3a7mzETeh1dZlsuxl826Z7seNZXaJ3wANqjq4wqxTgnTyivGK1PJPD3GSaZjTX+2mR9svlE4OG2QMH0E8xGGW8fpNJNZlntLO83v1BQyOyNnG9y4cK1T/Pal6ckdm0O/8sVF+UVo3VN3sU4nbqsOHoTadlv/nBBJTvJfF6IM1ptfovAZN0UOZCFipeYTUpjaTfS1PV0/19tsPE1aMt8dh58a1DM82jCOawqbU+/b+N7DxYM2ceFnhDlZVKpH5JRGMYm8tk5EreI0DHdkcuouc+uCuKS/NajO5vpfnPS5Qasvzmn55jlrufSrO64k1AH0Rw8c5UYTb86W6//Uqcbh1xfnPN1wY2DlHbZgFvi4IIjtxpJtyu7a7v2DsW4ykxwcXncJCL/Bo/W4YcmAX+kAAAAAElFTkSuQmCC</t>
+  </si>
+  <si>
+    <t>UNFPA</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAFoAAABaCAYAAAA4qEECAAAXtUlEQVR4nO17ebRkVXnv7/v2PqemO/btie6WTtPMDTIqoGAH0IcDz6VRRCVBIoJJHpqHL9HEleeUlUmeQ1BQCY9REIzSgTCE5wvwAtgKNDRDGAI0NA3NbXq8t+pW1Tln7+97a5+6Q93bdW/DioJ/1G+tve6tU2dP3/72Nxe66KKLLrrooosuuuiiiy666KKLLrrooosuuuiiiy666KKLLrrooosuuviNBO1aV8Cun5UXRhF/VhydCELRkD6sCf+g94j6L3vfOzZt3Y1flFH7PxVQQVsPFHBFwEEPQ2rOU5IjSCmjSO/SJl1UObz54uB7qtPG2PLDRag91gOOpfWAFXGlDoI/VcCfBLACil1ksUZJfjB/XjUp9qaAdCChBzAE4J3TH2+7vhfZLgsuANIEtAZE/YpmnaEZAyoFS3SYgt6uSkflcwLzAZQntgpgBxk8rx4PAlirKuuYtE7EKGqKuhbyBVB4mwBLggXNXWDX+twOKzVeRc6uEcZ+E196pSOV6IxszHym8UJ0CU3RFNkIgwORo6mH4uijAF8K0gqFQQhQR8eKpzPU8Yelbu6bmDP0Mj0e8aIUHLUopw6kKb6uxH8yubYwhsdvq/IHvefTstRs60xoAqUKm1P8VWEVKZ0G8EdE6aA9dVCHY0A4vbUmfhbQGxS4DsiJ/6pBmy5Y8BgUqzpOohD1dDiUHs0fCBANedihqU1pQoekw2YdFPHMU1QFONYN0RJ/GDFqE5TWTMMGJk9dU/qE226vmNm/Ddcz46OtY5qBlFDYN8XQaSPTnk/j6ASQMawi8FdE+P35Wv9zEFa5TcBfIfgHWoewB46GYNVsGySAKdYzKdI/nXymAt05tWGX8EdUEVOHMcIzSWifbBu/g2K9deK57IygTZ5ajJXfJdOBiJPQU2NxiwEM7/aNI1RWNGbdAAhGm/x59fTnqtQ7x2G+FrAQvw/Qdyr4W6TytXFRMyvsniYm1jdzoY2Dm4xsdKqbMu3XichT/QFt6KHa1FsnOokI1Eyeesys++1hFRVHvA9BphNaCDxPER+cdewlGS3XJv9vSejkcaL/ikFBSP+ZEq8m6KcAPD47oefcXy5/q27UtK0+cOrUikkxNhehA9hRldsYVo0DrE5IAuc1GtsDFRSeaqo8/WFK6DlpDFze/TYQ0eF+1NzABit+9QTebbbjBHynwp9Oirs6SbiwXU+A6dQ9l7ENdyvruBZSgMqhTY2k3tzt0+hsos5XX5XUw9zlJ68AUOxLYONJzSZJ1d+TNe3Bsx2YAs/7SJ7OCaYTipJQLKco15vAvW0vMzC6s3Jkczi+hRiLf/1EboGgC73am3ZGvf/VFYr/DzM2Q9t+2PtXYxtLX+RoBqHCtezx9w8cVl9NNC5/goXxCiCbp45GlYpjzeKtzvGJMwkVDiouuIsKxey8do51DQt1Jr8O+VRKKzOlnwNYuNsONEzV+LjA/WhqbQCXgKEDMsSRnzL7CEi22WVbnx28Vy3tTTyX3P/1QEDbfLG02sR4vJ0ctv/l+l8kPZHzTXM+EXon9+dxsynrp8vHN6YL+f8A0AQQjX82aMordFp1tHQxgNPaJGFdge+VSumf9S0Ym0aM0eF+JC4KhwRtvf4sSN6rqhcT8FZMvqqblfUv5jeaP4rEtTEBMNzPeDFlUDIl/UjJRrt6rlLzxhAZuUug821a+xFR8nbNrfcWOSw5KCryZUrM1UR6pCoH5fSUEO4PhJi4qpNwM0bWvG03BX+6Or5APB/AJI5YH1Slp/MxBFOENsCYFFF1Pei3NVS4jkxipLDr1GTHG9YTJDXLQBix6tZmTK/kknlcbNSliHpkMFItAo+1EZMJEejLQnzi3BbMrxkEeM9v1kbh2zH8pybktZ3YABGeAfL2n9HOwaZ8YJJPZ8IA63auwpc3/TGq9QoWRcPYv7QBH+j7GQ6MXkbT+Cwycod3resSyC+saBLhipEP4yE+CCNj8/GVvX+AhaVX4HWcm3MzEoeLyBcwi654XWkdfDblswuV5LKo5IJIhJ2Tpp1MIp7xfE+HMvGuAR7ZdSD+xxN/jlHfCxLF9mQFHvYr8BM7gI/hRSzmGoqaIRMDNhJEAXam/biL+7C2sRoLC4xKAuwo9uG3ljwJL1NWSHN75YvJSCGaTSm/3giraPjCl1xm3h0+2aydahNaPYeCnAI7ZhAzhC3SNlGQhw3Q0WnLhwxjpMD66kE4/6kvouoqKJkEGRkU4FDhDI/IIC5rrMJQUoJvGGRFDxt7MCzSsQjDAy9ggMdQpgiEAh585igcVFyPxBfzOcTRoWjYD7xRcrkTcmetyaekYyF+RHfalyRCSSzUKAwLXEIQDxj2iHY44HszRlFMD+4Q4GIDsQaRdUglmLwMFoWSINrZALYDd4wdhy1uPga4uttwhhwq1ECZUXDWFCMjBUM+MTBZxFm9yE2ASvn7lh02jB4An8SI4IPFAhb7B54n1fNvDgKxo/g8Ib7TzskDOs697aCZnD87N09+51taNxyetosdBYP1LYvT/get8rKUlLSUZQw62Hk4Z9KnmQ0GaoNbXKO8PwaTlyOWbS9V34SfbTgFJ+91O5pSDAzyD8S6nEDvGx/5cYKem9stwOVBsqjQX+eHCj1KGRPBqxEVOj98T6wXQuk2UdxKuwvEiFj/UpW+o4qXJlbPpEUK4xGfBWjP5NssFwf/QhXEJH/EpPvM7RliXCZ3wmtRmCFo4gmFJPjbra7CfqGQ+3xW7VvfHxWqUSEb8ZmNEGWRhKuQ2V0wtIyLfkWlUVm/fazUowPNv1Wi7/soe+BHL38MldIIjhlci0Sj9UZpc5vHOqqge5Uo91wB3QzS64JvIIZ+StBghi7P4xOEy8fl+l+BsJaUrhPBNH9jXCT9MUN+LMovTHxJEBjIFQJ3o8DePO6Se9Mr38qq/AylHETDEUbcu3mCEBA6VoTOA+FzAE4FUHgNpAwwIvReAp1PwGcUeHs7oQeSBH2jjL4qoacaxs7+QNUMem4+1UgMvLOrYH3wYhK2PjGR38EGCxT+G6aUHLOgP9mENHq5VsC5LyxtLntmaYaf6DEhDg5tybJ2puHJiVv/20BMQx6xpJnx/vvjlzCcTe843cJ7xXAyCg3RvX0nWyu6GWRXmYKStvomMnq0Ue0RH0NV/i9Ur9HWofyHjtJG8gw7XxENZncrcAyr5or+UvVYK46/A+AbAP7ZE98joFWqE6Zy8OBm5dh9VOhO78wtAH0TigsBuoeUrxPiPg+Dlf1PYNuCEbw0r4nhoeQ9zugxPuP1huWFYq/f7orZFoHspcKBdg7sE2LZAMEPvKfVdfUelK1l1kEi+mSRFJv9Moz6PnDHQPXucFkRUjDgeXQ1EZJOsZ5wINbKvmzkETbyGBt5lFjXAfgtIPQJglf/CKr3O+K7o9jNI44gRLe2FI7eGw+5LOpzlGURshr/QokHbMnGF/qUdo9VEB2dsL1xmy0cTdBd+bNAdCII85RcJurzZNcA+uYOJ3D6SGEAzjQ/uty/iCW1VzDs58Gw7qdKDVNMnvZJIUHKfVmzOBwXmsvJ07vEcwyWE0h4ULy5jzzfUSwlTslvhNqXWXi/AjycRqhqBX2o7j71NCjygBRrUYVSJPISqawR8AdmkYB2nIPb0ezAYIc71bcAdDuBduU3w/O6ZFcBXPAnl4pjT3NVNqaINjI4PmfWgBDxymah/8x6cQB5Kw2gHvegwUU0TKs1bekMT/zmTgvO5xU6nfrkqIHFNQyaOtJGpQRwCE1tJR9vjSrpfqZQX1RgOcoyLqXIXcyEXQw+gxhfMNafFQxqIlquWUVFoq0CbSZJtO+22gC2pvNykTA3KOdUjtwq8fJe7wRRRb5BhJHdtVDubr1A0E8Q9Kzxv3/T5kGg/SaQ0NZxD3owfDb9/udqs8DJZzS22EMaiCFk1gbRMRcjgElOjm2G0CKboWAEBSIUCHmzoGP2pBdrtfLxzZECBiWFakUItFhZtjgVR063sNL+HKUnqLMXKfRWZRRAGjJ9iXjeQHG6LWPX8KpNgm5TMeUCqNwTMg7wcxo9M/ZjKabP2iGFY35ASW9SoNKBRcINvgrAlflfwvUzCL0RwH2AfslQtr6cJbAq7xDSLckOepwbJoThT4r63MHFRSniQX//HuPRKhS7ZMpEzbm/jQcUc9uvuSVIiL1VUH8Ca+qZb0RVJn+IpvEajfy5AM4iwhiMf79LbWyMnkrhmgMPquIyNOMdtphAjBQ0iRah1OzJvBn2TMg6R3hnW8yYJnxiupWPE+vWGphvG9GGN9OZmvM90V5thD1gcggN/gF9V1W/GxRnkywQySJSPsOI3Ab2LiN7EAvt7ZvRu8XrBY24udHuFjRqg+YBa3+f9TJpO2vE8BFPdvGe/j04OLMG/0OQJdF1khGSrUU0R8tke0bGiLjKheZ+0rS3sPV7I5KP+9QcT8BDTPq5PNShSA3hxEa5fktGfrTHlZar9UuMYnOvOCLOMD+uITaMVGbO2hFBn1sT82eKJV2LYX68oqPYUeqftmuF7gvQLyfFiuan6XLbLPBqUL+ieZhAVZaBzBUA5hHzzZRn5rxXRF8V57cltRrV+pKMxfO9s3kcpGhYkas4yLfgXQRudg5aTyH1JG+cNK8j1ZFZNhZ2vL4U+XuDyIkHG7AL657L2RpYt0yVT3JphITclwCcK8DjURQSEfo99bSRCPPVuJLx0YA0KwuV5GS2bj9y0dp62rulBw0sLOyElAoAc71tG3k2xjgXbF3b7lIRQaXB70m2x/NDwKoelXIFPwOBsCFkXBlvxaljCE0+Tqz/COA2Aj9IQicHZWnmZb/kAYEiCsHkr4D0u2yNlrQEO3hK7WOjd5SuU8HbpvEBBVloP9VMi89OTpIw+o/diQVHjbYva8Pok+5D1ft7roTB0jbGCDblekrN6VIvJSEC19i+Fxa7UKkQPVUrpvcm1i83leYHjUTXe3U3MalV0liha4hprYD2I+HrI+XBHuH/wuxWkpFn6nW5I8kynDu4BiXZBV5qUTL008YT8e+romysXBcXMqjTOEmjRQCea1tv8NoHLNwn1fqvN9m2xMF0Qk8EGnZz18bfPIoIH27nJoU+2txhnjc+eGS6LI8WkKFioWdHQWjElvdvbBq5o3IykZypoHcBWiLBA1zSK10Tz7k2U1OUof0MWjp98mi7+1cb+2NcZs4G4y1EmnJB/9XCX+WaphaWUZMSdjhG5sZCAjBJBZeTsX9LrAchlBKouVFEnzfiUmU2BH2IlNY6z4uJ/QfJ6OFq/UDU1G8WnL545sof43eW3I5qrbcgW5AseF/tznRjdCTVpeIcP1jnEJjC0UgplNdMy94GfnJkzmUxF5JoU2fzfmdHMvNUWOXfjIgKaDlA6ybMQ1H9R4ieZTXL2bhJpJdA6RJRhdEpmUttZ53/38E30FZC8CUovhbeYpZWFdJ4ksAg+MFFbB4oYExbAo+UNha8fJWUzgHpcvL8eybyj6pEwZipKfQdEKSRdUsVdKCobvPOXJbK2O1kGzi++DBcvQLLfKwh0p039/6bNvGUEsOEbIzyQt+Ivk0tHTQRsam1LXulkP8QiK6h1lWWNlu5hs6YMNinETpnaLI3UFFgC3KE22WGJuP8jBNtr1TmLjeYGambzQHrNMaMoBONHyCHaFs4MgLijJ60o4ULxualZxiWA4VwkrLew6Q3CeQoMnRmcGzI+H9PNy/6aXXrwEP9Bz6CQ6IXsIK3wCVBX+JZl2ItEV8D0buVOCMyhyOjc4ho3/G1hXKGswm6dNpqyX4x3OBxE7cP0N9uhdFoaYddGSUKJQVb0ZZuG99/Bpa3+SYdhMR8oD1WT9BFZU6G7JxGKCsobuPoPC3eocMcYwRzkEzrkBKJpi0//9dTqNX4FiuFOP8SMLY1tdAgSm4uCp5QYAORxhBONIvglXFczxMokMeYhvg0XlTR+5TxBRB9AS1Ha+YyjgBwaYeFHwzgH9oefGS8dUIwY/+m4zeKWD1d0IkWovqLao1etOmPLXyoPmpdgDzK4ozANoC+lTVUTto+NV7ISD8hwHdz42sSTSnAWwJxEBeEzAOx5zzYM2/vXTDGo4wRnPLCL3Hdlnei37YVTrYIL6lGaEi0acCM4rDCU3jOLcAr2dJniTyKaORXVQjotQ28demTkCLDTJRBePy9r+J3Zj/uNw4CuihFLFZeptyAaTentVVgCC4I7OCMbKwf94vaYnvSw8jLG8dd+TwQNZ7htrEDW0EJHl9deSlGXQU3Dp+AiByozrD1IhopcGTP03hTeTPeVbwXR5gnsUWG8NPmKdiYLsb6ZH/UXDlPax1hd2KJ24JkLAQpJ+tN7gbwc4Df9htFZcXjIL4pBP3tnLVKs4mECNP9wTmcs8lMugaXPcM3V16Itxz6BOrlAooZIcoISxduxAHrnse8eBT1pkW9WcIisxOfXXINkizCo6MH4hEchq1D83HY4C9g0wyuLV8YBKHC/DWIbv5NyRnmjlqsX5Vcceo0Mgfb7+jcOFc8BuTtNQ2cF0wqDqFgTinuB2ETzUjwFjnF76++BRho61sHhtcNYsyXkHo6ToEViUQ7Eh+tVaWRQ6LncPibnsmtmTQtwA9E6O1vzHBH01uSLfH1yWh8+hueO8ztPbmzMJj9ZEKn2Za+os8T5E8plHTn+o4zUdwA5Gmel6cN0qlqVDBPU/pfyHAGKCRRCL6JnRrxRc7ha+RywrfggWimNCKGeDrMN/nv1dPqPA8ZqiCr2EBW/2ei0bWJK07uwVQt3EgD3Gy0BPfEOrz/72B7LArBln3joI52FMj/IW2BtHJ3IVb59d6/a0jx8zOvXJDRUZ9/aPDo6glkMTZBZHmG4Z8wk4FCBUpVW7rdgU/oGO+w2SXUP/bpie+C/upbRojKU4fmEz5g5/ree+Awf6Yvlq9jgX7CLJCrpj13imKWwASrqC2Jn6l9a/XZ0h2hLOj1qrubti6BGzi8/v7ivOy2dtFLm/5ufjZbVam29hAia1digptUMFn02OLG3/PEV3Xck7biLwMLx1bZyD85oXF3bSojqUWTtXdkcTEX8YezLp50A8e6CqDmxMCSMcoHJRh63+5B/5239v5u7aHS1e2m6esBEUK5kn52/qEj38GMue1cpbvUyoGdaoxc2U48AU0xi9DqWfVPyzvi0VfKJxL0ycnHFSDudS0ZqzB+jFZPXLGOwyitiAvZ/mz0kUkuKQHyPNB8MkLxwOn10fGQ+yGZkIPGJRCUXyfOFkDPt7F8B1sUM3/psed4tFJ/6qfuM82oxyOgZ/YBxkOrRe1HceI3LwQfgvXj1yUPDFLUs4foPbmdtpdnvBTCB7U7GYWVo6C2atgQEjCxXkOxvOQa5loo9vo1E3s7inI21elG1XErbMZ8ew6nRPIwFT3yVhIY6xDpVGPI03P2D8TM+FGMherGVuMywQwBZp6ChzTTGE/PmV8VjHEFG9DDaG80SHB1i/S5DrmHoNQjvYtKeAex3vDq0zCvGT/z5E+C1Rvn6miV+BFS6ZBYbdXZ9wwkl5viFBUao0XUXQk8YUIpriVxf0KkxY5DkD7TYHfn5AMGysMh8GMnT92oXJ6RObljfwl5uOyfTH/95U6GfeDqdLt0ro1ocdczBv5DsPRB5034rckhr5mUnfE0Ef5Sha9GyFnu4SBtX1Y/s2qLN44XlEwtkOBI6XPZC5XHswmaCiEaSjG0pNqKeyB/74nmqPl0oxp9n2i3zPGwyeiscmrrk0MTYZ4bQUGm5KoQXTtcGTzOK/+3afI+ly66dujdY5+LV7hZ9/JqfBSKdI16/AuBPgJo+C3jcdhDGm4adLxiBvpAKG5VpWtDcvfVXhTbk9UfrtnCMQI6h4DAVUWK8CBn/gqouT8LQY2JH/mAUY7G0FOuTStyRFK6qlGz64lwzviPIzNWvcOxv8yo3RRlUxJK84z09KKrULNie/x51MTNktCZSrRPiHwixj8Z0attQetz/tbn1cjfFkWCl3OlQq8k8MEKOY6A1QAOBbCkg84KKm1Ygce4JPdQQveC9JHcE/VvgO3YRRdddNFFF1100UUXXXTRRRdddNFFF1100UUXXXTRRRdddNFFF1100cWvFgD+P9uuQwyBEy3mAAAAAElFTkSuQmCC</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAFoAAABaCAYAAAA4qEECAAAZHElEQVR4nM2dCXRUVdLH/2kSiGyRRRBZVJYBERAUFVBQkU0UBEFA3IDBBbdRh28QNxS3T3EURVAYBZQZVBTFDTfWQSKyiDKsolGQVYIsCYQ933l+v8upeb7uvO50gnVOTne6X79+r27Vv/5Vt+7tlBIvrtQfUEpJOl7SSZKqSaokKUNSRFIVLvcXSUck7ZK0TdJWSRsl7ZR04I92S6l/gGvw5ERJjSWdK+kMSfUlnSKpXJzn2S3pR0lrJH0r6UtJKxiUYyrH0qIbSGovqZOksyRVDThmN5bqWeyvkvZ718x7+Vi+Z+0nYOnlA86xWdJiSR9J+lxSVhHfV6AUt6IrSOoqqY+ktpJKmvc2SVouaYEk76JWSfpO0r6Q5/aUXRNv8AaxlaSGwI+TvZJmS3pd0ofATrFIcSn6ZEkDJF3PcydLJX0m6VOUvM285+FxF2BlGTDglxKSejBIXwS871n76ZIux3Mamvc8iBkv6VVJPxfZnSNFrWhPSbdLugGLE1DwtqQ3sd6DAZ/zLHOapNqS9kiqLul/JD3tO667pHewzDqStvve92AmXVIejy3xpu6+6xkn6XlJ2UWgg98kUkTn9SDhTklLJN3LTXlB6S5JTSXdJmleFCV70lnSmWB4DUl3ByghwvmyCZrnBJynt6TvCbD7gI2buIa/Ak1ebHiAa72lqAhCUSj6PElzJD0LPno36t3c2ZJGStoS4hwuYE3EYqvDHFLMMR0ktZY0CNdvG3CevpJKAxNWPKh5RlIzBmu9pFqSRkuaFWXQCiXJVLTnmg9LmomL5kp6CFwch/uGlc+x6oUE0J6whq583lP4fZIOSSrDY2vfub1B7kjg2x3lew8x+J4RPEmwbI2y702mdSdL0X+S9LGkB6Fcn2DZnuJvljQX5fUOeb6SYO4rki6SdDGvN+XRs97zJa2VNFxSZUn1iAlOOnGeyVG+ozK07y94yz2S2mAo3uA9JukD+HyhJRmKvgTsuxCL8ILWpTCFdwhgG7DMNwiMBUk+bMJjEl8xUOskvcXnPEj4AWWfAnxU5H8nVwFbQWzEkxEkST+Z15YwQPcTPzoBgxcVVkmFZR0e9o6SlCZptaSBkubzXgdo2xWS3sW6PKtvLuk0cDKWeMlHPyx7DZa5k+M9mDpsgmkZPMejgJmwlp+AjCfxsFUkPILuTePa7+C1CZzvRv5vJ+klvn8vg/laoooqjKL/xk0IhfYnC3NyjaRJJBDf8VpLFNEX7AwrJxAQy2Hth/jcYTLGLdBAJxEUdSUe5+H1I5KGca4lsJDmDEYPKOdzsCUnNVDuRdRVvHv+eyLKShTsnwDTBOHvF3DMMh69ARjKc8c40qOctxzB08P3RvydREGpbMDx+QTd3QzyUrLKTBKhzziuvfGGjlh8Jz7npe5jJP3HXGdzlDuCgZoI/36aQRwRr8ISUfQQo+SR0KML4LpLuIg8FP0qx3pc92si+U4w3UlpPt+Nm6sXx7WkMDjlsPjm5r01YPtbBGInLqmpCeSMQtldDTM6kUDenJhyFfDhZbdPcUxcyo4XOm6V9ALPnZI96jUFrlqbZGQ0x3gp8MvcxCFw8s8MyCnAy1W+1FjAgQc33xD01sEMdhmIKEOArUJaXwdWUpfAaMWz1n/ytwnI+ysWXYGE5VHfZzysHst19KBEMNZgeD8MKemK9pQ1FS8Yj8IuQcl/hzPPxiIf5Bgn9XG5VShhCNZR2RzzHZb3Kda/MeyF2fsBas4GGtoxAE42Qxk9IzkVdrTSsBkntYCdNOCuKfFlFTDSF+vvAh0s+MJCKtqzuH9joR/zBel88QkUbhpA37ZiVa+BeZZd3AGUVOP/gyQinmXMAG+dXARfnoayesAC8rFQf10jSDLA534ovgTHrMeKg1hEWZTXFLq4BEbzNl6VzjW35d5ahym9hlF0GbDuLEb/QqpsKZQi3+TLI7jfi0T3yxkQj8ueRcrbhnMehpGMwnqtNCFgXU5QPAjGZ4DnwvqncIMTQihcTCp4UNfLpPIzeG25UfJrFJ2uRLlBciL8vA6P7Qx1TFjRI8medqOob33vewWb96FC51GRExnifqxhhGENc4CZuQHflQEfP9H3+maC6GkBn/Ew8x8F3YSRdgS6Vrz0K0nWeODxPaDtqYDPDsKC+1IPmc3g/69hLIFSInLZrbHeb4/VpVDunI5CD5lkYSuK7gQHzSRZyCdwejflJSs53NAtBLcg2U817Vxf1loOPN9hLMlJU6AnbC0lC2/KQdkZeE9Z8Hs6EGilPGXUB8km0zjHHu67hcleAyVWCl4WJUcIgv8AI7Pgq23MsVkMynQSgfJkg7fw/jdYwihw8hxccxB/F0PPqvmSHispWM90Sq5OauJJ8chBvKw9cOjJYKx6ge88Z5Lt3ojl9qOg1Y0E51MIwnMG2n5/8TGgYzgBI5ui0ZXQm4ch7yVIKPzYVAr368j/Xr3jOkb/RhTb2AQmJ7l4QUETst8BL66SN44Auy/OCqGTqljypfz/Kfeag6E8TtDbgye3xGAGwVzSiDMZMSAnqkXXNano/VzMGJ4/hLVWDVDWcT4lvwxbqErgGYur+z8nPCiWkr8k8K4BWpxcgkVPRkHxylbqMS6odiQgRrjWDLLbS2BWU1HoXSQxWSZ5GYKHhVb0fdz0N1jMeRzbl5EciML3ms+kcKxV8o1w6Hmm1JmojMWTuvraB2oy8N1QdrcEzn+Ae3qZ/7sRX26kJj4aOtkb2MnHqh3FfB5Pq0g95HcSBB0eHCyCsnXDQgWejcHaf8H97Q3fZ7KrfzIRe4Q09sskFNE3kHVuJ8HwMxMn2QS5tQl8R4RzX8H/N2PBPzJrflWMz15jgmxTP7cOsujbUHImJ3fyORnXM4zcAmOl7bBwkdjchJIFhiVjpqIGycvcGEoW7GRkFHgqSI4AE4s4biSZ5pXEnqjBDl7/DUhwm/9Nv6JrmlF7jsTCyk5qBJ0JDsdz4jEocwtR2UKKh6lLErjpaBJmsqKjbxIgHvHyhWvxnHS8cyZWvjfgPBV4PIDOxOdPsAf5L7oP1GwN3DiafA7tmUqd11Xc7jAToSn8eVlhLV5byEB1hJMmwhJiyQ8E7HMDMs54ZA3VSAGRw6J89iQ83MlUuHRl/7SdVXQaIyEKJ7ZD6ALTXOjkIEocxP+v+4ozlZl38wLFAvD+PC7sMwbobiVPXoKfP4YH5RTyzK9BTQXDOJ3nKUBnOQLz9cymV4DqTuK4ayxk2mDYiqxrH/WG782XzqOWPM93Me/xZb+idDv/5i7Iw70dUW6mFCl9/UIoJJ/BvDPEsfFKfbywPIzmaoyzP+yiJpR2BxO9A6gNfUuMOOpZ1qK7o5w5KLkRFn4XePcXLNAR+5bm+bM+JTsFbI+hZGEBc5KgkIlJOEeQrCH+iLp7UwznFfRyHO8dhh5ugO0sxppdUnVU0WlMpspg8xbwybVh9SD6unz+dkZts7mYRGRrIZWR4muWTLY4vlySiQ8nlUjNuxAbyvD6EUOJOzgdO0U3wIIPmGmmbNzjG0YpH568nNTTjdYkoCNRqVZIxbzNNRaVbDITyVeY680GBT5kuut48/0z0VczdHVU0S14vsxH9M+g6NKSGZWWvN6dEdyXBLctE+KYaPI6eFnUHf7jqXNUNJnnx6b79T++btcVwE66Kxc4RTsFLjSJhuhpG4jrTCAtjZgvm8csS2FkEqMfr3xNxM8t5PeHkW/RjbDqlAI+s98c/5tuI0T+M3hxke8Dv/qqc1twBTfb/G4SbmKpaQWIJhuZflqPx83HdaN1oyZbjpCVCgpp4a4Symzs+87FPDb7re7PbLTrL1uugqUl0XZ/AN1LRH6JVTAnGDegVPsn+GwHKoJnR/lMQRaXiMyGXZT3VQ/vZxA+8JVIl/LoGWb1CFlbRfDG3/meGlCncDf3A3Xhwko+GVU0eRd42M/fQVJhV08YRtVwOkxoEUqpRQ2mchKuUcSq9TxvYV4vCyYvN5VLQfX2YBA1I6Z+usXX7H0VF72Q1NxJEx6XmtaswsozWEPfAKXbdtyBBMC2JFcZBkrGQzW/ZsLC1W2SlebvJegJhubEtZaVNY1FwlM3QYFrpBpFbzVFpFNJQR/gZiZQ38ihSUZJsmZ7E0PMBfYw7w3hu+tSk45gsbOYTOjCDbnClZu5voVKXw08NaggFK8sh9bWxdMPkYpnMnfov6dt1IFqppoahu2/qG4aZSoyUpWgK64LqKiWkWXyvb2wkgp4lSt7ZpuEQGBjkKzG1dtSa1kW5bh4xN2zW3K3meahaGVgl4ydmGowzEb+1YzGaHjuWqpyjU3amUgnURjJg7M/Tcn1Yhp4bLrbAMoZC7pm8bgpQfoYJG7iuCwGt9nASX1iiC1FOCguFzHF7O2+AzqTCGzFXQ4ScZ1lxaphJENWARstUHQvrLIqZYKg4n+VgHnHvUnEaWeMpXyZ4MlA1xzf9zsozkg1o+0f9cVUq6zYY4sjURBW+xN/86BSTbjRPCJ7adoFrocNedf3L9hIahKDtqWNaeZ5BwwvnVLwJ7zujLdsNGxJAYfSYvRZJMsd45EtWPbrWE86HDzFdDG5lbJtqC5WhjUV5aLN9gx2WSilU7RLqPIjUch9Y9aOzGYuzK2xtsfGmj8rSlmP1XTBgvdGaRUTkNeKzqPANoA4xZYnnJdUwqLHwXh6AS0y69vzIkbrtqc4A+W+TmnUFeb3Y8kpSUwEEpUv4dxhVru2IqE5OcSxsSSD9w6YJXWHCN4PkDANNnHMGebOiGkZyDBfcBBQH4BFO8683fBR/9TWsZBKcSy+bMQERWHEBeC9hgzsY8APEbemGB1V4jE31ViEjeIlGY0+vvLfZrruyyTBOgor6cwP+rv7Y0kXvHQ5DS+ZcdJUd887DEeehnK/AJubmvlKp9OtqeTkoiIVAYd+YKrG36KbA0aeFAMXi0pOwz1fonekIf0j8Uiqr5zwC27/YchzuHvOMjXwigTduijWwUUp03KwIWIIdlVj6huZntoL86hkcMcR9KZFVCWLJjl02rtiezK+uwrzf9VDHJtqSqG2yrmH4NzTl+ZXQqdeTNsYQak5vOjfBeYcrGeWKfa7mkJ9N01TTLIBbuwmGvKSNLNSJeQsfAPTl23r9tWYV7wOguAMoCblg2xn0T8CBxHTu+CkJ5nZy+CZzPYPZRLoS06mbA8xYRBG1oacc2wNHOT5eqifoE9lPXOsrh/GrTTzXl8XIVK6gos/gr9A5W4Y/FBcmHOdRDo3kyW/MC9XGNmGJYaZXHb3+rVvW4rXyKI3077rZqRczdobxINuztDNb/mXNJwByyjFlIywZhc8Lk5SIpCI5MdYzBNGsllS4e/wD5K6pi7+gUlc7iMwLvOVSUuY6b7fzu+U6ihcM+q3TnKJpM+y/sTJFPAxwxfFi1te9S2zCCv5NAMF7dMUJNdQPcwzbWLn034xlEmQsabCWI/AeYQM+6iil0Hp3HJhJ7OZpXjQt7HUctP/cVMC+9MlS3aRufq7pAqSrIBFnNEkAwooeLJrx3CNnW9STaxsWicuhK0td8meU3QesxWKA3fdUuU61ByOlaxKYLYnJY7+6YHGy0eb1+dD7SbTG55pssUuPM50JQ6Lx651oG2M7qFypg77iXG9wb76bHFKWWbH45EFIWvUVQ1kzjCTCSKzvJTU+0PmOw9DeR0qHJ0Jsoqej0sdb5vzfNLbsI9Dpm/4ZLpNj4U0imM7noNg7B2+Slw0ecgkHcNNabgLxjgX1jLUQGsPIGSlDbRW0bkmivc376Vz0gr0mF3G/6cyylM47nbT8VSc0i3EKoDVTIudiSLCrCPvaLYletXXw/JIlBJESQOjk23zkX+xUEMiaEkK2DNR8L0kL66ospskZih1j8UEgxXQoKKe5nJSlkAeK0M9wr3MjnGMX6pQJKoHP25mdkMoBZzMYADnGgPtZvpQmli+7beElWZW+S4ed6Doz8xyiffB5YPMcLjO/dOpkRRXDaRXAUrOhjXFo+QSFPEdq7iNSt0KEhu3wqEdOYTl4bfz+LZ/r70glxsFFnU0JP0wozwc7ni8b4p9klmj1wfXKmopGbT6CVlJObSNgbawMoJERiz+cbw5h3zie0jAPiDFVT87QusO+9jJ/49ewKL7dWSI9YGKSbCNnZDy2WDcdl/knmm2R2uD+4RNCBKRzgFrYHZhVbei4Hj3Gh1KL51gVQN9K9OaUxbtQ2rdhKJbCVLxmkwCPOc/cbS14OcA/iVhGmGtojzKdQWVvyWy0VNI+cTX6zaL70t0qd0DeKyIOe0Ctj0+zmdcZeDS/Wn6yUN3v2sWjRatF5oG88fj4Mgnw0pcAvEUf8neA7UhbupkGxliIkpOZbGRU/JS7qE2m7zYe/dz7z1AqoPKsdE6cmMp4GGm9+uYi4gl91KnbUKBxbWtehF6im/D7MJKJzPTLBptElne4bZPdkFsIefeymDezG4HtWKc42kmDn7GKAMllqI3UZ0SQadzjGNvYv6uFDRvHXg9nfd70IdxaYxzxCN2Z90RcWz3Y6U7FM5d07sE/21Awr9I3BwONw84x5VmbebdvnrQf0lBLj0BcE/BjWoEHNObebz5WNUMsPrPYJfD6HqkquMKsJAw4qaeFhC8UtliLcxawzpmu+RaMKxHWDJxNYX6jbQSf0A6nYqh2OSoNgxNBMKYJduCFJ3P+sJ1XNQEs9QshRF/g9fHcYFbsIaRWLcXoLqbCtsNQMz9BSyejyXOUzLh8qcQH2KVTKuj0AUme1vLPYxgh53RVPXeIo+YDJy04VgHgelQu6q+5cxRpaA9lQR//BbiXw/lfQRMTOHmemLBB3DrPtQDMk32Np7nZ0EX23LOKsyWxLPecC50021d/DnKCWolbsJgvwD8lSY1Ho3rr2ALn1tR7qNYcho91q4Z/z28dpHZNHEPsPhdwPf+l8SzwaDdxXEYAbIemWM2tK4BUbq32dLYe74fd32IKZ7BWLnzKLce5j14+uqAnRWiSbpv3XoaGWobs6WbC5xHuK4noXAX8F3p0MNc9tv71ezWMNXX1vCYKaD1D7v8L559NEbjooNhJNvAbeG2Z2Jdt2Dp76BMt3vLPXy+Hx5wNhZ0GRbejr99WMgS8zMh6+C0h3jfrZZNZWBrUyptyEDW9XV77sJKnzcz2BXwzKlAydV44CQCZAWs33Lpe42Sh8ezxjLevUkjYNkA8Ps2ahvluOAFzMa4bYIHm22AB9BDcToWU5LAUxc37ArZPy7Kd+dg+blcR2ksMWgXXuHWSxjwqaTKNVHodOBsCLBxDgNwA7FmPJXII+yl9LNvhx2773QoSWT/6AgY1Z//gzZQnYzr1jJ1315M+zSi+WYcUGPbaevSkHguHnKKaR+OJQfwmvVAwr+Zq3PL6jIYoOFYZC4wOAKo2mESoFEY0FsofpcPLibwelho+00S3ag7lSxoAP+PhfS7ztQxKLYW3TtuQU05cP12cNL9GsUTQMAg3/dUglK6n2c6AU86wGMOQTELpbpBdVaeC/+dTrCeb/B/m9nJvRtwNpXPtje7uI81+2OPgYXF3dgehnUEyREwrzTBpjmuNo8bX8sgXE4RZiSzwtdyY+3B0+G48jMwh7kE1doUqfJgI1lg9WLgYD2KXUg5sjUs5kcC33K+182DDmVQ3maQunEtm3k8juufSK19NXz7HVPJexQoDDMz8zspTA0iH9p0KwGqHYq6nGDmJgC8FDwF3Hb9IFXAzGbw0Qm4Zn3wMtYMSFcUtBDrq0F9fAyDt5M/l/FtIna05X5fhNM/CitqzvfPMR7Zk6yxNV4xEIhMWJJR7BnDTWUBFdMoE26A53rWeYap68oEszewYLe1ZnsePwn4Hie7cenqYHk14OmIWZkwHfx3M0IzzBLnA2SQLaBtWXjfdVj2S2a7t1VUCF8prJKSVVWbxei7cuodtE71xWX9610qwj5SsB7Hgzvj/rH2rMtFsd/DCE4nO8sxzfGzqBG77io3cG7V70fECLfkOALF+8pwZvcjCplKgiSzfLmJ5KQ/1lyPVNyrfrX3HbuQbLOnyQgrwjhmFdAlmkswmgOutuN8eWZrtCXQu7tQrtuxy26IeA97bnSAeUxkWuxH4sb1Sdgd56gUxW9lTSRAjgPzvBv5DKu6BEt7BopnV7O2oGo2Pca5hQJLkMykEdi+wiucRW+nltKCmZBr4cFu/6Y0Ysmn/LVhoJ5jsKP9GlHCUlS//rYeFzzfYHNHlJgJT/U3f68muM4POJ8Vt64whSBXBizN9u1mM5KWgCZg9ePw8jv53DSMIB9MPp/3wvxoWtxSXD8ceR7spLv5DZadwMT7RPgfQp4rFb69iGphU6hgVc7pb3WoDuPoQfer49h74MqjQ3aUFkqK+6dQTyNA9oQVONkD9/0CfF0NT94dZ3JQztQ8zgQGGvvS+hUE7TfCVN2SJcfqx31d12oXrC1oacN2lL2JILYHeLA/7lsZC60Cn65h1uFYWQ0Wf0hSFfOHD4pC/gi/C54ORWtF8GpEVpbo7mF7oHurzI+UrTwWyrXyR/wBdi8Z8azSo1peEPOw17Nct1+I4+SeZXtMw6tZeNbvZYueB3iBuDg3tipYJP0fhbCpNiDQQ0AAAAAASUVORK5CYII=</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAFsAAABaCAYAAADXaio8AAAR8UlEQVR4nO1da7AcxXX+TvfM7O59SOiNhMRDoWwUbIMLPzAkMqZszCOxY1KQYJMixo5d2BUHlwuIIRQJ5djB+RPywAbbcUwVwcQBbAKOnMQJgeBH8IPwMmAhCSReAklX97m7M90ndXp69s7u3fvYuau9EtyvarS7d2Z6ur85ffr0OadbdMq3nvnDoyvBp0saKyzDYGZEAL4E4DJNwN66xf/ujyHfDUO/ZWn476si9baEUZ+lnFaQ//0eAD+RLyERHhiqY/tEgohILijXgJtrzGcTOi4/9PW+vM05DeA+AG8EkMyhrAoBPzUXH/trHdYBgSb0VTQdHilUDE+2ejpYoN/VkIBQpVdn90RES8uK+hNOr+kUNm24Q0kRFABmgNMHMDOWMKOfUaj86e6R0pcCGJxrQQpYU6R9wf6E73ihZgY2lPQVihAK4TOBHSfu0xGRBwOJlQtmKWM6cFqswzRl2GIlO8zUa2fr0Q0EwE8Coi9VC1RA1S3/8pW6vXp3bH9vLOFtIrGzSfdrFBwS3RQR/SYBf1+EAqcIhOA6822PjSanDcX26wCqapHxBgLg4YDoA4rwcQAvFuy4Ti02vlhgZ51x8Yt1+1ujhv+D8he8BqGIdoVEV0aKTifgO0VJbry0siZUFDkdKTpYyK1Z/l69zveNKTp7IKBPVRSdrAgRc7NefRWhqU0E7NSEr2vgayA8y83nEBTs9YHyT5KBcXlE8jahwPK3iYRx+ws1c8fSgM6JlLqgougDJYWBTPXoQ1TVqEx/eiTsrBExhe5TRHco4DYLfrH1Hva2YVTwuQF8IWLXLokIY4ZRtQyReK9GuM64eyy2d9uA3v7shI0mDJMmcNU2V/pQgTNbiTJxlp9fI+BnCvgfAwy3NsM6ic66dfEGB5zrQ6JK6pZR0YS8xNOkJPx4JGHIITWUl5LX6UTod9cdnIqmnH0xyBn0QI2AzzW1wx/SDOL0R6sqKQJVIvrdJZquArCWcwWleonRp1N9nv2d/Be5VsiWl2FS29qOGb59zPBDFhgnf23WZRVNNqLHncEQYaciPJLVAzMY7A2SRZZbJxLpfefXmNvNRGdFoBV+ZWWk/wTgi8cTXGeZ/4mBoezGSAZPL/X7YuvI157IfbnJrfSwxOKakYQ/P5LY9QMBnRAQbSLiN2jQUQFhdUBYTkSDgbxLyjWOUxIY1BgGpJtT81uRX6XpGkTAGIBhAl4iwm4wHlNET4aEn8bMT1lgpLWw/Hfy+lgIVql7oAkMnMTApQnzhQbYBuCLHZNNjIQZ1YqmjWGIGxWpi6rMXzHWkT7OucqMGsa6SGOwMtmvto6bxkDpP2oMPI30wO6ak6GoRLRuMKQ1GjhsX2w3RBqrZXpvgRUDmlaPG+5n0LDhVCuGyqupScaZiH8egJRl3qPJ2bv7CCSCsZOFZPBeBezSRPuSdJCfFnmzln0PpPam1kmG+aOGcb7YEL6do0U0ZVBnDDEQZ7p7SUinDDKdUmP+9HDMMlP6jmXsyMi0Xo+LNL6uL0TdAs9WE9ftKKfbMop8t60rwg4FcuXsjS1KFqgohZgZAelgX8zaguuxJ1vUmLynnITVAFypU17qAWCt72FSlyT3zFYiWqU08AdPcz2Awxh4uwUuTpjPaeOLmSjANdTzNXPnrlpya+CrZP3bLRG9aXVJ/dWSgO4f1PR3AM6yQJSvoBxlLV0+PTL7UytnqzuJz6u9/AvQNPlJQKIJNbFwMr2q2rsNxNtXnd510tI4yiR4siRCkyXSihMt8FnD/N068xYDJ81NRGtgZ5+mv50zwzkEI4nd/YvR5PNrS/o3BjVtTHwtMkdTWdF6ED5R1vSRAU1bGfgCgFukISJZ9Zz0yfXad8k6pyN+n1aoWevIH7XWTaCCHJmZ4yobsELKPlOLKD+oKm9JtB9guTEQSHnG+1XbwTZLs2iPi2uWP2iAEzNVMR3Kiq6NgFuLkK1EJ44bfunxkfgqZopbG5IRoYDSgKbjBzSdVlaEfi33Weyqis6e2vy8FGfqJ3EDIWF1SWOJ1u6+ccMYMcaVJS9nrSjzMD0GZNpKjBKJ+xbOrrRg59q1XmLT+nHTM2eCs6KYMWEbR1C1/NkEOH02oktE90TAP1AHXsI8gmw2+EzVfGtlKXn36/qCj9TadFKePGpo0XP+nAiluGlHFOFnlvEEAyM2Heea+v1MKiD3nI7RQrbrWAysE0sCwD4A/zrNI0dne5YCnqsoXK5TmSmEILvJAOaxkfoVywL11uWRelMyR6d0RowFbCWgC1aE6leXuBrxS4axvV+L+UU7Y4untKKXLGO/BV5mYMyyE2z5tGYap0uriZb7dMIuhMqABmCVTLsZOJqBjQCOqTFvAuMIBioAvjIN2a2PaQdTUXSZAh4vyLNDg2zn9WPas208uWQwCL8dEFbNFkhoBTNGswExJFoTKaypACeLZc6pHmXLPNzHtEfMSgDj/VqPRor2DgY8wsC1DOzIdLTxuj9IfwcJcIlhnFoDly1juYGYi45IIXllDTyT26KIv9+houj6PsKtrZZWpwhWRRrDsRV/ttOvE5Z/sHUs+aPj+oNviJFRtMu0i+QogBTR0pBSx4/UWiZJzuSE08NfZW9mymRKqdQmpVTvBzWLcy1wWtFIUBFEhLvKhKtb1WYRBNqNsIDmtNEyS3y5Zm+1wJHHDYR/IX9tM2sthCl2bZuwWtOp5vMy9yhk3xYFAT8IiT7me6GDnavd2QYqa1PexJIBc1fVXDdh+HOv1eBBSHioRLhQuZlpykudZzI9Z0dDZ2eEZy9Np7PBq+G6Pq7iV2nUoB1CokcGNc4PgO3Z6WEjeR6UOvMLQmVuVHGQZCZa9j0FXT2S8LUGDXfqq5pzDfwwBN4XAL/MGiq2a5WnWEMdI4gUzlkZKQPQFplYyIAlM7G6V9Qyfr1QN9eERM8fVdbXK0KF55BfcoiBPNF3B4SPAXgh6+nVzHE02fOPiYETAdzZMdmDAZ18bF944XDCH99VTf5tXUlhSaDxTDVxgQRxMIlED9XtjUsDGu3XtFGnzk+eTxLHQkLl/PLCsWGUJE1BAZ8BeDQjdsICcbMkl8YtfyNmrCpENjOGCFgzoOlmIpwXM+6PvVS/Ujdp1IYImpxquWV/zKG8XzETZUZyKEp44KbeDX1IMfCJkPD9etZjxTluU4nOuY/7asw3Afh1BTxWRJc6NSyzuIEAazZW9DeJ6NTJ04ThxCL2oRr/3DjT28/XTKuD/5CA+CgGSQY7Qj9RlYDv5+stsla1TYIkIbUbAHzI/+4013CSbGFVJvyDWq1bG6nbDeOsfFxSnE79uciufBOpHortISnZE5yacZhhtM+1a1kC3MLARfN9bpMZ7XWwqJRb+jV9MPOmCc+RnnRfyu+dVeM8Mk2+C3kn863RgUMjpCatGuNmTyERplBPwMa65TtjxrndqNUUbjjtZsvWl/TNy0N1rfVuYc6iNN6PLdNp8v5sH/A1Q7G9YdzyVpUNQgvAaDtIuFQBj+YnblUf80sFrCWonX5srjN/1wDv7FY92gqil3C9KlRXD2r6pmVsyL9zIXdtSeHYvgBLgkkzsWpxw/M1+459CV8yYfm/eYFJV8AODVwfEp2hCX+TJRZJZpL4g0WdjEzRIwTn8AK+bYHXd7M+wXQnMtfpoKZzQ6U2DcX8xxa4KzsvhItqeceyCD8eqru4IlKV88q4sV+2TLeMJnxSWdN5EdFZocJ6SUmmnJPqQMyOJEefgB9qwj8T6D+B5vQxtAmT5VI41hrGFxLwvPVzO0xLdgahsEy0aU1Ed44k/NejzH/JwPPwhEvU5viB0FkmUm3DjbDXSMy4d9zyva8YO7giVJstYzMBJ5U0NoVE67L05Ix8n//uIGW0sXSm1JfS9IWtivAogPsV6L8M89Ott06qiPZRpYRxfgL8qQFvKszmLJiVbDTSr6CWhHRpyeLM/TGL3/k2CRhYnwG/MlJOf0vaWlVmor5RXkeOEOGeccP3jCZcPiyko5jtMQnw+rKiTWVFR4utX7Vcy6RQYpB1O5nDQc5HwzsU8CMCbSfwU+LMZzetpl0R4WWZH+QTazgXRTc+aZSncn1cwnxlDFwwVz4OKNnISV+J6LhVEf3jfsMf2h/zdQzcD2+lkA+yaq3SBE3ipgwo71GsKuDJCcaT44a32CAldl9sg4dGYmtz1wrZ0SQ5tQD0yQTsxmOVCwC3htEa8U+k8Umd6uFWHMnAR6uWPzlb7LFb6PhNZmQcFtA5g4repQh3APgygAdsi/dwQKeJmnWfpsbMTcQrahpAk/z9bVwB7CdU08L1AUqj7FmyT5tyDjeMiyzz71vguF6QnKFwt/H2dh8YF66K9Hk15i1DMX+VgQd8cLUhbUkW8CX4pBwFm5HhB8osP9zmXtZcB1ACN3RxO8vH/+2NFvidhPkiBtYXbfd8MC8d1YjJEUoVovf3len9E4Z/FDPuNox/AeHh2WZoE4bRr9mlNawqqUbWLPmlf2MJNyVDpikMqbvXUvvkxxxWWuCMOvP7DHAmw4fjFghdGxByST0nl4GTDeMzIH6kanFXpOheANstsLc1pJRJcUkBy0LlfOlZ+tlIPCnpmEXS/TVlTrNx32YYZyfgd1rgqIUkOI+uj74ZIYqwjECblwe0eVkAG1v+P030kAZ+zsAvLLDNAs9xmojZyCHMr8WcgxpZC2C9pB3W2amJEy3jrczckwGvUxxQUycX+lclRW8ugd68VOPDCWOiT6tXDGOvsbyDifZY4h0R4aYs5hc4a6apONEc4qM4zcKlWaxl5iN8EqSkNRzIpnQFB5TsDK2DnayZ0qANRNhAik6wlKYyrI6UuDpfgve97IktdtcSp8/FF2bY5Y2c3os6Hwj0hOxWtEtp4JZUhiwtOQf2acOHLF7Lyxx7jkWye4hFsnuIRbJ7iEWye4hFsnuIRbJ7iEWye4iuTmpoGhfnXJFf9jiNFOjOSjy40O0ZpI1Tn2chzvNpKIqn5o1TmkmBTveK8ssx1ULng3aFbPE9G8vJo6PJpWsivU18SAXdQk9kX0KwS3vTkzHIWBGu0cCNNLct4RpQcAukzkyATxWrVnfQHbLTf+zOuvnensRuPaE/crG/+fjh2uxjItL8YJGy4tTPsmKhs4a6qkYiwqCkNGiq4w39YeG1J+hiYo8ENn01+rpUZGF03esnkfLnapJwGWNTX1h4hSa1CR5Qh4NwfJAtTTkgkRq3Hwmn/uiijRU1kvDkhgLw5UZzpJp8beoHEdtdtbPTBEvG+pLC4SU1L6marxrhdLtSF4ToUpHzRjcDvjygabxfB1gVqeILvLsIznZ5kMWrFmMLXaWukJ0uaCK9oRz8ds3ydr/VSCfIVPQWWV2C9mIoWkTSd4+c427ADUREhhVvjheY7e6QnQpPcHQ5+PP5DEkMnJqRLd1/d93ihRpnueBhjXFFnfmMbtR5IdDVAXJ+lnWb5dRTTs/LmlxwHGqOqEN6weui16+HWCS7h+i6i/UAl3VIC0eXB0jnirDdcLFmO161bFuU0Cw52tMV7TdjW1B/eNe8fgaIHxyO/yC29gkiBB0OZeRXYDT2YHLr5eN0E95sZbEiXB6BvtjJ/1HgkRjGe8cs/1mH93UVXfNnM7Mdis2DhvG4LNcrtHvZ1J118pAeU2hDLD9j31Dk3m6ia2okXWCE0r6EXW61SGTc4X5H+YhDy5K5xt860U/Z/X7tzbSb5vYKXff6ScP2JBZHaI3j+yOX3F4EkjL8+GjsNioIfLQmBjp6gSW/O+bBgq5bI+KAWhoQ3jIYYVmgOgoW5q8VoraNJ84nne16GecW+M8FoqgHA1qYVN026Go9ZFdgWSH27uUlDMgerB1Kdf7qfMA3Q6dCKi9PdrGXMeRgEPCukS0SfUwlGN5YDtyWGZ3q6wMFR7gsklI0ttB16abXTx1RUh8eCOjphGfcOXImyFZAu6c5LzayePyO7XRzFVmKOWFxartQWy/RNX92QBQsD+mqogOix8MzkC2Lhy8D8K4iBR8MPa3rYbH5FjHDucVlHj3Goot1EYtkH3RYJLuHWCS7h1gku4dYJLuHWCS7h1C542DAbP6ig6WehcJrgXcTy57+A52mdXURmdtiphmk22jS+5YWciYp/3tI5/8zCID/B3xOaPjes1bpAAAAAElFTkSuQmCC</t>
+  </si>
+  <si>
+    <t>ACNUR</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAFoAAABaCAYAAAA4qEECAAAS6UlEQVR4nO2dCZRU1ZnH/13VTdOI0ALNoigoDEkmIi6Jg4iGGJEYSdwXdHCJYkYTMw5GT/TERBMNRhMzMRmDZhSjRMWIEhFjTDSCRAxqZBqxUREURNmkoZutm17mPM7vmq9vXtW7rxfomVP/c+rQVfXeq3u/++3fdy8qoIACCiiggAIKKOD/E4o0+U+dfTrFks6TNEnSU5Juk/QFSTdJekLSryR92AnGmRfFnXhsESok3QyRI5RK+qWk4yUdwWuMpKskvbaHx5oXmU48tsGSZhgiR3hPUr2kd81nn+e6z+2BMQajsxJ6qKRHIaLF05K2SfL13T9JekjSibt/qGFoD0J3l3R7O05ymKRZqAWLNyQ9K6lZ0gpJD3jfD5D0oKTT22EMWUkTJX0HddVmpCF0Zpfx/Duiv4+RNF/SFZLq2mE8kbqYKenT3ucNkn4AgcVvTZG02ruuXNK97bDojZJqJH1P0vOS/iVm7tk0DwwldAWWv5z3XSX9ByI8QtI0SQvT/HAMhqEuDva+ckSe4X1eJelSSbXe5z0k/UbSyW0cz1xJv5c0UtIfJX1dUgnflWE7eoY+LITQvZjkcZJ2QOTIxfqJpC4Q+BZJW1o/p12TiVMXjfzWD1EZPiJ372JJH3mf7wOxL0nLeQabJE2W9JakvSX9XNKNELsBqbmHhU1EVkedn++a6KE3wM2R31oJd03m+2WSvippSSsnE+FUJGKI93kdvxWJb1Oe+yPdvVTSaI/DIiYYz98RM+xsxdg2SvqrpLFIc6Qqt0qaB1dfC/PNTXpQUsAyiqAgMgiHS+rPj0R4XNL1ELmYVU6Ly/GTy737Ig69Bn0biogI/8k4ffyK521KOb4MizwCRhuPZB2B97OUYGmcpMVJD8qFiCNOk9Sbh2xGjNdjkU9jVc/JIdZJuBlvxSfyy5LOjiFyFq49HZ/Z9wZeYCzTY353El7KvinHGKmFC5CuL/OcGiStWtIavJ0JSQ/KR+j9jUF5B191g6QTJP0FQjyIemlMMfiuqIprY4h1L0R+1vt8IH5y9PpvfjfyTg70rnsbKbkqRlWMRwqHpRjrNhjuOUlT8eOjRe6LW/s2132OMeZEPkIfTOAQYZ2k5ZIug/gRoS9C9z2SYuCRdPxW0oWeu7Rd0jex7Cti7ot+60wmUw5nnoTn46MWSTkJG2JxpKQ5kj4TON56JOFFSV+TtIA8y0WoN+defjaHyvoYPqEj8bwVIlg3axEq4zb08gBE/MoU/vMAFmW89/lSiHIXhI68j37m+y55JnG4cbnEfKaiq1+GKE94qi1insckHRs47h3o94Us9I8kfQOjOJ9rSviuOzFFN/8hPqHPhBClBA8iv/CmpJ8i1tFirIQDNwQOdjA+8nHe53P5vbks4o+RmLPNNb14xaE7Yuwwknv/HWKu4/3PPfW2P4seGtgsR9WtxPBH3P1dPJJ6rtkXpovocpT/AJ/Q38DAZc3knmPyl/B+Lav2UuAg98NAjfI+/xtGNdL/X8SFdDjI/F2XxzVrhuMcDjAZydG4oTuQvPs9zu6HH/yFwHk8x/M2IPGR2voSQY1wLUv5jSv8my2hPyHpU3BJMSIrRO08jFgVfvMTgYMbAJGP9j6vYaCrELtz0N9ioDb4qcZXjsPbXrBSY3zu6LlnoNObUXm+CxaN7z5SrSGYSTS6HDpdZhY2S6CUMX53LKGPIwIqgZur+TzyTwdJmo2L81zgoHriXcRN4n7jj3/KW4imGCN2T0xeIxrfz7zP3vT8+WFGPaxGv/rSMRA/e3jgvJ5Gwp8hrjiJzzfxvgwd3UKCLaGPhMhZxH2t+e5H+IrjEc8kZHHwx8VcV01CyGGksQdCLP/i3fM/JPydmmjAFfSvW45edtjLS7VGqYRXY8Y0FKboF/Odj09AxHMZk8M6GLSM9y2k2BLa+ZcRkfqg+IVeighzJyv5QcBgvoxYxWGOeUY3BmTHUZXDxVtgVEp9jrC3mWybxeGGOSKD+HAOvz+K9q5GRebDmwQuUf7l26gkESH2MYRu4Sm5CZajNoTOKcfY3cjAogDhfEQ4KXnUlftyJXNmm78PQjVZPJYjnD8DHeh+I1c0NtO7/xDSnPb362PuE87A0BzfOWxnjJei3yPJ+hbM0dvo7BbBlCN0P+P7NfN6hQzYr7GuGwhzk1DB5HJhqfl8uKc2miGUQ6RGDkMKJpnFi8Z9Ftw7ypOIebikDiWoJ4cV+MBxiLyGQwPm+AhSESXE7sbgv8I4nLTsZaXDDbDOXBD9+z4icDMWVKzeWiWjIuGKbfwbLexXvAhxPnpWcMbVBB5fiikkZwl952MPnJdUjxRaHG84tTkmh21R4Y0pDquIcIUxvI3xrDLS0mRdT0foTSbC24kOvYIARnDztMAo8B+iIg+DeHsUiSmLB41qGosRTsonFxFMnGUI9HCM+nB5m9IEZigLIHQ9wZUb60Tc3tWoFvnejSN0jSFiA9bzWt43khPO5cvGDTQfosDnFAxsF3PdVlRBM8Q4JfD3HE4ydmY5kmBxNcS4MsHg7RVAaJGWuNW8/xYRZw3vba9JeTEPbTJu0Q44zSXRH0RPhyIpZXoOLx9zzRi6psyyCcPawzDNbC8UdpFge6GR5NUoItuhuMhOAl0sENFxQsYo/7cgeD3ZNZGuvN4LczsK801ivihAMnwUG05sNAFRRyGL9F9MzkMQvAI6OqMfGfOvZkj5CY9iK2FpL1ZkIjmDy1MMNkTs4lDplazSFhP8698nMZ8Wobn1rtDlYIKXZVTvu/OMP3NNpK4GZ/hjFIXOzejHWpLnW3DKR6fob8jlOuXDBxCmPVFjOC0NtgcuchYO/g42YYqR/PeJQI8me7gyg/K/hgvm8O8zJI7OZcUaPcOVD60pglZ2QKPiZnzbtNgRSOgirhuNqv21iUqnY5hvgG7LnddxMj7pVMTthwQSX+f76hQJ/tZw9GIvR9EeaCJHkhZ1gYRuhC5FeFKRIb4D+k3Hdx/NtVUZQ8BLiOOnkCs+1WS0VuQJW33Up9SvzSlcx7RY1YoF3B5wjeD8N/n7aPz4p9EOaygOiN+flyFZI6KvgaxKb+OCRQvxeoqB1qQ0iB+aAbc3VrVCfYQ2AjV4xY8T4GpXbXcFhcjfnp+hQtBIROfSmv1NAfPFlIPdlrIqXtmBHP1RK1rVagKucVhk1NMYk0hyxec6bN2ODEl412k0EX/0UJMgmWnKNyFoNvmM0MFuTnF9WryaQh0oIQ/iY40JgnqZBNkZ/LvE9ZlkuPgBdOsRRFgu+7aQDN6EmA7PXGhOYRA3xOSP2xuvYHNCEUrogaSOHzASP5RM4UC8r184JnJex1R8zixGcD+I9VOitUlxld08hA5tvVq0Gwi9JkX5TYFRcBG5mDOYq6u0OOKXEFX/xt2QofqwhWLpWqKdvujOx/h+EDo7xJcO5ehauKE9+qqT8IiXB8+HkB7CLtizQRD9UaT/UBh1DUWEeph2/wx1wP7ossmUY8YaIzmCiz9JcJOEpHyvw6KYrv2OQuQ1PZnQlSrEPMSQF6NeK6je1JDCGEMIfgFtFAfSQbDLGI6G+iJTN5nVd9Z6GOH3AYGJnuYAy91AFNqa5sjWYk6AT705BUcfQGltBJ+9Tih+kdljcxEqd32GbWPXmO6gu3C+XbXYFTb7pVAdSV7E1j2wXW0J/c75sCmQ0K4r1aZz5+NLP8r7C2HaKJ2xS0c/gU6ZajbaLMYjyJqCaFlA9USIZ9KE6r263u7A+oBg5KNAQu9n/u7Dv8tQFxH+FXqud81GGaKyZ6h834XVdCjz9HLINoKmgARRY8x2iN2BpITX2sBUg+1C8tXpJOhYyt6XXY0/zr27G+r3piFwIp8XeYFKqI5OSnk2BUy6tXntfEgKpD4MzD7mShlfSidrNxjp41KXI/RCCprNcO1PaILZ4kVVoRFfUpNNc8KE/ObFEDQFGNcktRDK0fYaN84JlLa6MY5f2tY22w9xvYnbK9hpNciU/wXhQ3Y5heSW87la22j3agxwyZq47q8BbcRJUrImYbFKmb8NyJYSNU8xavYl6PcxLKE3w/qu/PPPkr7PvuutJocR+Y3/ljDgbQmBSFGCB7OTbqcDicBybcRZgbc0hIpQkhQkeU1Jpa/vQhe3F30V99xk2ig+oI7YImjz+6Nf9vbtnQNhl/KA7VQObiSAyYX6gEEn7XGsZyIv5JGQjdTm3gsU+SRC5/P/jyHe6MG4diJBQ0xrxDpUSJV/s51sH0Lvp3BPlhGzn49TXmk4tS9VmFwD35nQ1ZQJdBXdtblEPm3Ak0917MgjERFzXee1M1RS5ruSa95CuuaRmGvRO2IJHbks/4W4Po1P/Tv0UjFu4DZj6MZiMOPQgBeTb8J74mSFfOeTVOeRirPpH29EJTQSAJXAMDPIcTwPh9/j7a1pMdnlNIDcQ+RTSUvYBRD+b4aAzcT0F+fwrRv2kJ/cFmzKwdH9ifK6oBqct/QSG5smUMR+A06+j3taBEeW0E2szOdJ7w3jofejPtx2ijoT1Y0h7PTRlDLZ3hlQl8P9O8GkiJeZec0gl/Ew8x1OJXw0zNpCrfnieyeZtzF0Szoirjf5C1srK8vR1d+U4LMWm60bScinZvLp7zgkuYq+zu9BT5/7/VeMwdxo3Lzx0Gs0kvyQ/2B/0/0mdM6xJJG+gu6227waiSCdft7Kw0cQEdYxofdwg6LPapCOzSSrfhzThJgLDaQkBxDOrudVyzMeDSCgwzuovBLG9BZezUx25L7B/HqiEnriyrqQ+3bP1dwHf/kHJv9xHaF3C8Rtut+H3Icrzrqm9MtMRm8Ig+qCdzEO12cAsb5zx9wBIlkTzjemaF1wKEEKfI5rauWzsqa5s8kLjPZDBbyGWnBlqnfpTHIV+yPNJiMnVX8g//wP9ilOJKtZRXdxEVtw5xhVssYcVNKP1zSjcvrzXTMcWYeh2d4Kwghp2G5cMPdq7bPcWNweRkvkx1AB93r7u2eZ7NyJ0OMQQ+SVpJtjnYBcuu9VVsYGHf0g4mmoi3tN9DeQtoQ1NJPcZ9KH/1ewL2roSDywKlPVrmXuDbh6M735rcJhqMw12Xy+7B8IXBaYz3pQPj8L3eZKUa444FTLOPYABh+Fs4fRD8Zxe11mo6rcvO6EkVyPnc1iPk8EnfdwlKSg4Vl86e+b+L6MktdN5v6B6L1Zxts4l9xAZz5bT0R9t3re0+NEdi5/0Yek0TSTIq2i0/ZMFiEv0hyZeRhtY+Nitqz9iVVtwJK7jfBuE/rdrSZDxyJLuekWwxDvkDjaG6m25zw1EGLP4bvgI45Cj8wsxwq/xqr2x3AMh+i9IG4VedjvcV8p6deFVL07Gw6jv9lK3RSMbHfmPQv1+Tre1IfGdvUOjYBDCT2ccHs63PsBIfls9HZ3kwu+He/DHWHpmkr8jv49jW6khW0KYYY56GU1UXJ1TK3xFPzsb4cSOlR/LsCy/g6Ddz1Jpf6Ik80B1OCxzDf3fy1G3expjGS3g8OTnPPhelJc7bMZ6T2RwKQKg/hCmgJzKEc3QNwymtPdPudmjnJw/W0vsiDVhK63QPQebKd7vZMkmyowgFnGOg11V4SnMZjtJocRuNnzQ7bgCPwizQ+25vzoS6lm5Nqe9j6uzlOEq1EYfyENgD9DJ7blMMK2ohwinUd0O42xfoacxbF5TjlYggeW5hypXWjtQd3D4OwTOT0sFxqx0H0R1Y3c09bjNduCsQQfPfGBt5ozN3JhManiO1q7qamtJ6IfzsBHwhE2ZN2GgYws9Bt4LJWomLiSUZbJl5g8xJbAynsp6ilrwv7aHCF6bxJghzD+T2JrKryqyHuoxJfQ36FNkrFor6Pne3JgiDspayuZOndkme1525eq8YHovgqqx3ubY4YEwep41noW60W46yBC/eEksvaG2M64N7JAtWbBV/Ba4h303Zdx92GxyljgVRC3XdTc7jrj/xj032fhnl4sTtIhJEIi3oXw9uSBjSSHBrMHOwkuTVvNwi9Crf0+4N42o6MIXUJV4mQiSUfcpCS9Kyr8Ef25Ei/gOrh2Jt9/muRWOZ7NIjjzWDKMxwR2VW2C6HPJ2s1LuS0kGO1F6NPxLEpd4zXcWpJwn0tZLqIq8SRqYgcLc5U53PUZiOCCnr2wC9dioG5ATZWQU/8imbajGUtSq0EDOn01C7wDb+TO9iBQexE6A/eeSm6gnIkVe3qzEb1bi679M+K70nveOHOM8tUJ3aml+MCnET4/5BnBCnI0x+MX9zSV/YwxvK4gUcvvPkmk2C4HDnSU6qgg89ULA9cEN26G+/yj1RzcSevfhGh3pPjNM9lzM4vgKldNsq9pIi9DAraiRlYGHs6VGh31/7CsT+jriMM+EPd0gqLHU97/WxZxOoS8PIfPu64DtkMnorPkiodAoLMpNqQlssMCEj7DMZwjwm7reHQWQhchvueT520LFrujGwKMcQEFFFBAAQUUUEABBaSGpP8Fdc8BzQQn6S4AAAAASUVORK5CYII=</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAFoAAABaCAYAAAA4qEECAAAgAElEQVR4nLS8B3hcxdU+/s6t24tWvVfLsuXewMYNF1ogdAIJCQSSfKlAGpACoSQkoSdfCB/p9ITQmwGDMTY27k0u6r2tpNX2vX3+z9yVjQ22gf8vmcfzyNLeveXcM6e85z1Dlj/dhP/WIACfsKx/C5pVdcOymqvzQ+5dhgUE9CQkS4fIEfxh5+hv13brq781O3TfyrqCR9M64PcCLhFwAnju4NgFD2wZulXi9H/OKs27yy8LV21s771epByh1MFZnAWAZp+AEEpB3nQL+OG3agSMEO7cZwe0Ozr6YqRzPM5TVSOh3Fzrwnp/cm6e43vTppRv8ztF8B+e4b8y7twQhXDN/OL/2gWcArEeePNAzoZDwzPqgqRxekFgl0WBnJAPFsdDhOV740DPF1oHkmUvSNGz0lrm0bRmwuUQIIkcnAKHl5r6L2na2z/j+vPqnqwt8uL1nQNlWw8Nz4AMgDPAQ8hKiRBbXJRw3UGnhNyF07G7NVy9dlPrDMHvQnnAY/l5SxlKqa4/vduCf3jcmy4ejP7hynkN1+uEA/0vSrqtowtCgcj91y7gFjlaGwqs28BHlwRFTPqf2aVIWRTvd4wgmtKwfywzqyNByojbib6oOXtRgdsjylKS6joEGEgpuudX4dRpzhx/+vRJhc8MGU5kJMkCDFwytfTJg7p2Z0ufwrlFIauRFJxFSDTfLaBtaBzDSc2E4MIZlYHnL14244cxKqvNQwlPgzR+yh1vdNz75PsD1+VwroEr6qp+q+jGf00Oo4O9ELoT+n/tAiLPoSTPvYVzEGwZSK56qmv8Dt0iWm1+Hkokgi3rD61wUguzywPY3BadNAhh9vQC/3sHB1OIpDUMxbV5/dF02dyy0IYkkTv7xjWIxAJME0G3K/zzOVMO3vjcHvREUhA4Yl/T5ATUl3CIa0kkTAUgKgK8OXZZMdcxoFGc4nJhftDbXOyUzYv/vuextzsiX71uQcV9hBOYVfuvjGllORBqfe6Tnju7IAl4noBjS/Mz3AnHEVS75Pef8nu6dw9m5sb7wiWFMt85buhISQK2DyQWhHxyuCTPu1ZvHrmifVSdvKiCvueTCESdw9ahTIOlUkzzcuvL0nEcNL3giArwJhImFapznPjZuTOwe2jcFrRAgNRoHAErDZ3yABEILAEWlXlKeeSIlPg9oHtHFHCcud7jkc0xleaOunm/2yGPmf8l81FZXgoh4xBPehB7y5JG0R9WEFcJCCGf6SICz8d9Hs+e9tHeCtHnmto4ubCTd4pQU+nS7rHowqWTil5cWJ3/yFOb2684GI6cErUKHuFcEnJcMsZ0ZQVHBNSX5W48mJagqwJEy2kx4QkwqUKBkmInqkqctgJIAORhAVv3pmEpBLJODBDK5M0JhLOt+ahlYlhXMKAbgm5QIjl1mitwBlM381M+GruW/hleSmlBPgQpJJz0ICZoV4aiJ6agIseJfInAxKcXtksClgxJe3Z1kPM+GEjMFh3OVzpHkuhPKotH06qnLuTetKSI+6A4KA9v7hhZvr29yGWltfRYKp33RtvIqop8V8eS+uCGAdOF7T0WUiJE23MRS6AiFSwLompmH94CqGCaap4TdCSFI3dJYFimqWNNTxKnlQexqjiAbTvHLleTGa4wP9AWGUslxijBpzEd7Do8R9DoMpgz/1ThSoXbB+GTjmOfUwuwCNCbSsM7loBmHf4WAf0Ed60KHApk6w2I0s/7I4m5cxaXo1QEHtkan0M4grpS394xXdLKg4GmrT1jK/IFq37qlLxd65qH5iTipnfWZNerLeN6ujcVhcBJ4IhCiSTj5QNjX9zcs+5My+QooRxldypwDv6qBuFrIZ6sJYd9PEeQVqnjG682OzZFTPrUGVzlA63DN9zzbt83nC7d+O5pZTfHRdnSrBOL+ehnNEBQoyXgyqgg3KcLJMpzcnBydT5q8BToNHmYDj8KKWybDWJBFrKnOJG4DQLU+ANNVU2xgf3D8aX7o2LxKZN8A/2be5aX+JxdVS66nfe4UFfg2vtB6/CKV/uSs+WQb9euSHoudA1LCsS3q3kNcYgY0TmIJixKLARFnp/klrt10BkcBW+wt2Zx/fXFOfE8tw+79vdnb0Dg8Ern2MW6NXK6JAvWyr/1FcVjFJUFvvAV8xq/Wy0Z79Jo2DY7RwaBvWiYgJmplCTR/qNFKUpkoNJlAhY3EVJ+8vA7uU8vaPueQRHP9aFiMIWKHBlOMQbBkYPUWBJOQQRM4GMBKQGcPBerDzrfX9MSuWSgd7g+7s1RWgYj05bUFz7easnK5PEY5uXK6x8T6A2DA9GagsYA2gdH53q8kllcXrFxgHJIpAG3JsKhOU3oBk6vDzx+62l1/8NRLQhQzuB5oiRiSZ/AKx0ZAvPwfVgWKvK93VUFuQeUDHHW5Bqv1HrkTaHysnfLoHelRnsh8uRDRSHsKxacLieC+bngCAe37JyQKUVxchhg8cmn1OaJU342QbMvaKaFtG5CMUzwxEQsY6A7rqKAT6FfF5EiHLiPyFoWOfiDcjM0AodbKH6vO5GXHFfFpVXOd+bkS2iOAXJx/m6/ryczllYWdWZQuqkrvmpykX/LzPJAs0aB1lgUOosmBIUAHHRTUPslFzyKNe62NGjs3iyCeEbHgZ6UbTIou2GTosYrr51XX/PNuCJiVQOQr8SxTxOgZ1QITIIToSHTYKa1bqeMYI4XbpaiZvOiiUFhEWJnkp9ldA4mP5ugDwv76AXD7pEtL5Ez0RAUkZZlEOtYSbslHh4r9Na/t/f9bHtPbJ5uEs3l4lGbk7/TVERMdWrwevie6SHf1gOR+Jxt3UPXjKWpa7pb3PbmgX6qGxSqJUHkhaPug9rJd5i4UUBYxGHamtk5EMdonMIjkCM3mFFUkQ93AI4qpDUJad2CQZnzzPoYpvxMwLLkgFMW4HZL9jOaTHE/q4COM/qHEp9d0CcalHCQUmnkyA6IDjGbFbNJgQPhFAsNtwV8Yt+BsdTn3SKXaiyQN5ZLyUNqRkNTUgABR90+x4Fo9+jSd9tjPxc4wbxiUs7a6VVBDCUtvNeX+ZgfsIUBgmGOCTuNhAIcHDUgEP5YbSCEylSDJ9UJS6+2X4groyCfaIDTCZ4DErITMmTkejhkzMx/NCV3y8J/TtCYcIguNw+HUz6S2rBlFuIpzJSemVfo27a2LXoBBx1nTiu8bdNA2kqbaRRXlyDgkLCg0rXrjb3Aps5xvtgnd8WSytub93UjxTlg8d7j+h72J7ach00HDnXFoZgsuaLMNB8jLEp4EFNBZ0snaqoLMJOkmCEAdbnsc2TcblhJHRb9z+eHz7VE/rOCBiaWY/YRJn4HqfXI1JU0UCzzO4yMcgFzDasmFe2YN6kIigkkx0ZBElFUubk3nR7eSEcUYW69b9uCKSWZjGmhK0IRHtAAiYBqlghdhW5YDiZMNtkLUIysdrudov0Hh8CBjyoyVBOmockwdVDLAK/pkCwR4DRYLGY9LNj/Iqq0c2D8Py/oZCwFh0Oy7faEVts+qdlUUVThefN0rWSWIHBqY8C/2ZM0IVILOw2KpEkgu5z95zSW/W/3sFpdWeh9itk2O761HKgKOCFxBEphoGnyzMo3SotC2xjsIUzIyCXwOH1u9RGbypA/2hpufT/tfGNSEbYWBESkDRH1ObmQBR6aaoHjOHs12OviM2a8n2XMyyX/WUEz4SZjSfueQ/nBI8I2QVFamAtXbu42ly99MYNADZlHWDftt9BQkWd/nwcMwcq9oboEMDw81qrZtHiyB6h3ZW0TDbmfm1Oc91yVn4csAGQiBGAClgXJxmPYP4Z1FxXmvjp7fvGrk5xJ5HEZhGQXCgUHOJ5geCTjtdxBp9vvD/MwAE6f0OqswMkE8kr+A4peVpT//+ZUyUTUIYu8/ZOzszOC1HgCkXDkmOXIPLimm1AnJvuMm1AkFgEwDJFNzTCg6gaomcUuWOqqM2DUzJ5DNy3ougHTzBqnbGKRnVY6A2qYE3+n9jG6bsIwLSiKgb7eCHZ1DaArPO54uyc65c2R9DzC6bAi3RPQ2YSQJ5Sc5WTqUc/w/1fnq4qK/t80mmmGRTjX2qb+6z150lBpjvevpg2BUehDCla4NdR6ZFujP2kc7wjVAnwCxRx3Bhp1QKecrRkM0DEmvnBYB93JOIiSgSHw4AN+9vbtzzXwttfwqGOIqGk0jWrYPKhVnlpbNGnfcGxWFZfSpnm0t3TdzKegSUIFVnvAe52jV7buDFdetqDi3ik+dzptGllE8OjxKe16g1f+dIImE7GyRT88t8chYutAes4/tm59cFtrdNGDF8y8eG5BLpQJVJcdKxs44hSPN5jGDCc1ODQN/kInMhxvJ10UnP3z1FwTq4MplCGOg4ob4waPEjeHoJuHSKittTwo3MkUHKoCymyupsEYHYNckGfb3+kYwTR9FPmShoJ8EbUFOejRYq5O1br47f2D563ZbX3lnEm593++uretoKTytQSVsGMM2DeuG39at/P2Pf3jn7/9zPqf1BY63xxWnShmr5VlhRwPnft0RbACz6ew0WQiktB1fY5HkveYPDEcPMGGttGz73mv9+/DYSOvqMAzVunW12ujgziSq1CKCMeEUgSXeKwmsGPYyxPcPPSYBadqIWAY4CQes3ItvDeeQGMogLPzDMjMGarEBvwljkLiBczz8TCpCYNa4HUDkpIBncjuQLLCTo6MoUoS0RiMgiMiDMgsnIZqCnNWNhQtu+rZvedZBo8ZRQ53Zb5DEgTH290jo3He74WUK2GR27nu1d3OsfdaInO+NLzvme+fU3/Zikb3mmHqQ2pcwYGx5PSGKUV7Pdwno36yDbl8gvrLhGBN0+DVe/pGLrtmdcPZXS4RhzrGFj+0ZvdTEYv3sSV6eYP0q1w/RjO69SE0aWMGOgw9A1H0HpY9DJPC6+Tg8IkQxA8PtiZeaqWHYpMeQ5HTa+uKQbNntCasKJuarfX0iNGkH4kYbFRN16AkFbzUZWRTZvZiCUFXNLpgUyx5D8MzJAlYVhU0l+TJzeVF/qQEG+pGkc8JL3EOfWVR1T13vdF+V19K893+8t6nq2XnyuI65/ZDqSH8ZfvgbUsV/tUr5pT8OWNYJ7XgskggbG8Z+dgHHDmcWnPgTTX3obVND8yuKdyYL4pWrab6ztne9mjE5HyspLSyIfTK5Uum/oGjFqSjXhq1KHSTIqLySFEDliRCEgimlThQFBAhMCDnOCWNw6bDpMcuSiYE5gzTGcWT4/MnBZ7LOj3dArWD6ax5OzzZ716Rw64RA1vDGmQ++3fdtMz+eAbgJYTcBibleJWSgCOVY0Yz7OURTgZHAmC56pdPrf79pq7RpesPjZ8ZTcN/08t7H3vmG7MXl3vcoxbnzNz1Rvt9NXmeV0uDnkHNsI5B/Y4eWtqCMC1wbCmLOZv+FEXCABw8jzf2Dn5/LKr6SpzWaCFP8dimzm929ccr2Unn1uZv+Ok5077gMTlVNays5lCAEzhs74kgRpyoziEYjxuoKxWR5+TAOyUb5LNwLI7AhMBN/MRHMRVKUSBRGO4Adh7qXNkT1yNVlcXv2Z9bCqCq9qoglIpUzTCWQpx95OCAFTVumDkBODgK9nKiKSU5sHsUPEzUFvpfyxiZW3TRuyMb/YjQNRmpWBbNc/Bc6pbl9Rf9WGl+fUf36JJDY8nJj23pv+bSutBvXJw4Gk2MeNfu7/32pUvqf5YmFjjLQqFLADOtR5uTne06hFn5ro8JujgDdMcMcJS6dvdHLocoocDBdXeMpvDgluHvEoHikqkl931xQfUdA6Px0wQirOMJ0Xies7XWFJwIx1VYMm+D9QJ3uPbIgHMcI0hWwJV5C8TSfczc8tRIywKXJoSJglUxbINOnNBpHk+Q5JzFT2+Pn/Uly/nejEoPVI8bcVmGxHPo7BicYUXNmM/liJsWs+fAaY2FWOx02ohiCsALH7QXr3fIWy9qzNn8wzOnXz/YP2aHfgmnC7BEEJ0iaRgwCI+4Zbp6w6Pzf3XulPN+v6H9njX7Bq99ctfAj+YU5/+uWzFTLJB/6cDo178wr/jeYqc4bqUVCJwfpnRsedAhEQjacZZvQASopGF39+i0vmiinBnTPNPYzGWSlaW58ug3l025YWGJ78BvXm16YnqZd3Dx6VPfZOFW83AccDhR4pZgMjjxI7bzGA2eCA97o/El/2geuDIejayKpXU55HOOU9H7IidwrwamlWyskRmElqFRg0Nb2kBXVOeV5FDJLIcLAvHwskBMxu3QNSpFR1Pz5sysfVyQstUuFmpSnmP1CTgFYGvz4Jlu1bIuWFC/oLHUCZnjYLgd+NeWfnx9VgG8EstbVBTycYjeIDwCn3mpKXPFE7v2fP8rq6Z8b35VwatPb26+7Zmm3soppcGWXQNJDCYyeeGUvnBGnufVYUOHSj9urR/timSR2A+XKUsiiO00hsBjw1Dy85oCjsVh9ZPKY1VFoYHbzp46V0iYmase37dlc1969SklJbc5eIHKmQR2NXcirllZE/ARoVqmhVhKQTyt2lNRNKw71HPJz9bseue1pvC1G/tpxb6oUPhuT6ZhIJq5qb1vbP0H+wd+ELVc6NHd6EkKsBQVa9v6VjocngVRg/t3NJUpZWETW0V7ukdW9KhiWaFHSrjVJLzpKHI4C4JJbYGva0uUbWgbO2vOsro/XDArFw6Ox94RHQYvIaFb4thIZHIikShkAuBMA0kthWZDp9OnlN39zmDm3O//a89Oh2WR319+6vyvT/M3ryzzHRA4y6Cmia0tI9PDiaRdJGB++KOqu3ssBW5Es3B4xiygZSQ65c87exe/vq8Pb/dETmVmI8ibSm6Op6s5bXke3dj24O3rel8Oj6vuyxbV/poTvb2tXaNIxyK2bGVRsFPjo4cdgbAEpDUKZfsw1J1haHtG8Nzbw99SEjzPwjowLEjgQCiBYqgI+Fzc9v7w3ftah5cOD6noT5iBv73fdvfmA4nzynN8ueF48qLWlB5IUyBkaEJz98DZc6blPLa9fwSd23ch1dUDSUujyEXgkai8t6f7B186rfr3IYEonGKiyOtB92h66nt7O242qPbrlvHYip6OTtvSiwRoiuv4+4COA3C0Xjaz6s6xMSX44xe3Pffwxq6HQ+UlfpfT2OOTuAjL0fcMJJYJLg+axxLn9o+lZ/uRpbMdnktCLgjRjHlE6ySBw+83tv/6g6i8+aHT8ja838J5OzQdcyrz3h2JJN03vXno+QMDifnMlk0tduz9xqLyu3mRg3dUB7FkEjX5VXtaeiq0qpJ1ssC12cuW4R2sxihw8BV5oHtViAJBMpUp7kklp0DmwDPciJqgeho5Pi/8DgEPrmnB5CIXuXhy7leHFDT9cF33My3h+HLCW1hZ6cW2vrBVksM7EgR469DIBTGTCg35gYPrd7X7CzMaxACNhRUVYR+wYUvH+X4ZBzxBV9sUAN2G5fv37uYf9/SOrl40qfzpG5ZW3uLKcaYi23fbabvGcajIdeEKSQYTeiZYdu/e7q6LDw6Syc9s77qqbXBg2sXz679SHvIeGI3p+R0Jrb49JXEHh5UFW/sGGm9Y0XhBWp+oKDCfV5QLzmKhFzUAYiCaThevb4+fVWgoRlGuBxmD5jFWii/krL3htb3vHxjIzAcnwOXRlO+unHG1yPFxU7HAEQbLCNaqmdXb+mLJBdc+sWnPmr19D0YT6SUsCLOxEApoHhfE4hBQkIOk31MyrsfzGbjJ8IirZhXijlU1KPc4MCXHgYKggOV1IXz72b0XPd4+sr5lJLkcBo/V9QVozHPjhf1Dap2DD/fFMs6NzUMXn7+o4Z7hgWhN/7j6rYqGRlcmEMQ+hweb+hMNTcPRi8+bO+mvu9rH8ETzwLQHX9u9JZmMn/rg+ZPPuWZm/n0iR1K6/iE5iMXllOdtM8CQ1IBLjv70jBlXuV1EYWZ0V78y5//WHVhf7ZdreVFGOGMEP+hNeeIK0f7dFP781q6xqvG4gvDErC1wgSsQTbBZLlvY39G7OjKeFpYXUynHaQgxw5KZYF/Z2V3bPkLyIGssy6F3ntVw9akNwZ0a8zISZ6e+TBPyfY7xG86ade05DcW3vtUb/d697zStf+DtQ8+3D8aWGpZlA04smNQVMHiYxRyUoWNEALb0x+AkDoRTOv61P4KoSrA/nESSc7uf2TM0lZmUopCIO5dX49fv9UDRhW6k9O61e4cvr3XyO9M8lL9ubf/lGQ0F/8otKxykJRUocjvw3r7ury2eWvmPZMoytjeHl//w+b0bS8qDm//8hTkrTg3pI42eMTQ6YnCLhwu6zIHartq277xJwbCPmpr8LT85o+YqF0cNiBQ9SRJ6vnmwlPI6kqoldMaizm6V5jIgZlAzVksBNxi5ks1pHkB4X3FkKyMSwZu9mYsZ7jiQRtFAmnPrlg0lQLcr3DochqXecs7k6y+fWf50CjrcjiykY8WzyBtDyVTVwpWL6u+pDEipu9a0PLTm4ND561uHzz+tI+/P1y5pvK0hz9HnlgBTI4rT5My0SQQqcjg4lMCa0Bg0qHA6GE5CUZvjhJKh2JrmIfAWfrGyFi+2RPDElg7Mq8lvS0LkM7H4otMbK+5+6fX9d9ROK/zraFGonSQsW0Bd/eOnk5RRWFea+8pL73cvem5n6+tXzK5/8LrVtTeqiobhUQqdQYNQIMoRuDgJ1LRANIr8DHcMRM0S1Ksb6v7ppm7fz9/Y93BCVW3Px5IrVjtoGozygqEXgYjY0jJ6+kKZe9jOsADkzaiGsKNl2D4hJRAOhPUaFjJEDVplQXIQ5q45Zjt5hPxS+NKawLXnBqyX453dHyJyDNhhoDAv2hgGi1gCIsWXF9T+cUjlnI+va7snQy3y1u6Ra7sGtp7+05VV3zi3oWztEDU1OAilKmXxOojgxNqmhB0DLi0P4NLGEjQNRLB1MAKIAs6sD8FpmbhzfRsgyyjMd7e3hFMNhmUl3use/bxX9LYucATfpGO6ncBIFsX2tpErFjdW/DUZHin909aetcvqy/553Vn1NxZGRxFOmKR3VPdZmhJjfiTHbaLU54WpG+B0E8nUIFjoe7SwWRa0vFD6013nTIrf/k7nA+ERWgiXxnIFOjAUZkIIMuEPx5LTBXeZWxZ5Rp4FC6uFy6pcdryrGqZrzVbDxbxoUskU+512Hi1A1zGlxPfaJafU3N8xElm1J4WmAlnsNA9XgEBtR1fggk0y9IoEISkLIt25vPq+oJUuvH9994+IJKE1nK7+7nP71sQupF+ZLgjPujg6BIuUwbaJKng70QZ2DMfQPhaFavIgDgeIrqEy6MI9W3sBUwInKVhRFXxhUFHn9o+kVuuZxKGvX3LaF5sH45if1hA2OTzTFl4cT2bcC0pc27/x942b6vMcB25fNfUamtTJ9l6tVnRYBgl5HW5nXiypqhCdFpy6NoG5UCgaQcxwQDgK+WdCTyT0vI54pv6ahVWXb24dum5Du3K+yVFHpSyhK5kRmGKOpPTSpMuf5/c6UgyKYOcU3tvTauMOhgV3xmCCJogpVFZNQibnS4fOmVP1ZHnI9eSLW9peY7JvXN7wM+3jHBkIY2M27OmYCOUwgZl8c0XjTfsGUpPfahs5l5NcSOhp/sfPNj362xW1BV63oIKFDbwOi9XxWBpLCZIGQZIVBzgKQnk7Stk1EMd+lhAJIqpCvn6nw7/5rR1Nn9vVFWu44+zp9y3gSKZX0eUkB7EuJ5gMR/ounlrEbXnw9Z23HRzWG577zrQpOW7TiI5poRcGkhfm+Ylzcb7QRSLGQTh0cJyYpR5MAFch2cS4mUa3ZqcRR4YkkZG3myPnZZLWWTecM+O8U8rSL712cP/180tzrHjXKNdvqVDhltb1DrtdDtHmmvjyJAiVfjc6R6OwwEkmtWy6kWpRR8+4lrl0aeOynIDD8+NHd7zdNZyceed50y/ym0TPfJRJzNA3Xs4CUUdlgOx9RBVYX1s6+2ud0Q82tEXG63giQ7Us7hcbBu9lDtRmclHGaBNBj3ogzuYyZhN3jYjY2peAyehnGlDjc2+cIelqgKIuGHQlGqtzn1rfPTpl4972a/Jqiu4P5yRcY4p2mc8TyDz7dkfllQvqf+32BQ7G44m8rkji0VcODS4YiqW9Dzuc6s1zCjomlzsGLRMDoOYRaiSzmgVOGWZuwZHiAibwk2vnq3d+9997nr/rjQPv3Hvx9MXU0/BEIdWp2SV4GUwLA/zgKBUEkaIWYcSoB9zpU6pQW5ALWRQPI/xQwcs9qmAGMhb91b92vNk1MDazPCT0rKoNvpmABZXHMVPjKDRZRlyhiCSNY+bgmAGnyA/fvHzS1zyCoJhUAMdbiKYzSGgmZEJR4pVxmJSVLShRZHtTbCQcDBnUCVuVgu0TdLfUpftk0pdQ5i8sC7zePzQy/663Wh8pKCz+I3X4+t47MHo2eKXg8R2RyknFoaYbVk66laZT4stNQ7+97q3eMwciatAyTME0LbciKa9oY4laZZxwacWFdMZhz1TGCSvNg8+kwWtpcFrGnoaSwZTC4Kt1+d6Wnt5I483P71xfw+eIJZJDN3RdsEsdnEFFg6MFvIA5YhyCKICzdB25LomxJDWBBQ+UPSixeEslf9va+tfdfdE5zNFds6D6bofbmUyxzA3HzgwIVFFAdDyFwf4IhibmQH8E7kwErtQoZuU61l85t+w3MNK2mbBJLpSDLFKsmloCzqbAkgkLiSPoMwsdiV24NbOFUkvHGTWBA0nRERhXFG/nWHraXzf1PHL5KXU/qpbEbuYfNnTHz9s3mEJT3xC+OLPkdx5e0HZ1GzV3b+69qicSAxFNBFzO8RlFngMey9xlqKbCS3Jal1wwJOfEdIFKDswKxXBK7jgW5EbsOS83guUFSf3r8yuegCyhbSg2/cWDzY811Plkpyhq9n0LxCjPk7TzqjkEJeBvnUkI7xzs+VKZKD5+ak1Z/G+tB5IAyahvabsAACAASURBVPVLRqant+fmN5ozX4KooSYnp+OM6sJHecWAy/o4CEVte0zhd7PalfkxEJx9zmocX24svnNvT/z093tjiy2JaauAtEbw9PsdIKyjgJiwwCrZZhbTpVkNNlm8zkpXhMLlEC05OrZ/S7cjzxI4YX93uOHKJZN+nomOSZYlnjHocx/a2TN45njMwpQK775z51Q9IUsWPEZieixp44VoyHdGP1cuPZzj5B5fPLPh4HjfEDhZpYJgHYMl8zZ0qsIyjn1miyM4dZLrt1V53OWdY8bkV/eFL5hTIWySZaEGFg+HAX1ZVSjFOcG1dEjnNY1nXhCe7ld/8vU5Oa//s6UvEtfNDAOVR5J6zaN7h26GyHJjGd9aUXeTw03iMZZpHGfYbHuOIK+o8AgcerxRAxjXr6q5ddfju9coFpGYfWY+WREZEqfC0jmAVxgn2L6uxaLzD9M1my3jdMnKSFqL9hopf8YQ5YJC13hNwKPs6Q9f9ZNzZ1/7+o6hK8ZicILyWF2X/8yQzqc3xNPBF5tHvl0acvYurM39R0ND3f9V+yyjnKepkIOnjuJc6Bkle42jbp7lBs163jG+48hwCMoPFtf/5PqX9z1nSDzu3dg3WxZZOich6MF4sUcbf7lHk3aMuX+2OKS/IHwwFC9amKqrXTrZv6V3bP/w1ni8YSjJcZSY9jK9qLH8LwvynM+nurtETuD141W+2H3oloW4lotgXu4JBZ0BsKKqcN3Fs0sef/T93q+y+9IFCsEwbJLh/FIJPTGCsSSFLBhI2hwNMuEcs9EMz3FaQU4o0zau5DIqQI1Ldq9tH779gsaSS1MZau4cjq1gqyCQI4+f3Vj1h41dkRlrt7Xdcd7k4N3fm82t788pTShEhORgQQ1bQcev+Nm8vngMYlj9GO5pK5NlCYurKp8/a0b5Uy9vbb88pQrQGMLFZ1DmyW0iqplcnM9Nf/SdRPG8hZUQkinTJcbH5n95Tu2W1i7X7q2dsWWMp0oV1k3k23Xt6ZN/tHFf07dn+R2PSITXTyRFux4Yy0D3nLwwHCPABbNrb33z4MiZQ8l0MTElgJkMi6LW7cbCShGdIwpyXTL+smMQRBQ/JJfBxmk4VVU5i3JUEij2945IjYXu1jNqfW+NZkbkHX3hRSw0OWNS0QEjmZ65bmvzjd8/s/FnDbnStubWHptbwuqC9HDd8QRC1sFhQPCBeuhxqoGEcajFDVvav3XejPLvtA2OVB8c0BZQIbsC3S5Py6jhwCst4YvCqXRufVEBhAK3bPyreej6ryys+n2pL+ctkP7rLd1Abb63+5cXzT3n1YO9X42b7qKCkuqMbpgnFCATtCjycFrAccz4MSOQ7+y7cG7xYw+92XYji5dM3rTDvCf3R7CkRkaB5IDCbD21jlC1sudkNT9DDo+Puh2eMkOkPDKUh8YLByIZU81o4vyeqFrFOxzwctypd73T/NSXTqs9c36Jd1cslbZXzacZNg/cUuHy8kdINR95Wrg4LpM2leCeQ/Ervjpv8ln3vb1/42BancJM1sq6wNqqPBEbXxo6P8/jII2sED0536muPzhQ/cetA1+ZWlb4QoGnVSt2SQduvXT+52Eo1tMbe275wfzA+YGhVqgn6Q9j2iHwPKY11EE8ooXHHxIBiuZX3//GnsFL2iNaNeEECJYKXaRIKxR1ZU6s6czY1WxCs5V123xyJpKqIZeXVpYW8EWdr1vdzKA7unWd3rJjAGW8Y5Kp6bwginj+wLD1zSVTvh4sydu1OQZwqmhTEcgn8DAOU4Ef79TQl1SyRPXjDNYwNE69W7c1tb30l4sbX7zp89NW/e7tg88NjKoLZgSMrY9u67p6d294+srJBa2sLCucmi/Q9Yck/G7dgYf++EVx/zeXV3zxtLryt4NucfwXL7X8cyxt+ipyQj0hxsH4BFW1CS2qCdcE7nGSt4IalzR8+bTCv935TvsdlGdsJglEpNgfSWLfZsVOvxkfgFr0CB+Jo04YahpD1Fk7r1TezYspFYLlyLHyMM/pQX8kkmfxPFQzg9U1xU9fMsX3Ym8yOtEaR5GSRXxyLyGFzgk4c2rZSY9iEUk6YzVt3NWHp3c333XD2bO/JJzTuLx1KHZhP/FW/WXDznvBiXDIrmcZrUVYUlOBX28NI5UxXf/4oPOuW8+ds6rAK2IwkqxY39r/OaeX0/7SQw3WRvFJ98jaLr7AGzilLEujPdGwU3YTWDat6v8e3TfwPz1Ro8Qu1RsCMswUG1o28tAOU6OyyYudxHAUb7b0Niyv9iVzRYmG9QxqglzepZOcuH+zUU4zOpwuh/HNaWX3eEFQN1HuYWTzAdODIQqM0xO7EfZe/W7Zxm5O9sBM0BnZGs13Oweebkp98YqF2q9OrwgdmBLwP3Hb8zteG0ppQfACLpkWepcZXGF2oRPlbjd6jBTe6cisvDocW1bjy3v3te19X48nNVdBMBgpEv0aPgX5SSMUsSSPkYSFk7VWM/fCDELA6Rg5rbzwxSeHO75lSQIk3lKLA/7e2YVoLZZo1Od2mE6nk/KEEMPUo5lYZtcY5VbUu4XdgaSqnjqlenW6LZObpGqsOZLGKXnyXmVa4MWQWz7oErGH1dBVPUtjYKFaSJKwgBfQbUy8w49YBbYiRVmC7JIx4RJO8gwAFVn4wvPWMKuuRy+/drnn513D48s2dUZWMjPl85C0LFj7u1nCUiBLOKXCj55dCVBLwR82ddzplcjil1v6zoAlwQVLnVbMKbB3ADi5qBmAsjSUxBRpPAvlnWCY4BA1JIyoLiwpz/nb1s6RxefNr3ykwet4w+d38y4/59rQoRfsHxoJCrrNnWWNdtSiDkuQnWv2muPcKztGvsZTXyIvD+AtM/iPA8rkQo/TdBd7X4rrhKxNe868ICiskQT+CF/Q5mpQYAoPe+UYrGBhsSSFO1KgjkfjGB2LfCJfmsuyTdMCrBh4vWR7T8fnrjLyfvGnTd0/02CILA9YXeZ/saggr7/jEGP88yL+Z1YxnjswANMANnfHF3WHo/9ULL4GREdxjtV7VqM3ziLZk3lt2w5SE5ONRDadPukwEUAGCYcb02tytn9XmHZNZHxw+X0f9P5OU6zpkXQ6L23xonGYj0sO7xSRBdkJAww4Vh7jsggfwxcshkDaoK2NbwtEQ8/Uqnt+e/6UHynHuR0nMJHu8xAEN4hHZl0EODichqrTk8p5Io7GUMI0dIooIzwOKOrU7S1D/9w5OLwYnASeWFg5veavIdWg+50mhHAqiaVlHswpLcSWjmEQS8Xd73ddMs56HijBnNLcF3N4mKzvWjWPH+xgwor6GAZ4BLM42aBg+HQ4pXme2tZ5x5v7R7/QN64U2mRomxrL2yk3IyUeRs6ordgTTFX2ue0kTRaCgx6dj7KYnDOgagRrOnu/e9FQ7f953XKbeVLvzArIkg3Q1zaWfsK9T4xoEv6EhTMssv6h4bGFUUMSf/V+50WKxtsZ7JSi0O6llYENmb6wZAKa8MaBDufFUypxy+JSnNczajeE9o5nnY7s5Mz5tQXP7eyOVMdGIyhwkI4TeW3biUgEhUVidkuHEyU27LEcEp4ZILNvfGHfXzrDkZlgxVtRACGGnalRm8bPTJV15DvAR98fOeazIwaVMFPgAMMcJE6PQaAJlv+Zn0TdZ6glz4H7FL1C7PGSqlFf4rD0M6blPPzUB+7rxzOaM6zq4CwXLBLFJY0FN4UVU/3X7p7zp0wuf0EIK9xf3x/Wvn12bRBnVwfwcssIRJ5C1yycVh9cV1rgO/THNXseKpSEgStPrb4zdZIbYablUCptl+iP+1gUNi9te7829Xuv9zw/NJ4sh6jb7b4Wze4bwvEcnISC4YmcAJuUgpP7paOlZWs0ZxhwBcWBLy+bdmuRQxpOm9axLcjHu3fTROvAOJRP0VsoCxzWtI5/UxatwPnzKq6qKfNu2N42sJojEiySxoqa/DeWTS95szcSPUPLKZ3MviO8NGA++U5v17dPr5qBX585CRsHYoim2UNSXDiv5vbEkIBN7dpZ+TlW/Czqu4sSah7PVNsInUgRC7iPK+RsGwaBZVjeW5/d+uRQOFaeFxIxKbcMM0M6JuUEEfL4wMlMKS0YumrTfo/QnvHJYY+dbDCTY3HQJPkWqSD0l4CbQ4jjTvpVpuxpmHC4nJ8oZDLRqv3nTSMzhuOZ+m/OKpbPbij4SVN3aplipCSn6FC/u6rxhyU+gd70QttPvza79F4GgQhfWlXXdfOfNkR+sq4r59crK5p/cVrdlute3v3lz80sfXZ6ee5GIaOWxjU1T41oHjra73VwXPS4TpFasPw+RJzejwmETpgWkRDs2Nl2wcIid/6dq2oZdwb7ogQ9Q0N4q2sEI+oYxlQTaVWHZlC7iEyPssCfRqvtoy0RvKD9ZsWkuH/Rqsb7ONCTdkHYcKgBbIpkE62TXcemBVPL058yqofjRtFrnYnqaTVFO5ZPHn3h9R2pS7+xsOym8bFM0y07em/Z1Rtd7Jhb/OW0yUE43ccNTC7y7/vNW91LNUN9/etLptxwWW/c+Nyi8t9JMmhTOD0tpuluFyHCuKLmF/td0ePtuGBaHHJkAeUif0xWyDQkyahmER0xy4S3qPKDcqvvuUe39Hxry0AKgwmGlZvZzk87ikCWc8pMBhE+osaf7GTtE1gqkDFDm1uHf35gVs0/Jaej3zqJM2TpdFzRsbGphRWpj6yi4wvabl4KRNNGjmERCMnBnFrRi+8trf5JiZNPnDmv7oG/rNn2/WcOjNy2uNqzyZ8b7IsMJyB8MGJiVV3w0ffbx5Y++H7P93jR2fPTs6de43VxeLaLVSmSFUwjMhpk3Zeb7yoJtLCs75iuVNaswwGFNvR4rDw42+4CbsbmPNj+tZf3RH/QNpSqh5W2U2zG7TsMgrIlT7M00ywmQT/KpP+klIl1iDPcjZkoASoEUfFC5F0EJ9mOw6YSu10cfjTda0c2H+0gOHow3L07oXvfPTgus7Zsj2QVjA+2IVQ2qf3qRdXX/v1g9w3Pt8bvZRDzaTXVj7gt3k7dBFMzUVmY/2Rpbv8v+iJa2YPvtd1X7HWOrp5c9NhAdwRj4bjL4mF74w/6aE53xrLb144mMrKCdWMRD5+Ds/fnOHoI2dTc8ft1Bx59a2f3JXaLg0OGQb2Axfq2DfCEMwnHUwjUhjY0y7I3sOMJz7jdR7nWT+7W4wyH/VN2aOZZ1cFf1nucXZxAToq9MI0eHEpga/NAFsg6/ju01ZltqhZWkW9RiOz3lnAq5JA8WDzFg1e39F7517ea7jENHsV5eSMrGgpedbkEYAQQ5lf54AKUq+ZX/fHOV/b/ShcF3PHmnofiAjc4rcqztjkxwiqIdg9h63jUO6BpOKfWj1kFMg7vL8aegXUGW+aH2C2zZQxfyGiW85HXt/+mqTNVdsmi+vtqg3yXltJ6fYbWi5ycoCkLnkGV848liSemKHJK1URVM1Ho5Mwyv8PwuHmNm4CO6YfNACccE/kNqQ45OlZXBF9XFJ11NJ/kS1mqMts5obC4DIxMf9xhWTBjGSTSCjKplJdV8FnK4LQ82vzqSdjeOrTsD+80P2RaIsdW65WTy39dwpmjmYSNXkCQJgR19byK+1/e3XfFnsFk47hheB5Zt/epu7+4YNH0mryWNTtHYAocoomYUO7nMbfYAc/EPiiHn9zQDOjR9JFeEiWTgaEqMBSFP3dq2T+kkHZzo5c07E/R057pGFs0Q1a9wpgyI5xWcuI6daUNzqFZECmlrGeeDhNi7OOJJvMwuInOIJuo9wnmI9vMSbgcyRwam1btznGK/04o+glw5Sy+IYk8lswqRWOe/4Q5Leu34cdSyA+58HJTT4m5tylbf6wMdiQ1UnXHi/ueGlUMD9OG+pKclsmNlX8+YHI23GALOou/2r3Typ3nTrn2S3/f825MkxwDMTX3lpf2PPfz02r/6HURK6rrnFP1mTNZD0om7SOiK360ekmCALffY/+fsTATDhlDlGBP+/DstTsGPtc0HD//f4cydbZ6iRKGGE1zIgm046vDdvGIQnETIPThDaI+ulPICcRMstBch2EUDybbH/ztxfPWFznEkRNlhmwFyEJ29Z1w5y87K6XQNMVB4VIUFTzRDYguiXr9cv2P1xz6XW/EKoSs2/S461ZM+3phiTseVybueJTtlpbKFlyZxV5YHNzy9aWVP7r7jQO/J7KA9t701Ife6/pfQnjKYlufnzP+uvsgnjlIf/XoZUtvDcj8kb3i0qoB1aBH2szShuV/bOOhn7T2ja8iHues6fkhLKon8BEBxBQRU5JoHx7D/lELaZVk7+BwRskYS2SCcHDM3hufIm2zwy/2PRGKoef5JdHnczlGzBMUh7IkeYpo/MQbLdogfyyT++62g3d/9dxTrk4oignBAQkCufvdtj/t61fBicTeLeF7yyZ/31PkW2+mKBxHnUOI7O8+8mr7RYIvL6z834SZqnn43a7rwcvYOhizUw12otIATV1QVYtb3ms+/dW9vbu/ML/yzxkje7NpJQON2XOQbOPOaNxTku9ef31j4QODSvL7W0dSNTuHk1MHoulJfqcHFSE/ptSGcPk0N8t00JtIvP9Wl5rpHY3XE0Mpi6a1rFaTie7UTxtIT1C6YGpYMqXy71N8UidD6Kzj7M9DJrLZQUWFRo9XG8wOtpHK5tahy1/tVs66XBcQ9Hm6OU5A0lSxr5+3u9AsI4PvnVb36y/Orbg/MTSEGYUlR1bIv5mgrYp8+xfm7Fpa+1atINy6HyxquIFLcvGHt3ffYjGGUBauQn2hLzFT4BCggvXAlrafrmosedoji0mGmnm9XhAhDarHIQsi3HGjP8/j65dlAV5P8EeNFVVA86jTbZqrHtvTf/nLm1q+AFNAjs+BOaUelIe846unFj0WosF1hYW++oSmF3fFLDelDLOzddSGMz8hnQAlJrEsk9T7+MGZpcHXqMTZaN7xXBw7U4ytQom3u1txuP3uKKHbAL9q+J7YNXCTQAhpHrUkK0m7HSKMjGYKliDYGezXFtb+5vpTJ928leNI63BiZYCPrKWEHCkxCP2BoP0fdqE9XHTmwXda535xbtVdNyyrudXpkUce3tx5XypjiA6eM71IRsJsoxGeN9rCicp1ndFls6pyX2HwYgnHurBCoAwYoqqtVbYm0exuMIZhshbjzMK6gpeWzy5+6Z19Ay/d89qBB8IxLf+tVIQZss/5Be5zgWBgx+RqZcdkhxVldHt7l4JPo8hH6n2U6BbP91OhqL40b1dL1Bw8uqP36HG4uu6RKFSNUcCpDbXajbe8aB/hFAh2to0v6htPFFcWeHqTaZ1vjQzHAKpahiB4ZYNeML/0B1fOr75f9Aloer/j+n6DwxZJfMs6ImYVQjKW/W+aA6ZXlf/rxqfW79EJN/qdpZP/dPOy2v/1iFbzI+913j9qiVPbDwxGPY18tpve4PHc3p6vLqj0vyLYzZiMsy6ACIVsSylQOv6xtJddWDcMeCiPy6YXP1XkFDt++ebBhw71xmfDISNGdMQiI3O6hyJz3kB2X73PNrJEAVawYOHY5o6xRd8/a97nBYl8lABrD6bM1R4JhU5i9yDqioGxhA7OzWGoL4xR0wlFFrlNXUP/w7JXnnAk7SDcroyo66bhLA4E2392ZtX3FlX4XuM4GY9s6bzm4fc7fvnIBVNmlAo6DpNgdjONruMTRy4sO7nuhaXeF+99p+WRmCI0fmGa96d51HzrwcvnLj/UH7n6VKcS9fsESDShscLj1t6RM/pievnMXHcPa4S0rGw/LMfnwyGl2Y1NFAuO1SfmQBkKOL8qtOV3F804/YmdXT/99+7+G1IZTmB+gZMP02c/68ZnsEMuwrpkFRE7+8dXRw2tJsfjOvjRqIP96uEJgk5il7UMtoHLxOoxCQelvRmVxeVIc4GSTb3x1awr1WspmXl+Wa9YUJ0s5TI/XLpg6lOnlnmHhnoijn8d7LjjkY3tP7x4atWji6pzW/WjNs/YPapBCHg+7Jxl8N9Ny+tve6d9/JI/b2r53nut8tL5FXn3XTc38OhplaHfdnS24u4DcYRZQCuYiKaoq3NsfE69l+uRJBmmyEFhUiQ8qitqUMpw4EgUpmUcN/pNaQbK/O7YL8+e8eNzp5W++I9NPV/Z0zV4aU+aZANaYh1G/LPYxxFw/yMnso6N/ljMy5hTBS5Pa71LHGSwr/WRzfgY89gtcSDHKdSKPG933Xb0dGBfaMritGo42PWDDq8SMJPGpHxJK1s86X4t4MGTm3u/9NKerhua+hKzJQdnXD6/4K6+hAn1I2GOYB21kwSLIEpy/B3XzKu6574NzT9vGVNntCX7/jGazJx94fJJP1lUVddRlx5F/2h3z/DA4HwWbnzQHDvP0MUXt3UO33/2aTV/nFngPpSZsPl54KDlBcApCkYtDqr5cVPABMIe9NSy0Pv5p8vvHxwu/9225v5T45y1ZNcoTilw6bWUiBFTUQ6x+k3MtDjVyCYwNr3GhCBLcHOESyqWYZqEEk2lUkPINfSFGUW/GDalKDU+XFV0QrBVbsAv4mP0A6fI49BovPytsOuaS+u9t77YFllpsc4m3kJNMPiBoVhWOCBBc/I1t/x7+y/f7Ri9zO58skR8ZWHdg5PKcg6xl+igxzZbCsbRmxuwJU2AK6fX3rGpa3zpB12jS6gpYE3zyGVNieSpdyyd8pXrpha9G4qNv7upaehihqZvG4ws/PaKKuu1fW2Nv3hq0zM/vXDOOXOLfT0C29yENWhyHPJcLkxjAF2u094W4qMaRO2XbNmmR3Q6m1ZUeJuKJ5X+aW9nfFHnYM9GjpMGRMN8ZljnzN0RCxnTpF6HSHlJxtICT9NXp/E773o7fMWGuCqJvAOzqn3dV88qf6nSA+xJ4xgSDDMZ5S4gIH1cyGxnsb398bw73tz6nNOVkz63vPqXPVs2LGcxMzHT8DrJFjXHg3faR09/+I1DD7eHx+qIzT2RMKfave2aBVW3UbY7u/HxVSf0qh9TMkgmp/940bTLf5rZ/s7B0US9JMjo66fl33m2ac2NCf36uWV5a1yennRa0V3DaqY8mUoV1hSG/rb2UOyxu189+OzvL5z6ubyCwPDh87HrBnlgeXkQPdoxFb5jBU6z+4ImdQspYsFR6dv2+g7rXwcPdV8KJ+5nHU/Z7M+0a5MM+izOeP6u1lauH9QyVwz2JpY4HSp0iW4Yi+svDcU5uzfmyH2w410EU3zyx4TMsPKRlO6/7Y2WF1p7tTn3XFL0xYMd6fy2mMUsIAJut7l0RlH7y3v7vvbAO81/zGQUnsgOu5GqOkdsv/nMWV8AkRKR2HEejHkuR4GOj04upKOk2jFw5yUzLphSkLNb0zRANpHik/KtL+//4yM7en5WEnTG7BWQMhxPHLIaF9aWri3P5yMHu1Nz73h5/2NJRctj1t8xMQ+XkqpYXZEHXOTEETEDeVJUgMaJ2gPnNP6gptTVxrwUz2lgm03ZkDMv2O6yoqxkR8pViAunlz3M9g/JcQk4pTbYOWqOIKoPIar0YTTTj5F0H6LKAKqC5EhMfdisM4pa3DRd339t52PNfbGFfr+cKBJcL5byyRqN9XNYBCV+J7f2QOczd7+y95EMS8FFJmQTk3OFvXdcNPv8uaWeDta0n+f++GSDv/qWW2yC4UcnM4PFftfoqsqC5wb0RG37YLoBdpeUgEP9sZlJU/OyEr/FKuUBYcOFk3Le2zakLOwcj03uHtdrdFXxFlQXvLrDImg3gbaJ2WoCXSbQw1iXlgW2j6JT4sGiglhaw7hKoGoKZlcFUCpQBL1ivDDXvWtz+/CFaYU4CC/YNAP2kGVBd+93ltV9w+uT1cpiT3PveHzmrpaR+jlVoX8uqQltDMgySt0SZvkJJnl5TArIkN1+JFjpamKy6j6LNv7w5v6Hnt85fDnjhM8o8O888/Sqh/f0xy/d0DK8ihNNRBWVbO5SXITPbp/IIvZVdUUv/vS08kuKy/K6ggLDM+zc52OzNZwA/80bb4RgmcednG4ghzfT88qC/8zP8Q+PJNKVo3Etn0UDbD8imx5gmFhYkTO8oCLn5UhU828YCH+O50Ts7IrNjcpcrKE08AHbPo2ZhMOTJTKsGUcaj9jOhzok23jGkypSpgBf0AmfV4Zq99MAdTnunplFzv2b20fPSSqag+d5WCaH5dML/igU5b42ZlAEnZI1pyBn49a+8Pnbh7Q5p1aWPZTWBatc4HBqwECpzKGIsQQGouDGY+CjMQjjMThNHf88NPbVe99uuY0TJBs8+vzsynuHIvqWV1vC3x5OxKexSk+WSKvbuUJdgavpyqmFN960qvamAGfakCVjD5qM532c2R5RwP/wuu/AoavHnaKusq1+yPtb9lUun1G39tw5VY/6pPSQpjo9qbRSobLKtQp4JcqtnlnyfxUhqWNde+yKiJLyU0HGYO/4ksvKA+/O9nt7RZVDLit3WRyCFocCluKMDED1ODDkdGJYIzZcyZsaqnKcyBU5eNje06zWSIG6kLdlRnnOxtah4emDKa3Y7yLa7SumfXumVxgpl3n4JQ7FPjE+q7Rw3cam3ss8AT41pSq0Y64zCSfNhlos4hpnjWesMUoQIDtF7B+Mzvzx663PqIRKTFMLvZ6R2y6c/D/q+Hh63cHwDdGEWc5MjUeG2lDg++CiaaX3fX/ZpG+vmlG8dXh4dBLb4UA0NWiqCuMEsztFIYwL8gksZXbIAqFmXtnc+9899J2l08pu/ercmt/PKBd+ny9llv52c3ilF8rMPMlMDxm8WJrvH/98Y9nfH3gn8XNOMhFV4br9jQN/+ME5c1c6vK6x7J54JIuIZgwENAOOiQIdSxpMhwjn+DCsmIKw4bOJjkUu0bapcZbFFfk3rp5ad2HHWM9BzopL+V6i5AdlG7yZ2EYJFX7H3ttXzj5ry3D/6kluS8xRTT3LYaf2NhU9BQVgO1D73lfpywAADGpJREFU2M4Vmum95ZX9j8UV6uZEGZaRxBVTC/5SLjhG/aEgt70q1T2jyBgNC979PztFfinF+bfOK/LgraYu6akt4/dVVoT2zy0OtejGifDViREehxAO5pz8IAJMmRd84V8HN97469f27+6eWnn76tmh9ZW5Oeuvk93r2a5eEckBB9WQGE/hnFL3vS/mui7uHNMaiATsGEzOfK2p486fLa3/ZlrPAu1sb6M9w2Nw6iZcH15mAqQjkDmCdZ1hvDtIcWljCEOxGP6/3q49OKryip/73rvvzW52lyTkseRFJIigEA3IxBoRVECs2gqOj/HVqQ+sb4eZttYKhbbaKozFDlasxcdYqyiPUUFBoCIESCAhD8ImS9jdJJvs6+7d+/w6392NWi0YW6bfzJ38sZndvWfv/e455/c7v1/XqAgt4SSIqkYonEJTGYJJU4QJ5+yYnsfkW9tY22kCS3c1eKxdrCpQuBmWpTmj7pFxXo+rP0SAQAK8tbPzmbb+0SmkyQq6okGpxx26c2r5b1BSAtpt12+9un6ZOhyHjiSCBGeFClpyv3loYOGLe4KPeMyMtLy56kkKj2d8U5n8G+s0Tu/KxtF6xFDgA/PPW3bPX1r2r95xbOP7nexI1cRJGxdVsfue3q+1XjazNDydSiU4GUFggiXx+LzKFT/f3PlGRJRpgubg9c/775nutm5rnlz2blpSjQfoF6EUzHOdufeJ2U7Dog5YXFcTVChlOagM+CAja6Zf9aW5KYWW9wkhO5AwmHhgBKqAQYBoHvAcH1a8YShKS1JWSFEsTgyRBCQU6gTYCAR7j4UWbNzbey9B2A3yTCFPKCuaKu7nLXp8SEoBzbuIthjpeO+TkH9ROV258bjeFDwZXdwRFgNuJ596YemMiwst5qz4tcL0zCsJ9Hi8R9LYHcfn6nzuxguuW76p5a/tYdnXHm1f/u4hdrmV55Se0MnTJWY0WMCbNTNDI6y94+AREclQQFIaqCoBLx4MPntBpe+fbhsfxT32Uawq9h2MTfxyIYd50gpQLhvYGQqSspK5d2bREw1F9lXxaBwEJ8Ab3TGYBBIsnlwAipcBZSIPvNUDKWDARGGKO6CEokMfYiDMAKQSkmv19u5nMc8PC3HhAsPKEURLcOjhA72Dj6YlmRwWjzPhjO7uS+pF27ukHOFD1sHtNSfXLKy/tspuPhbOYv8CFdxMjth5tuuaPruvUP6E839nlPAfrVw8ufmVvf1/2BOMN+FIpKUs0xpRyloRVwZkHIxvjWEqmjLyYWNbpgG6+pMVz398/Le/XzDttgGRUAX1K/SK+FKW89uFDP4xeqJJkBkrPDTTg/U+TtX67avah1NG+8NR6obeY6NQjiWh8wg2BikohwVGFA2E0ThYaAae3peGmxuKoZlT6Qd3dj0XjGWq8a2KQAKCZeBkUqNfPDDQmIPQ8pk2keeZ4JOgTDCnnNl97zXnP1HpdewJJXNBnmiNgcnIRs7eJ/9OHxb4GksIq+DOri5sm+K1Nm88FH7k47b+20IpqjqL2fnYl8rw7slNWeHBTgwImzHvjXSM+Cqgv9auHo4Juk5asEwbCRaaAJMhp4RYGhCJWw9YnhSbmRmCgCQJDE0Znz2kIvh4SIDw6QxcUeOEbZ0kTNIlqKZykm4mmsAmaJgMTzHIIPMRHKlpGRkL+pMojWkSHAkDQ0mt2q0P1U50HQmPpopFGXkMJEQfAzDV3IFyBGiezoLXZeu6tMK17o6Ly9a6C2xqXMJB1mCSLQYcqYI+DhrE91bbzeAZFZbS7ru8dtWFXstzpNU0d8UnJ5tr2YLJhCaWIw3pHGfGM95dXSIVXNpYcrhEh22tGWro6loz7IuInFfVzh9OCXWv9kiBSNvh5uGM5FAURHAUaDaGlMvcLi2iwgcKYes5PRg7Luuox8EzceyWsaFtEObXu4E3MZAZVT2nBuPVqigG9owInlMJYX5fIu1PSwqlafj9SM1p5jSv3XUinjFtGRmJdSgqefhHl057WHIkYDIjFEQZ05UbPuudXqqnXSzF1aU1ZMNFkcdMjwazzP67GvwfRkXpkxJOzuIGmKTgCwegzDqcD/I46Zcd32MkTBRTgIfmaU0FlbfB8Z4wFFf4YOX2DnimKQA2G0+ksioy6yp4TQT8rl0DsyTA7Bqra+OuroBby171aq92UyqVqsnoas40xnhI6Pn9g8p9ktHlU4EiaSBpHUwMGphR5OktsjIbj0qmtmVFes3fQ+IdrX3JqqyS9evGrT6mg6Z9tRfhKxTl3otgkVGFFlq9PdfWMe8nVMum62aVhJAE4d3DOtxkSYLqdoLMs+DkKPACAX86MgozsFBWMAJuKguVHie4nC7wmpLgBOFLKsEYhftMsftbGwDR8z0CLSgZUFUSCFkFiuchcjoGDoaARCLJ2gPFKMlwxDtHBFt2IGhdPMkU2DpsatzVemq6IiUvCWbAhytE3ACmDO01wBW9AeaSOh6pzyuSYwVdEoGTZTOslTxRYjETipSdcjgUN5r6bgcPMYzjazpUl/EwCRMr05reO5omE4IGsiE5Rhv3KlZGIBBr5CX6mHcdBicUAJajYKKFTrMm2+65db691/jVfZuCZA9f4kpfP9me9OHCN6uSqWFRGlI0yCgC+JwWsDsd4OPiYIXsuK9mI9Cbj3aNO9CJ0QRImSyMqZ0SeTBTQHDjlqj4eCihemIKxY9IulmWgddUMifpjq9UTHYmtPycH2644zpCywUFk1MYoziJlDqY/SUV/m1LAwVbT6Ql5xuHQo8KCXGJ107vnje9fFvDBHNby0C2bGvb4A29idicBZN8XFOV7zWwcatfaonOGQkGm0MiNSuSAL+mpwAYDgiVxm5l+Yct/mGx21PuOWI8uLEzHEliOyrRZpYFL4WyATs71FziXmNRTJsA5SYPUJ4DM7fBChNcFIzXatII9KpX3hnnv+fkgv9N0AnltPKqLmtkj/WlGt9sCf2yPSLMwfPrwKi5XgjCGSx8jdwypoDAgdPCqn6e6vIXOQ9f7yM3CK6Sgwsq7fEP+wYdu4+GV+w9Eb17cpnz4H2zqh+r9tj3k7hE50gQMzjtQ9DaFZ3y/OHgmp29yYbZFZ5X60sLViys8SZ3RVJOdzbW+HaPsmxgKDE1IstViXSWMWAV/OA2qlEuT87RctkFbidoKrAcD1WFln23XFSyYtpE9+72jzoUXASNidNiWeZFVxZCmZ+HM85r/4dA0wx7dj/Dsy1c5ZEUhVMwub5swk6P07pTyMoz2k+fuv0fPdk5ekb1UpTmVVX8ACFRBikhzmRJ/cBrC1Z6XB9lCgo+vXsKd2x7hFIu9TMgigjebhm654Udx9aYTYrw1FVTl805r/g9jGgJKcm49U0cC6KigkRREPDYj274ccP87d3RRb/Y3La2tT92c1QmHllS7/vz5YXOD0Zg9IPGxgnMDtFWx0bDszoGo9fsOy2XKrJm0QmySEGIpwgOQxFRkjUNLQrYPi/0F7/s1MW9NeWFQBnnRxqGbGOBNtDM/8Lh4py5VuDUTwICSj3mg031Fx7sZIapWzyyu1RLFCGnnfDaLOjlAyd7dwh85r6FtapPFGHDAL5SKJjpoSGS1Xx/3NK2bnNL35IlDcWvP3nltAcLzGwkjrcV9dvj8cgwXtBBVBDMqvS+u37Z7E/X72xd/9qHB15KxALzaprKfnJTrWk4jjjFpDBHll5YfmSAD6xPb+unFrrSTMBKTBxMZqxOiwlkxnZqbZQaeaCpWNvbm4LooACyqmFZ43MVnnPsw4KQcWtl8O6raZrVRA9aJGKQd1rBbeGBo0hDGw/3PCQdQUU6CYPdBHyhQ+XaHd1vd0ajU3+2oO6xO2dXraZpGjIYWSdy5JczFesoT0crMDPxdTdcdENNkX3l01u6H+8eFqqevGLaD6cUsz1VvGJkS4KMvQN0jCFrFoboxqKC+MBiARitEVAOhTnXixgX4fh/WLiZr6Gc8CA+xs4Bb9FSXIQ6VgdJ1vh1W7ve6xxKTH1q/rTbH5pbudqBCxmQwUarYCN1YDHofpZvivLy7tg84f45tU+sXFj/087+0fN/vfnAW1pGNZ/n5AzjAy2PX+koV+x9dZz74H59mZhz7JU1nmVUmDjD8juAmOAAFxDSJZHErsWU95W7Lip6WSfwXswYaR9N6EZPGjcrFIqAQdzBOcMy9KIBGQ6at15cti4lZv0xIVPCAJVNijmGiJbX5/p/rIEgS54o93g/60gXacPhun8BqMRVmFFA8HgAAAAASUVORK5CYII=</t>
+  </si>
+  <si>
+    <t>UNICEF</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAFoAAABaCAYAAAA4qEECAAAWnElEQVR4nNWdCZhVxZXH/wVNI5vIoiCIIoK4xSgkIS6BKHEDNUqMDoiRiUSjcRIVHJwYFzSJG4mSSFxQ0TGOiaIEt8jiEtQ44gbioKK4IK20gNBAQ8vSN1/d+6vu6tv3vXfv627oOd/3vn7vLnWrzj11zv8sVW1k6dE1ap4UlEimr6R9Je0uqZuknehqlaQvJH0maYmkDyRtzT2MQJKJ/XZkkm9pLBrRSSXNkL9tJR0n6STJHCSpWlKppENzXL9IUqWkFpIWS3pC0tMcazbUohn1ZR9Jv5b0rqT7JJVJukrS3xC/uZLWSvoSSa6QNAcpfkrSNZKWSbpL0nuSrqPNZkHNQaK7SLpU0g8k/S/MPhemneedP1rSBkkfS9oiqZekTyU9DpO/KWmGpA8lTeP3LEmPSLpJ0qodOcgdLdEnSnpJ0tcknSrpLEl3og7s376okXWSfizpJ5I2SdrGyxhJO8eiw+9BX98q6WxJp9D2S5I5aUcOdEcy+mZJt0u6QtJwSW9j6P4i6RBJJ2Dg/inp75KmIpWt0dnrJd0maSYzwaqT4yX1seadtmybwyT9UtItSPYOocZGHQdK+r8C11hGTZfUWdIoSZ9wvJ2kh1Fno7yp/qCk73GdQXItfc7fHpJelXQyv3eR9BBG9QReSFv0+OGomjOloKput+ohj4OwF3mQTEoa0alRJXoKUzsfWSmbLekrSUfAvA7ANsuM8agBx+S+MMceG4q6eJnPTzl2lKQBkg7gnrVI8VJmxw8lLUS394ejcz2YmIusKntAUsvGYE5jMdpO/wskvZbnmpZM6RWSTkN/WkO1AJ1smTcRBnbkngmS5kvBm6CM1zF2S5HitUidZdzl3rOsFN4Nwx+k3TGSPpJ0hqQ1kpkpmZKI74k42qqs0yX9oTEY1Bio43Ssvp2i8+qcCXAKTDiQyUjRqUCwc2Lt7Aocsy/hF5KuxqitjDEiQTiCiyRjX9RgST0l/QhdPRH938G7eAtS/o9QbwfBhTVnjHymzwfVXABcbBDDG8poO+Un8f0ZIFktmZpOnwbCOAgDOKZAu/sx7a+UdK2kndHF69DlAQztGsE804drZmIAZ0UoJfhcMtZ5eUwKXoxmTtinKvT+xzLmeWwGzToPMlgvmSeZYRNp871iGdVQY2iZ8Cu+j4Q5lvaKmB6KdFfJvBEZoFCynsz4jBuRpicRjO5wYwXooxKV8AnSOyDBK/wtjP0Wv63BvBidb+3FQEmrccv3kUwl7Q9FLSmahQE2KKPLXqQx7AjDWqFnhRQ9jIRbPTw6Ykao/6wKsCrlhZgeTUv/CfOGgKlnRhKqY2DcQCmwzs4l6PHjE9q9Bhsxhhdu1cIg2nROEgw0XVArxzJL59CGDQl0ZkZ1zTqIYhhtO/rvSFZ/jtlB7i/pRZj/EMdtMOj7ksbRuQPytJuPxsHEssiQhUZwBccCT8KexwbEx7gLRnca+v8SXsgSDO4pobqKbMqrtPt37MilOEhWiPpJxkLGn2cdQDGMPhWd2x2pvplBPwscu1/S+0zDX9DhclzptkU8TxjJdnxvmaffD6EGfONXzbHNqJcbCDw5+oTfF/O+AhyhFhjtQ5hVAvufmPAyC1JWRreJ3mromJRiCG9AbeyKe4z3ZXqgM3/nDbg6awehbd69Br0ap47Av+O55tvMvtHMAvvSD4teehBXspOi+8ye/LaQ8C2+/wmo9xsQyzck9UZwUlNW1NENFdAOg2On1fWeCpmqQG8jGSfjvTlLvRbUUMhRSKJFvERLGyN9GfalA592MOJZpO3HxDh8WkbQaXIsGC36WBYKRqDbZEJUcgMOS1svTLA3hr4931enHUBWie7uTeEuMO1Mfi9REKIQN4zja2FTSKsjlZKZtnqzwu/zaiT4YV74+3idNycw2dKeSPXrkrkg4fyM0ADWyvr/YHiFYexH+KA9x3pmGUhWRrfzvndBf+0BM8bKaBWOVicMoQ/lqjFWWem22H2tQB3jiTnfhTQ+hcNSiDoRLpgam11P0OfOHm9+RrDKzvwjPY9Vse8FKSujfR3bGeMnJKUV8WNLBzPV4xLcKePztuDgRJA8QgW/QV052g8m98vY9ljadjx4H0fmYH7/G3p+NL97x2DdtiwPix4SpPhEtIrBC6aVMuhnmGYusrYvuTy/MyOAhVmolaf/oaAtaa3Tkcr5GOdiyMas/4MBbqXP/fndHhRj7cqFoBZfUMqzPC+rMfw4ij2E7rCV6D/yil6mY+9wXU8vjGmh2Y0wOivNURBafN+d/28ido1F10pmBsZyRTS28FnvIojTQRobvPhMJecT7GoyRRJtUnwiF7sTTBX3biCv9zWm3QLO2euW4wjY64thskIjaIJymTqDKUbP56MOXnh3FTBVxNXLsUE3xtz6BUj42LTMy6KjB4Ep7+D3l3RqLL8XRuHLUA9VMy2nex3PR3FcvJlgzuxYGHMwurOx6Yc8ZA2+gh3DatxzEVrt78G5W3Hrj0vbjyyMrgRLlgB9PmTQTm89Hem5kDEBYco0QfM/YICG4GpfT2bkjoTii8Nw9Rub9lYQ7MYL9ulpvrcmTrKMKJ5LHG9I248sOto5DNfgMGzDGAmGPOVdW5Vwfy56nZjDknrx7Lo0mrBpU1CpjNkdaWZ2hUZhFg5SW2bTJBjuxh1/MTkpi0Sv4O83sPor8Y5EtKscD0p4gWnpyBTXGQZabKwkDe2EgXfq4b8QxBn87o1q6U68Q57BL0hZGL0wwtHhbJ4A9HKqYQoRrZ/xe3mGdg9JEeA9xrMFEfmQNE5BwnX+72TaDBPLODsSzO6kt4QXPc67e0HO1mKUhdGLI5wZ8uQ7hDzL0dUfEETfien3YYZ2e3veWC7qX+94XaNe/1z8uqRztbQJvNzLc7JKiVJuZcauAda6yF1FgRxpHcpqDJ/hewsqi+Yh3cPA0QbXdLGnagpRFwYYozpe1Ax0eFPREvremZm7EzPWINkTcdGP9sIQr2SZuVld8MlencMY4gzT68Zng5ZIxysZ+rBH/cN1RHE5qah8xrIhdB9ZnHIvtuHoRJIBVzFrHd2c5XlZGf0maXwhhf2QApc52SIZ56LPztDubrlP1TD8UyKCd2bscyGqgNGjvBm7zcP2ewJV7d+vc2ymB/1SURZGtyCmcDGBcIFre3pooLIWWwZPA43SUNpg0ybS/y9kYmV+uoT4zaFEBW3fN3kY2RD7HgQP3iVms18WeJyF0QHI4o/orecwij7kWomuHiKZD72seCE6OgezewMZB+M0CGmbkqHf+eg6CiMnoB4WR5VRYXZopXdfCZVVC/AhJnBv6oxRFofFOSV/w/qehV5bh6S18cqu/sy5SRSzFHrOMCz4y+jIlVj5X6KilvOc0whclRVorxBt4gX+Tgo6SmYM8Zg2BK0upYTB0Xps0UQy5mcT0WsSRssrkrEu8l+jv2GhyXvg4Y/QZ3tE4cfQk7PXnZmi7T58ksgZyzZRTNpUyISSnbUurpoy4QnRSw3bugqkYcOt5xNt7OcVX37K+Y04LyfhkD2S5cFZjeEGppqYSrMk05bYh+iQY9aZwCRby5HFU8xF74QRtShcuiwlfCwjZjKV2XEYaogIpDkU1/5idLGroNqfPKVgaKXHZCE8aeFrSMWUG0z28ONhJDDvRlJe8HJpfUjQWsm4LKGdfPGQKtSQu2ZN5JEFERIwIVJ4NUVf50RRwOBcdOr82lNBK/p+Ezj6CMIL8kqBXwbG3eoxuYLKp0yE6kgXvIbWSuZSUvIi5ryUyF4FHpWjUWQp7iRYfwbHV6N+BjK4UiTkfbzM5cQRemLxl8F4n9J0Go/TcwfdXcbcjxD8niMjPcErITZ9HOHa8702r61XY5iCiixyDP4imaM8AG/9/zdQIV94F36bKqG1BNf3poxrDhLzav1laXXovejjrjEdydsdw6cQDUbnLq25LnrULRjrQaCYUpCPI4c4vsVMcPSY92K2B6NDuoggjKu0n0yg3Pf/u9HZuVjuERjUKLdYI105n2EiZpjjYcr+JBLSRvF2oV8/8ByQSZSpDUElGdr1V3C9wgud6hncl6hQzTT9HTWE0ZswJNMYSFck5XxUiEvH24r9fljtadRI2LjBvdG0NEm6uhc6cRR2oCEF88MxXteiBqyUf5fpfypO2CpiG0LCZwHjXBj4OfqSumAmTgwgTd6rfh4MKXWF41/AnMO9mmnhtgaglZuAS4eH0m40Tya09Mdy77m4wwtxSo5opFUJ32em9WCGfUK8+VGE7evetXcTEjgP7H41amVFQ3jV0EH0QUo/541PoVO3oLPdNe/A7PE4PC2k4AQcoDuRoMeAYj8qov6jEFUAM4czs+7xkMN8Lz32kRRcjv6/F+P9Bi8/18rdVNRQRn9ENO8hOlNFNekGJPQN1MYyz9M6mRq53kjLwUhWsQWQ+aiatg+HsV14ua6+5EtiF/sQQx+OGnmUmTcFAeji4eqiqKGMDgD7bwPFxmH4pmFEBpFjLENPOhoomWcVhJL0Ljr+SKQ9S74xF1XBoMG0vRi1MZdwq6OnUCO3I7HlkpmMwb6C2ViGGmnQMrhIgTzSwHWGJsTCz7COxNEaAlA2PlBNFebbXpGgkPSTvBJZUeU0DIQyIFbvl48qCePOoObPX2+yN8f8DHoAhncq7mJiHLt712ylf5lCovVoRKdGYrRCZp9CQKZD7IyNeF3uTdl7YueX4hgsVX3qQzhyn2jG2JIA46DdRgxwGdP+nRwptN0ohh8QO/4rcoJHgpXjSeKtoJS71VCqYXRDV87W+hzfAXvGc3zbKL2dQFnV72PS/xoGqEBMJK9zk0St0bfDvHNfEey6kf5cmYDLy4Cpj2d5WE5qtP06asf+Ao7AeFxaF/doyfKE/rjs/wCDD8ABKcU4ps4qp6RutP8KGHghhnsBCOfcWDOrCCLdEAuTNpiacgearjDdYtROIJFyUEkVEt0TRrSH2dtwhNYDyVahHjYVeFZrVEQXntWB2HIJ2ZNK3GoX1zbAyB44VhXYj3lFx7rzTbYm3oHGSYfNr/VD17o9NfoS8GldoI013hrCZzG4rmK1Lx7eUL7vlaLObzPq6UNc6vm0934joZ2ctD32VLJSfR2udBZajfFcRuTvBGbHWzBlELBtFrCtA7Byr4zPWRjp6eCx2kNF7LFUQKKTGZ3Z5hSkEmIKxyCBByLRcei2lZkwm1iDv2JgIDjbZVsqwMjPeNf0AOGc5C3P82kTs+RdZshsHJGqBm9mVTSji3xeSmqPDt8VSSxFSlejR/0OtSIgNIGa5Z8A7f6Ex3cXmez13j0780K6oqu3YiNW8iLXJXPKUeMzOr+ObnzJdrTB2x8p34P7AReHEBOZ4EHA7wHNLkP3n0NlqmDk4ibpeZFU2AUvKvraEKp54CB07xAYfF4MZ28iAjcW3T07xzrwZkHNaTs2KAwtDsaT7EnC9MY8N9yNTi4F4WRePrw9qIGMbhJxH4hT0RnUcV+Ke55g9UE1NSVDm6JjDaFmKNGhiuhGkOf+3EXQ9ehJlia35d5mNbbmuGXmZYRUgW2ZrPGDJCGWFB/fbhrr3xwZ/WUMG2elIpfHNe1GsE3L6KLxeNPhyu1ALqzbGqGxLn75DpbovLr3NALz1ejbhz2c3PzIhPHsX5P8beP1zyYNTtjBjDb5mH2aV9mkMDEQBMmMNmmkP0j8mu7egjQQY7xzwoVhkX1z1NGO4qHRLYlXNQ8N89sYk93G4cZljpoBo3NKdXV8I7pkpu5wTu+KRDu6j9rpOqtqm4lEJzL7agU1uycYGRuTjjN1u8cHkigehZyStHS5GamOesz+lM//Byr4xpuZZ2i8pYVuf8JmivRys7ZF3WuiC7e3RPfis43cXJalzIWolCVqHcl0fwaOzUJdqesoJSZelmPrN5/i23NGK9FiL8Ix+kJKBQLyaIVqgK+M1haG2Oi5mn2PIpB+EwaiRbTxVPC8ZIazTvxwr8p0LWmpR9mgKtopoBZuHUFAv5rBXJSjHOFAlsR9l0KZNrzIcvKCt9HHfHQWWfsBXt83kkabR4TQWy0Qpssm8r1jrPj+ehLKhnZs5dPrLsPyiLdLzOwUG37MJ9gu4guj+N6eZKrb5Gksx24p0N5zrHmJdguIzN9ZFOQozJAEobRG52tVyXmUBuTbsWtrVCwT3FBzpFbausiYu7w9VnPRJkrb3KZZ34wxPh+N1ohODziJ9jFrodS+Ygs1/exxgMV1jD6VwsHNSO5rTMU+DM7VHx/FWpFRoQRHjPRx8waZelrxTG8mifjII6ijXmxuNYRZe71kyhSEIVT2bbFSaB7whKqCUogX6e8BXllaGxLMX9HPlYRyA/DzsV7B+lzSZS0QCYunm1xHD2fgIxmATzcRR3alWmcwzV7O3VwN9YxtnH0ri039lzGVtYFuRcK1MmGpQyVTYrzH5HKu86V0Bky9l62ARO7ycZjnvNY9SfY6t3s8mfU61NSo4ysqkuJMFmrg0tiWbZE6SgpB1z02ztt64hNSXfE7tsTWn/RG74t493jv3PgcqmAjL9Cty2nn7e3nqE3sd+KWoE3N6AWUf9WniHH/jJVeRcxLgnS1x3aObWD15zxrzheTOa8gYetqAv0l0WXe1phJtCJWg3d0MXxratVRbwrVUMS0KvQdO0IilG4zXJ/ZtZHT/rHS2uQXGdG6kDFBiAqsd7mOhvwa6ddipQpJ5NcE9lAQGt81WfB9UzM6I05O1XN/GXN1ihWsX9T9GeLHg7wD/UAuuZY7b/MWeipUHyasRclU3tXUjE6DYDxKlSno5n3fnLpmrrbJ1rG9nw/IuFN7hxhuTkVNzeigvo3Kx0QT20k+8TZ/kEHh3KBrr6aBlrFxr6T0LK3ercouQMUzulAVaFOSHxlrVURftsRmwcwU/xGpLhWRonNv0SQcy0UlrEhN16P4Tr5pRpAL3kXk6+SSFPs4t+RltObFbI7tlBtfClKYigh0OYn2sWwhJnaPWf08ZBTbwDX9QHIf+8DLI4pysDxOjplGeZnw5q5gUZHb1PtA+JBv1dXJnh5fSXlwpnIG19nPvGPRhlSJ/AkPDs26G3hmyu+wfBBbWDQyT/NdKRfbl4/7pzZzvGv29zbnTqJWBNmu4zOmmJoRx+g3vWPdo61skjhtdqGwsIko1Xys8nb8FVHHqN6ufpfP9mboRgWaAUaf51WytqS2Lxe8GxFbkH9XMWN3jJ7rbW2jMARozDme/tqJIvK5OAwJ2DWXEk5cQ95Qut37v4mGeMTPyTiXAAHHEZtwdIc3xvW4/46GsgD0MG9zwR6EX/2Nsuy2F38tJoXm/wcI/8EdeHOL2FfjLcKnA7luXv02ahjpS0YazvrG13hN+fe2rGk+ep+VqAzHuJ3DgJQJ+7mQfk/y4hDTw61+6r7r6Wwa6GgYq8oWMd5FMNlh7jdx/eO43cTQW+KY/UE+TPzYl9a98Irceu6fMoBqYNKWhK19N3FsS2RgCsKOr+peX9PPrR5m3VBzc+0wFjHL7vdwbTeMlls0tDxaahGMzuHYXEPQy7nYLQkH7OcFrT6v/Yc4iQtGt3m7mq3JZVSTllb0YpvIvkyhddE0DexGVS411NNTK/zfqpAPLSTTu2ZfzyD4ol46qd77Dv+bj1tQaeO47r9z2oTB7grCMgM7GPuiI3RUv2LMqjObvbFttZYCGwq1tRU2obAqRYlZqRQMloxbqmcvtoEo68jYLI3nxtdrq0QKXFbGeke2/3WFb0Qn/QvcZelNrG4ztAAAAABJRU5ErkJggg==</t>
+  </si>
+  <si>
+    <t>CEPAL</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAFoAAABaCAYAAAA4qEECAAAgAElEQVR4nO1deZxcVZX+TlV1d9JZSEJCCCEESAKEsAYhAQJhj4AwaAiLAiqbo0FQBEZFXAYdHHBEGdlE0GFTFtlXQUAFBNkhGGASQghk3zqdpDu9nfmdc79XdevVq06kK+ofc/kVXVXvvbuce5bvLLcimDIdG72JhBFUw9/kc7UW7hsF4ECI7ArVNQCWAlgFoAXAMRCZB9U/A+gPkaEAhnCMv0DkSajOL45VbVz7Pp5bfG8t26NXorDxqVzRNgNwEIAnASzKuD4JwJEk4PNQvQwiS6G6NrpnUwArIfIyVAcDmAfgWQBbAjgcwPcBfADgdgAzMsY4AEBfAA9szIXG7e9FaGMbY5XPkAhvQvXecKXIZUak6VCtB3APRP5UfLrIbezJ3qnuCWAfAD+F4nVA10DkrwDs1QiRI6B6HoBZAP4bQFPgVu+gBQIb/2kAds9M0qJjYxEgj9F7bay+wcl/DiLvA/gyRK4GkANwrHNzicifAPBVqD7uhAv3x2I8BiKHAjgaYvfqJyDSC8B7EBkCaB8Apl5Ws892J7jIPQDGQ+TLAN53Lg/XP/TORb4I4F8APMHN+XgVCehZm/3CRiW0AGJEM65bBuA6qHZB5LPOrSUifxXARKh+C8ALkZ40FXMcgLMB2R9ixNM5vMdURyuA+yCyCYBDKC0HQLzjdqjuQwL/F4A3AHwDIiYtrztTi5iqGQtgb6jaczdC9Rqy/Au1JvTGUR2BWAcDehYUlwC4iAT4OlRXQGQggBVQvYTcdxZEuvh0HsAZgHGwvgIRUw2vlfWvujdE+kHEJOBxiAwqqhNV49DLIbIt1HfsXUB+ApEvQPUqiAwA8DOobgGR3wIY5Bul+nmI/MFtAvA7AP+b6KlatNxGIXRo55JrjeN2gerXINLbVYgRORD3YHJQsqIxAG4EsC2g51Cfv+bKWWN97mrjFef8wP3LuYG/cz0PPMwNN6m6FMAOANb6Zqp+GsAnudF27+8BeQCC0wGYxPSGyJdqTYyNwdEjXByBnQnLTG+eC2Ak4MSeCtUpEIyFysEQMYL+O4DHoPpVVzEJGiipkTFEI+McjUAnAK5PTbcvBvAqDVs7RAyd3AbgNKj2gkgdoLcD8iGAWwE8CNUrA8fCJOJiCC4F5D2oNnNMUztHQfEHQsoet1oT2iTkmwDqXT2ovk7d/NOAAkxUXR1cQo5tJtde4wZJZAJUXygSGdjTjamLt74OxUMQmQHVs5z7RB4DsBNVyTFENjOhasS5E8ChUB0Kwc6Ekjex70tcZ6ueD2Cqz1n1OrcdAX9vAVUz2LuTCf7pCL2PIwNbpKKPQ6uwqCOgeARQE8/vArgBkEVUGNtD1dTLf0DkFEDeALTd9TmwG4BbADwEoK04ikiLS0rAyvZ6hCrq41Cd6khCxDbjUaje5JpJcSCgXwHwE2cAkWcAfBrqCObBYBewDpB3AN0DIsYEp4e5+hg9aoX1eml/WzOCbgbV9yGGW90xGQbVa4kuPubcHowNXB+qGsf8ksT6AgATa9Olix2hBN0aeBWJTpY2QNeVzV21CSK3BZ3rmPkcQjzj0v3cyIpcBNX7ITIbwP9w3NtcBYlcCdUzfd5BHX0I1REQmczN7lGrpTG0vvaCGOiXmYAsg8jmjixElji0EjkJwPXRM5/zRYs8EoiFayGujydSpaxNGf4tABiaMWx8AFQPIgyM21KI/AcA8xinUZXdy+uDIPJtqOYcd4vcCZEzHXaqGrL5BRRDoHgfqu9xA/cpGt2P+qopoVXroLolVAuArnbDomowa0eojnXLr2rG6iVO2AgxxaFY0gQXQPUpiNhz10Hd1ba2HQRXONQLz5iUDKf39zPAIeRQLsrGudolSOQuqP4ngBMhcjzU53Uy1ZXN4SEotgIwACKH+0git7vtEGmnxIzg9x/9VVMdHXCwOqENxpm6CJ6W6Wzz6kx8/xgFb473oJBxeyDQeCKLE53bjMsgPwTkzx5EUjXn5DuEhudB5C2iE+PSE6GaqIGjIPLfUDV08TJEzDja87+GSCON4HZ0u1cD+r8kvKmSK1yliNztxA+QsiZRplpx9GCo9oFq4lbXQWQFiWw681momkp4zu9WbXD1EByGZNdPd9EVWcPvfgXBSl+86sUQMbFewWudZJIC4dc9VAW/cpfciBzaQhL7cqKTXznONndeigr+j/Re/4eu/ylQne3GVdiHQ0qDpx+95Xqsf8LrGDoFiV4bwoDOGsfGwWVu8NBmWN8OtOpzOHN7dmAqmra1Ewf4rTs/JV18JF/T6RRt6XpYZD/OZX8AVzPC10TYZ4GlHfn8ixxrMD+b4zOSsRKLtwgDTQ1cy2yoTnbs3wMdXSvUsa8TV+Qdur3HQ2Q3qH6TQZojyS3KgU1vzwXQyectVvF8UBfOsVs5h6lOZJykFepq4XF3523egSD7QeRYblS/yMH5V0DGQzx28SpUF0BkD4ZNVxK/j6HaauaGjPWNtpgHcAJU+3Nus0MwS3rkuNSKo00FncyInEBkiuvEEPgx0L+5c3spGjecGDsxMNu7kQztUOLm/YlUhkFkG4gFjByJzA1xFE8KfOBOjWq/4lySPqF7AXIDVL8DkcHuxJTGnwU1N79o5D7knCzC9jadpkMgBiNdU3+Kf3tA6Nq05eQIc7sNfxqB74bI15gRGeC4tEgEF8s50cgC1Xf5/iRXGxqlOkoiuJgh1j+4bg2GTYsEi+8Pny05YEbuZg8mlTh+jodWS4yyhHPsciwd7i+EqJ8cCMggj6X0SHXUps3lAse5iKk+416i6lbOdUEMp0FkBwaQDnQus7CmGVGRj0HkX6FqGzYOqk/TfU6o18UN+6knDQKDdDmBRFYzW1KuA53YFneWfq4mVG2Ms9nXrhDZLEBR5CByoCciRBbT6Fnk7xUACzxu4z3Lez2hVK109OvcuV0YtjRdfRr1sgWV8gwwLaKaaWHMeJ1fC0ZzJQ3XGs90iJSkzT1NDxZZ9O9aV0+qRrSn3PAFg1tXvL+YB8QyiKe5toRIK1Tn0S4Mc2QUUmACdSen4N6oOVoOEfFE2AiZFNamr2Wse4NboUbJyDfp1o6iSPeFyAio3uE4VNUIazr4LhLBOOZhfmcEGcbU1RJmQv4FqnNogHakceyA6gTX50HtbEKVs7kTOU6ulphnAiN/xqkvOz4O4txAKbwvbIyn0To43usucaqXhg1RUzkvhLj2R2+10tGLGHwBjV8937/HhRrHDI/siRF+G77fEeJOyj1QPYkEfJrcaurnGwDegupMprMaoHoDA/i/d2cFqWx3+LsWogbdOhm0Wl68L4y9smgzFEMZH9mJjgyY2prA+6/w5HCPXPCeuJal1zCHRqrmXn+S1tuIu8Djwm7ldWsUVa5vwCi+PxYKi4kMIyH3hcijjgRUj/NUlMUhgugfzvTV11wiQli1XGUEwrzkG66OHK4HZBfOLblzW4jMKm2KDne4KfIVqD7HQJZB1iOhagwwK8LdH6nViqN7M55wHnXdFFcbppdVbbGLAkxzVRX0tXjSdCuvx5Cy2o99oTB9fBUzMN+FSH/HthZ8CqjgJqqNLnLybIZNrYNXvZTB1FXwMrcDdEgxD6i6GUQC6gmEH0hVZ/ceBmC+Ezdg/7mAWM7x8z0lUK0IPYdZlb2h+BZTVte7NycyyiFYEL1tiBxuh2JqKBPAmcVewsLHAR6LWEADavGNb3s0raQamrlJueCAyNNFe6MeIDrJkUVoZzLLvYafJ9IWrODn8TSKQzyPGJjmFne7Lf0GPY2oZmlPCFQreKeEZMZ9n4TqbUFvy2bEp+p6NjgB/d3BCKUemzAoX/IHLKsdHJLDXU+G/N7nPToHPEODNcV1eKjNMIO1A9SdoyWEba2Mh5hq2Y3eY9KOguqN0eeDIB64GkQEZM7NG66XvZTBMzxn9BQ01DJ6dweACxn2PJexjAGcYL3n6oDveWrL9K0F29VhVkzkhKu/C9UHGM9ops49hRHAlVAdFcrAXE0NJBJJ4NsS52bFDyBqMfHvEjrC0USYS1KcY9xvBvAyqB7G8S2UYNLzLESuJbZ/uKcwuJaBf8PSv/MQZAimN3n8F07A3rTma7nQM113ByhV2cSdjItJZLhoi/yAodH/hLhxs/jzJHdwgtroS5QyPpQsqBnDJVQZmxLSTafuT2zCsQw4rSSagaOP8LrA0Uoowvmwp8SpVawDdIUv9dye6tEh/4ckWrcFnYYbvNDFPD4r3woOyoMZ87JI3y0MFsUw6bjiHenCSZShDvvw+6CH9Vmqn7MAnenBq9AGBMTjGfGRjHXAA01mF0TGk+ClxEQPWh5jJtQC3iWvecSfkxxeiaWEZAQXOI0B+SnOsaYHRUwNPEJIV0c9PpwiXPDYSdAr5hmuo54+jBvVzaptLoZm5NdQ90ynMeB1kXuGwak5n4xwL1R/wkKeUV5QGWpPbLMvZOi2Zwp61l9q5hkmzeLM9zPucAEgp3i8wV1h+YxnQSxn54lRed5DkCLLPUYc9O4PWVPX5oYvcN0JTDOZ3nyeseepHmWzrLXIqWUzKBVC9gsb57ZiKr3DNhL5AJYoTOW1ozxHGWzHl9xYi/yb42eLHAb10qNWK4cleS1grcRN1IebMmBvUKqXx5JVF7KO44fk0IvJWaazP+ucrHonnZ2ZhHcXuCMR9LGhkg7qzznMD3YWGSZmdHNwxMvExgU0YpvvCYWLOJcWGnBQT2/F7NCngwGWz/l8e6pWN0JJ2DIu/n6PhpmaCEH1DuLQQxlHuBviET7LIVrt84+9NED1DOJxC23uEenhhYxRX+qh0ZB1uRmq3ydCaS7OoLS4NXRCvg4Ri1MYJt7SK6JCNdRLEDkuqDhZRIg6xw1sKPy5E/C49OpaEGZj1N5dQ854wnVrSIx+yMnnQvbDnAEvZLmL0KxvFG/+opcHqF7IGo8jXRoSopcMXp7jLXbYGAeUQhDogLAJkhSwb860l23qb1iN9AWOO5vGeQqjho+5a2/GuxaS7pMdtWetCb3MF2GTDqW0ZvWfcuKLHETHQGnpL2fp7NmEeon3NZNGSui4nAyRicxWG4KZ7CVnIn2ockbSJ1hOaTjTJStpgsmMxt0RYh96NuMqh9N4X8HNPZr+wCDH1sD9NaFIsWy3ttVK8PIu1aNIcIt5XBAQgMeQh3nxYcg6m478EUu5fsxCl+vo1bXy87301qw8bDT19DaMyC1yVz0Q53yoBfXLjHs/CL7iHqLI9wjtzoPihxBzaDxpPJcBse/QuQHj6TWBdUnbWEcr3mc5181u8MQDM2OYgjqW5VnzWZL1oZeDibzKDbmRxvBBz9kF0V7KxOzj7L+F8Ynby4ctxqQHOHZWCwzhDaieSE91mnO2yNvByfFnnvTKJkNFob0HdS90WS0JEir+18fR+pFOLL3rRYYhP7hzKBfz01ONnpkOaaM93eiFctrlgIVHMZ9Z51NYBrDWudugV2kOE51wIm/6SKZXVQd5UaTIGawREaqEOxzWGUwzmxACRLd5Kk28iHIkRPZitufqSI39ba07Gm60iv/QjGu3drSgegvgePcYXtvNU1IW6BfZHarnumiHuT7H1zauQy3Ppyw2DwhmudffhcLzoVQr/an7WxmjuJqFLzFzXMyAUyeRxw94zcKtv2CZwZY05LOYW6xZ+xsJnezaBnG2YdsXWadcgOB6qP42xCnceP3Jq0otmOPQy+97M3p+jsclfFgZ5onegLs39Qx7aB2su1jEZEK5uJeIfLjXmoS+7vR5uWdq4VD5K+vvrnAYGVTI30bkDZD0cKBzg1VH8YsNn4SdJXG45McllkLwHNQx7KPUvfdBdQfWu32qYrzi3maMmVZn6ZxhuNaLYdDdoHgZ0GNCjNyqUrEnxOPT5gS9Sg904QavLZ2nrEbwv9OBzne9pMpq5+CFNZ/gkYjzvBwL+As59ZOOSkyvFolMSlcSLzq6iNLnyvvq3ckJMemFEDuC4Ry9i5+DKfHXHX6YqJQM6L59hLDFhhlD9AAChudWuci6UfKMRq9w/MJEVnZl9WknREZD9Y/01NycASw7qHBY0ov1L/Nl95kuF/mGV5EGPb47o3QJgy3iibELaHSrt/LseiVd/oHGMN1aQ1xDfuknoNSRSI4Vny8WIVfAyUeyRmQbZsXXEga+QQmYQW7diacIxjEU28jq0vfoic7l8Ym8e6DqBeyDPVZigawQtl2y3pnXIPC28XV0eTOrfqpDM3PLwymqAayfG8f482YMc5YWGEKkrxGC7cnauF5+ID8Qvj8LJysdsHBEYyY36QXfCDsGHXKODcxtrl8vZ6ov/FPp6LgtZM3G+XSdK8cvEskPDD1DLP4csfVeHgsJhjPHwP3nQnbckcu+NGgTIkO6GV+To1iIIaLHPCxbjaOrqYqP2DYeR2ftfvn1ROx35bGIvuEwvNfqvewcHBySsUz2LqQ0zEvNbZQXoKs28szKB1Ql48nxwzyNZSVlIQr4Oo85v5G5zqw14J+do7ufwIwNOOB+pONrOxlgR4hDFiTdZhOL/5o/K3EUT2K9UvP19KBtzCPKPW1bh5+IcG4+uUjkVECdrYWZkkf8kBGS7Pp6Nruyn43W/hE/jBKpIe0OHllCYJrHidV/8mF9Tkun12CEbMpiv7YhTs7fqW0IR/dltc80ft7VIVMtj/5ntVD3/IojjQ1vrawBGc+av3rWzE2nhPzDWjmhs3faAuPmXd0O+GF5S/18y4P3gQsPY6nuCdEzk5lusoCS/fpLg5+qLZ1AHQ14JO33zHjUMcJnYdCvED9fxedOZHntlQzq71M84xIqWH9WPAuIomQc4jFxd2DQj2cRRxAG3sW+NuffceHXFDxVNtiPdIT3dzNbNIQ99+EvL9xK5oNvqOrNfoQj/MrNpqjSNoSjuxhsedoHUj0iOBl+zZK7p7FQ8HzeP9hd2hBQusaDNgEHb+GV9WFDf+6i7m65S8t0ZlMm85C7VYvuzDMkY3gmpplzeI0x7WNZtfQBYLUYZQLWyuMeLVCXjHY/oBnGnuCZbivECYeN6nxDQqWq0vHZ0UMBVuFqiYnAgJMAncgK1cmEiScGRtPlrOtu2nBClwoJk5fQ47Ik501BhWgblaxVDB3oaadQCns0JzsgHGqXJyEeVevDkq21nODmPC31GBOrg8mJz3gW3Y5ZhLIDZYnAGtaALGJW5mE/O2hF6MA5EEwqc3BCDd4O4dSBS0gd+yjwYNCp3NQdWUjZ4fDP8HXI7qzk+cS3OQYCM1jBvaumc0kjy3lewx9h+bIX3aRyhUmrbgxLN+a8di1sipXlbkfMamT4LCD3MSc4kPXM93vwXPUHzkUhhvEa3y/lxln8+Uc8fvEOzwWOJI6+1o86B4ydHMNo8gPwwYNcxtjIWBLljeK57ZKhe9ArnWyMEPT/d562GuqZcZGn/BmRqzhGL2LsOiYY+nqmPlybzgTyYNbo5Si9uzM2M8YTD7ZGYH5VcpY5LCWXNw3QBzB1304xYwW959yWRdw0MIqADWAwx1zgDta29Wb9BFhV2p8BpHbq6cbSr3kh+UGqBurWBi58SVAJGpKz4VxMexXnYiBjy0mfOdb1NbO2ui/jKMKg0wqqkv50cpbR7e/N+SVH6PpRClo9sxOkbxGPf1TSkw5Lnta5PNhdTuxVjCM0EEY1hZIpJ1pd8ZRUOJHVQJFv5g+U2LUGXm/mdVCUmzl+A2v3VnuReDhX3srvu3zBpYnn+ZNtq7yQMhCvoYKFwuHQJs6/nqmtMEY4ry6UlqRaq6k4z4RZtNh3J1VYA/tb65wdThusZE1IDqiYR47JifaCVweF2HBbxWT/v/W01bPc4vQC00Rjy7i4ms9fLaOQKH9NIjlV4gLpvpChrqrFFLLGjueQDgKlr8X9VLs/PU+fT3reKF9fui9N9cFDSjkmKysHWV9QKGvy8UgxAbt9LrXYCntR9nBlH2l7Eo+Z5XV2F0BLu/dZ/UjGurMYtLShDiu7x9Exp2aFDbvLOKQXEF+P+5LURCukJJ502UDpBWVL44YQAxkcXvEduVtTz8aptTLJLm+F0qQ11Ql3Ly06xUlX+77ajkeUylIBaVGM+0wv3P9mXUcpYdAtE0S5yPS8q0lyd/OPiV3xfeivEPXC71I7WG2XJeO7bsOiGbo6U7d1o6OzWlo6KuYpKa7LmJdWIXbWfCuSwlXWU+GwVONCpHa3nT9EW5fycdKdV+MmRJLiv+KT0sfx/Cs4LcOwdRf6zFITIiVO7qQOyOei+aaTG92UM3Rq+YZlrT81t1ym6Matqwtoa8eIrTbHtltvEQjemaovSRMhTYCOTqC9HcjlwuLy+Wz9m+W+Ju9zfC55rWsL80irjnRLX29dB9TlgYY6oGVd9EwkFdWQSTKfQi7Mp5pOznguUh0Zu2cLqcvjki9MxamHTEBeBNc/+SIu+vlv0dbWAeQk0u9VRL6zE4M23QRXTp+G7bcejlxOfLRbn3gBl934QIno6U2LibO2FV866eM45dC9UV+X9xHfmbsQ51xzJxYuWBoIVxT/FFEQcVpHJz579P44f9phPo/rH34GP779MQpNBoRNfzaG23IobrnwVNz90kxcft3dQH1d5byTeUTrCqhDUxyU3NDejk9M2g1f/9RBWNa0GktWNuOCo/fH1AM/Fjg00dUiyFB+5KB2TD9iEk7YbzwG1BUgbe3o3aVoNUmJkUMabRQnry5VY4ZuignbbIEBhQL6iOC4fXfF6UdO8sVn2hKkOHxdGybvMRbXnf1p9KkvIK+KH512DI4/eC+gNcNXy4KaCjQ2FLDfdiOx3RZDsnV6bPgjiS1U3Uk+cMB24cexjv3+L9CZz+Gtq76BCduPxK8feqZyckhzZCDUZgNC+Pbky27Eq399F7nGXmgxFZTPpbgnJbrRtU6qq1MuuwlLV6/Gm1d/E3369wFy+W6MUISa2jux386jUZfP4dQf34IFy5ow4+cX4og9dsRv7v0D0Lu+BNEqIGYJLHR1Kda1tWOdSXS6OgpZcy9DHdWhWfLVqrWt6KAhbCgUSvdISrdlcEGi0Ztb1mHN6pags+2+2Bgl3JsW49R8mltasWpNa+kryfgHEdLrsfemsvJ5rqUFTWtbihmyMG4WIolarA5iAa5gzgzjWQyoZBmfZH3826uugA+aVuPi3zyKP8+cE4iUXlz8UIaRKOQkMoZV3PPidxnXLKKUz6FQyJdfS29wFWyv7LOQz/sr3J74DJVjZU0jqLnU51yG35eaR6H4ZcVCywlhxqN1eRO+fdWdweo21EcDpz0slMQQWZnmkkhVGJ6yW2JOD9cEVVRDNVhXrZVxnpY/H1dKZdmf4scMxycLpZS54Glgj4ydtc+NDeVELjo5kWFML56t1QyXwbKOyvBKVWOWLJTXW9va0NLWXpqmZCywO7jKebSsi0pEtFIXl67FTBDZkuKNKSatAnHLHZa0+KXFKVM84/uqRdPC3113GYP6TfqiubUNs9+eS3iISq5Ic5XBef7dbZfRrqNzuRxymrGp1XRmRIPddxqN4atWI5/LFfvtVs8C5ZxdpG/KB+lGIxTKREZSC08DCFThvArClg+aLObWs0LR/XNvz8XeZ1wM9OldHeyXja9u7a3dPP344nRen/lu+Zyy0Ec0p86uYJZ/+cXSz3d0JM5XNTtVnE8kPaji7sefU/2U6+jiA6moFaJdzOL+uGVwVHLrT+55CvOXrsB7S1YEoF/FQlc2cRth7coHnsac+YsxY/5iPP7cjJQak0pDFbU8J3L5PU9hbWsbvnn8ocjnUpuUXl+FVFQxht0a9vTv3qV1TIQDA/GLvWTsYkp8owGTH7a99qE/4a3XZgF9epUTKJ5c1qLNmPDaDY8+i5efnwH07Q3U1VWHWelmCI/o4OoH/4QVTWvwb8cd4uqjjFPjvio2X/kPYUT3mT9g0mYufS4FV6M+c5kLzWwSOjQvqiMC6xHtM8Unao1GXDOmaW6On6ky0eT+3vWFUh/SjWRlqRG2xoY6NPaqj+7NgHFlNiiOwUQ3dnZhh9EjcNDEndHYu1eIC6UlgfPKVRXZomHhXLq6UOjXiBOP2h877DSq1GnSWfFVBVvHi0obrYoxM7ipwihlGL6KsaqEbbM0lKQlOHk+lnKUrmtw68+ZejAeuviLGDFkoHufZbQo4+i40zTwj/pt6+jE0CEDcevXTsKXD9sb6OoMHB5DwVi/a4x92WUXv7NNWp+ur9pSgf9qhKsgZNUPnG+GkUvrfClxv3Idpo7q8nkCqCoMW5ZhyfSMtGiE1ppRo4XuSgJCRcSTDuJHeFyp1yy378TvKt2TeFRZxK62EVlGKzZQ1bi8jAapjYp1RxnKqMJ4Qg7t6nIkY6+u9PgVxjCtE1NezhvzwgGpn5/7GdRz0JfmLghOh8U+0gtOA38RrFwbYhNXTD8ei5pXo5DP4cHnZ+Dm+/5YiuumYVQZgbToMudi7B07C2lvMyORW2DYwPqw/wrkxspMd4xgyr1Vu6O9owvH7TkOA356Pg4Zty3aO7s4r2p+RNFhqfQyvdXV4a4nX8THd98OJ+y/h3912zOv4q4nXqjMtCSLT3NTQz1+8bvnsPfOo7HPtsM9VmEIYta8xUH1xN5dcZKRCvJrOSxuWo33l67E2nXtlYSNxy4SCyhTYyJYtmoN5i5dgZa2DleFsxYtw4IVqypjFVnGmEO0dnTizQ8WYeTgAThm9+19Pm/OW4h1hj4S6ZbIVhUfnTL96/6v/2R4Yz5QRydydQVMHLuN66E/vzUXneZGF/LZ6iJLDXR2QRobMGbIQB/fINWCVWvQtLK5cmFZHlqXYuAmfdC/b6OHN9uKLnjquSwDmnzf1YVN+jViQN9GfLi8CV2diuGDN0FLaxuWrlwdvNRqz8YwM5/H5oP6o76QdyfKmKatswOLVjSj04jtEA+xJDyFR688MCNMmtpF67CjE8++xB+hNVhVEd5cj8NRyENb2vDOu/z5OA3fIb2RAa4AAAFYSURBVI7CZTkIyft8DiuaVmPF8lWAhWhz3YxbDWLmcmhqWoOmFc2hDxHM+2BJ6CtmmvXYgq7OTsy3rE56zHwukoxKOhQyxSQ9WZtMjDuzHItqhE/+Wh+OfbvJscUOT/p9kitMG8y0g1RtLdywYngXTDTHEtydTxHr7dg2Zd2TQdPyA5DVoFamYegGK8dgX6twe9WFVEEeZU5qldhCVr8V/cQZ91hdduMRpg38hkhxipalX3JMTzjj5qpcn7m45H9VJpIW0SxYljgnadwcDxKru2rzzUIT8aZpNwyGDCbIkrrKxZfr9uKDMZdUWFvJJphG3mB8b4VDkRFOrLaYCgOXcmfLXP0S3s+cWzxHpAhftt4qc0G82SlCZqlNRBuXkrpc9OOn1Tk7TbC0WCWwJnOSGSLWndqJn8ucQ7ygaHO6E+N4Dlk2JGvsIi2KA2fDyfQ6eSnqow8A/B+vj5DYnX0H2QAAAABJRU5ErkJggg==</t>
+  </si>
+  <si>
+    <t>OACNUDH</t>
+  </si>
+  <si>
+    <t>OMS/OPS</t>
+  </si>
+  <si>
+    <t>PMA</t>
+  </si>
+  <si>
+    <t>ONU_M</t>
+  </si>
+  <si>
     <t>UNODC</t>
-  </si>
-  <si>
-    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAFoAAABaCAYAAAA4qEECAAAdPUlEQVR4nO2dC7TN1fbH59nncByvo/I6XuVNhUhe1ZVUtyLJTUmiFJJCualLD0Vv1S0ukm7inxTKRXlcrzzKq0h5pCiS1+GgPI6Lc+5Y9/+Zjdlq7X324aTGuHeOscfe+7fX7/dba675+M451/rthMS+s+V3RqeJSF0RqS8itUWkqogUF5EiIpJEV7NF5LiI/Cgi6SLylYh8JiKfiMgqEdn7extUUhxtTgWVFZHWvM4TkXwisllEvhCR90XkOxjqGHuXiBQSkeEiUlJEyotIDRG5RUQeEpF/wezJvLb9Hgb4azHaMepoHO3+ICK9RKS5iOwXkRki8qKIfCoiO6Kc80cRKcgE+FRKRM4XkVYicr+IPCEi80TkJRH5MM5+VxeR9SJyLP7h5kyRPL7WtSLyZ9Q8Fl3KwGcwuJswEd1E5IMYTBba54vy207Ov1NEqolIO467SVkoIlfk0C9njiqKyBwRuVtE0nLPhjDlBaOdVnQSkeVIjhtoRpS2Z4nIBNo4c9AA6ZuOysdD2bxyIqdRM0WkjYhcICJfYkqmYWpClCUiUzFLQ7D7z+IjTopOltEXIimjReRsEblGRNZGaXs7HXdScrGIdMAGnwglcE6yiNTCZMSidSJyh4g0FJFEEVkhIn1jtB9P+xKYoCUicsnJMOpkUEdnERnGYB21FZGJgXaFReQVJOtBpD4eOgP0UY9JrCAixUTkTJj1PQjFTZwbxGBse3oc1+5AP1aijd9HaefG8yc+H+bzHO67MzfMyi2jm3IDp3rvmeNDReSeQPvyqKJzXjeABmJRcSbkeiTVSe4mJHIzTGzJJDj7flBEytD2bDR0jYhM4hWLGW7ixmDLrxORpYE2DtUsY3IF2Oh40IIxPR6v04yX0cnYrWNIzhJmVVD/Bsy4perMvvPgjnH7YlzfDbYP8O4HJucfmBr/vCcY5L3e8aLgbmfzrxKRFJzgcPoQokQk+3ak9YNAm4YglxS+uzFdifbsimNs/6F4bHQBpON6PHF/w2TnwDoGmFxFRBYgDZfF6EgJnI5rVwlzVFNE7gOVhM7Lz8snN0GLsL2tYE5P7LGDjKUD5xw3Y3qfifZpGWNUas6rHe8T4VFMiofRw1CVASKSChRTuhP7VtYcc45plohkImXRoJ6akgaYi8sZbE6qmMUrFl2AMxOCm94wrH2Uc4oAKd8Cp1tqDVrpao71x+kvgdkDc+hPjox26nQbM/8ODk8xrJOW10XkOQPN8qH2O4jwNiOZqeaaThpHishrnNtIRObm1FEoxbwKxmj3TgBVOH8xlvummOPOFN6M432c/tc2vx8FVb0qIl04dhFOeDLf3USeG6vjsWy0w8eLkbj1qLSzT01QJYeH38Z+q8oNY3LOEZHdHHuDTvwBm/gBJuMGbHA0SuTezbCTlUAdZ+AkMzAtm3Bk83m3EekrniRuQSh2cf+76e8lJlR/He06l+unIDCzQSgtGPv9mMdPOM/Z+kEisieE86OF4NUY1Hl8XwEiKAEG/grg34LvAobuDrbeba7lOjcKSUkhX9Ewht0uS4R4A/fbgNprkNORyR2BlNbEOd0L8yfym2POX4CX5Zjo8kx8cczWNwiO7W9XxjsaAXL+5ykReQG0dStjbg9q2cPkN0Nj3PWmxMPoyuQLDhunsxrGX80krCLKewsHVJSOuQ59FLjmvTA2AvNCTE7F9nWGSX9lMrd67S7C7s70jpcBbXTj5Qb9KGbBOe+vReR0GPU5k5UVyMkcRcq/pO1oJu4WzMsy+vkIQrMKO10RrbgX+/21vWjIRj/O4KyDW8aJXTAfjskbDcQaiNd/NHA9d4/J2OHhMC/Va3M1k3kFPuF8BuczWfADIQHZhv1tgMNuAvRsBf69DdMh4O69pGLfDeROvsbu/g3BOIwEb2WCBnOvJEyKGJ+xDen/BRMsNQIBrEYd9MRPUblHOLYbuLcTDXCOsUeUjN0z2OwbSXFugOmKRgYw2FEMfGrgGpaOxpEZnAnDR4HHB6HOc1F1IWBJJME1KHCNITD8Wb6vx0QpJm8D7F0KUoowYWswo3ViMboPjQ+Y31zCp5/BkluRQI3yHjM21KdLyOa1NommjkjaJCSmO9cbGAPaJaCaTYkAq3HtyjGQk3NIfxeRb4F6n8Pc87jfStO2L+rvUw/MR02OryEu0BRtC2z6evp4DFgr+KYgo9M4MRNmH6az+QxUWk6bdXwvj6T2D3QyGS14GrxpqRNBzV2odjR45/Dwy6CTeXxuhGl5ifNWM2GNA+dvob9bQBFbEJTpOEdNI0wDvvmQcRH3fdzrU3vGJYzf8emIiBwyZvFKa5IsoxuACpJxHnuAQs1o9xp2r7mx312x1XMCg+zNjZxp8KkP93kbe+fb7HNQ9fdwwgNwgvWYvPE4psZoWwrXmm6QktJt9P8yNEvN3wGSSx2x6ZEoGb2HybOfxffCxAF/wUEeQcMOIJzlaVfVnPMzRtfjPQkPvhlmlOeid4AdOwPvNA89PIAbHQp5ALPhOmKpIcy9gzD2W89m90SKtiC9HbHhWwmcErCtWfiPKfSpAd7+A5x0EhrQAlMxB7v6ENIsSOBYmHQfr9O9/i4GgSgen8aEuQn/PyT3KAjtuBHCJLD/LxhdwXwuRycEiXka6PYkCCIL6S4VJTXahdLU297xJLDn35A+QSrWwMwXKW21JZgIoY4Ek4+2tANNuZc+L8HENCVA0bFmEcj4+RJ3/+3YZZ+GIf35gKZjEYApwNlWCFSyARHKx18wOtVrkEYE9BSY9kGM/VjaXEdU5OdyI+RAXmKGLXWjIw94xzsiCb0ZUKz6XrZ33cLmc0tSm3thss1PZ6E9aqpCad0X0DQfPk4G5qkfGEIfriEiXcEkp4Hxf9E3y2j7uRJRWDcY3Yvj7wLPBJs3I9DZRtxwvHc8GbV9hDyypRuMmjmJH8dk/EF+SYm8BKY8xefGONgq+JdeqPsd5gqZSF8BNMZ3fhPwCf59t8NMTTWsxmwImj0X6d7hMfonFKXMTUDVlcqCD9siyQJzNCApBdyaF2BEW9TWL7C2QV3f8I4Xx+NrpaYKzulppKU+Kc6HkfTO/P4BfVvOeYUwbT1J1HfCuT3L8aIwrAP+p4ypnihlcI+2gXHNQLiUHsIkCX18FVtvzVo6fUmI4ISqMEtK6j1fNMf6G7BeEwewJtCh5iarZckl198MSPMgrvtJ4JwEqjfzsLUfgNvzE25Xxt6/DvM1K5eGc7+UY3+hTXGg6WU48S6Be04Go/t+YB5ap3ntrZ62XI/T/cEcWwNqKxmhElLdk849OBRVrVnYJaUaSIdf7S7NBC32jp/BwN/yjvfCPLUDm4byzA15f4yB7vNsaGGCis6Bc1uZpHwbgqJ5HDuA2pf0zlnCRJX3jq8B7p7N9xQ07knTpofxHzsxsy7lWjvCzaoTFKiXL8rsCOpxB1Kgs1wd9fOpOt73K+/4BTgxW/W+B7XeRBbtghhRXg1SklcTlQ0imMgtdcGWt2Rys8xEKm1kEmp6x/fDH2V0fq7X3whpHWOjZ6P1LiaoEwH412UmNFJKM4tHupOlamXwcrkoi1wqc/yAd7wKTkavfyE2PsPAw5BdVMqCwW2xe4OQ0F0xzglRImOohL9ZGogoj8DQqoHzvzVrQn4Eo1fEH+xFOzQeGMW7S2BViMDQJhwcy6CqgRnfBmn0QcqVTjdmowSME0yHX3l2Tu5qpLU5an4WwcEuOtY14OmPGru9CidmQ/l0zE3IT8SiY9jnd9CwKoG235vKt6VtBhtnIZxPgdD+DM9qEDh9yGfH34KacaqILVnO4KphC3tz4ftMfkNQj90wfCHBx3VImW9S3LGrzPfXTdknjYnUzKDNyk1HYpaRjfMLwEK0lxk4HovGI5lH6esZgbbpgbSA4JfsqqUV5Doak8BahP2fiuZofTUhydT7umA3J2AvX8QMTMQpfmlucJAcwnXYZWVgKnmSScaxaWhv6RZC5qIggvuYcBvKN0VaZqABl3kLG4uQ7Dknl4yuysQmcu6ZBhMLfqghY57knVvTWxL8Oe8vwzPnsP8JOkpECx1lJpnI6Saw6lTw6RBKNn+CAZvMDY6TZrTgXCWgEq8fafNTYsVQOhN4HoxM5x4j0aybmeQhfL6cQq6lBNBNYSY8JJkhaoK2ZCAUxQwWV6oMslnA9yz6l99b+LiW3+oTDY+gTyvwaRqE7UrCywod7Y4UDWPmNCG+G3VTOgxSSDM1M5+KRInsBPM0nLzENM8sTcCZXoFktces+Ov0fmCyJuLAbvUmPhplM7bJOK/swDK18+iDfzzFW26xAcdZAec6DoHINNH0f9pFvEClG+o8BNVWRq3x6nw7kdQNJt8bzwpPJcXnewjZfZpCWnQZzmpUzKv9f7uQDQ+RBkG1iQ5D6KmMV7BVKu5F0IeNwy4NDP4HAqK8c853VQSPrg7lTCRpF5Gckh+AbKTtdCDSXaHKbwzSYGA50ZtP67jeEyaL6FMaWvE0WDbepbVf0X4OKh9CLeX84ipUMrCIcr75rAt02pmYw/Hq6wied4NpfD2Nmplj/uKPtaZAm4CTujNKyjREGqZOAPIVDjTqR653mJeTUZhZlXv28KQsFu0kif8ktrlKQIiKk8v5MnCd8p4JLcD5mjyqigDanIhDTEcjJhhQ0kqGGv3N5CKqmTbrGXCaMRk7sFPxDFoLpIvQno7e76mU+ccw4UuAiMVNYl7X/xXG48dDFqY2Y8L9Fa614InP6AjOzWpAa4RNzW9+mFzJtPnPOpIIs/qqqYSkEWBoPmEB6tLBnPwtXvtC+TmtxbnlRFXoeDb5h0dMRJVKSLuOiKsxNvh1vPlr9GkEjNoQY4eBpR1ebbIzMMzfaXA5jvdH73gapkMZXRhEtM+ki4/h2zS/MpmceJsIs/KNydRFiNk1OTKDGW5ppNyB/Y9N5biB6ZC/sCVEjc36tkng0aGgl9l0TjNj+8gdn4svENCFMqhjFMdlaR+T0YJjVfANIwJtW0cRlvqMWyX9XOCv4u1sGK05kv0EfC7lfGWElGBdCqBagi/DRQ8z8DIwxgYH0+hsftRZNWBmHPv8Mrw27VH/T4k07wicsxsTl8nk34iHrxzYWmGjxX/htEuaIOpRSlCfeufVxff4gYoAEj4zkl4H7avKdb5BOLUk2AOz6+qsRSPMwtOYDlWFanRqDTa0DpHO2ebGM1D3i0ijqgbsisN8RLyU6CGizQoxdmRF6HQVnGIRmDzEBEs7cKAbzXn5wb5FSGq1wQz2CdyjBxPgpxEiXNeO6xzv/QvudSaR4pu0cddcHcH+6VKsdXSiGJ3X1Z71ebepw11ApK4mclIaijbYRSqWipn8cSo2dwn36QpDynnnZINAPkYD3iPKs1XrLAaWaRx8Ntr5d4ToRT77hYZS3noNS/UQAlvQqMi7msBtTOYcArGCOHOn6QsjJswcis15n9lONOigLu9+OD0MuFTCO74M2PMFJml7oPM3k92ayYTcw+AbMUlLiFI1XZnNBO3W8hDefoHJB5dGAFqTgRuLw7wV6DkGhmkRI8Vk7wagwaF1zLcTL1hsreaqFu8FMIkdmPDRTJA7tiAJT/4NMzQRFXkJ+6tBgMKVNAao0juLEPQeszBF6UEY7sJZXUZgV/xUhZmveWq8G8lqxvG59G8Fk5OKmXuDMLkdpmc0eZqDpHebEJwUYv3f6UjZVsOwmgjL3WhS0wCTi5IEs2WvfCbtcJY5djvm61WTX3eatyeCmr3OwZLYoVpAqx1m5ZJwcZtPyCIf0gdps/QJN3SD/gEY5+cOUgNFAqV5IJ1GoIPTsYHJvHfHZn/KpI402T7Nr1dFdcuZsP9dc8+LcMLTmahQ1eZO+v8u30+jLxpkFWEyXsG0/N04c+eInxcTcQ03Cfsy3LgUklDQlPcLwWxb/nmTCXk40Mk+dESXsfY2MHIMZuoRvLy/QkgpCWEoYvCpLZxeRjLnIy+oikbppk5YAh4ciuIci1DtfgotKo0zTfC2ZxwDLY3E1yn9VQMkZfRuoialspiFVByI5hsUv9Y3axyOoXr3Bbb+HiSF2QvPX5Bzh6IxLU0UuopBWGpCRyfxW2j3UyFv0DnRAJOX2YwZvDnK4vj+wLmRfH8eXiUaDcmAP30987KS/LSIVwwdh71SqgBOTTbFVsXMi2irAcx0Oj8m0Fm1rX812NWuElqJE34Fe/0hkWkCwUhumBgPJTK2TqQ074piMmqwiKcH0twOYVmAtquWL2ZV1BPm3HRw/k8JMb/qfA+1NKW62GDric8ETRRDMpW64VxCS3ingrPrmDV3lo7T0XqE8W9wj1CB9GRpI8wZjT0NRYcJmMT3Td76ZZzyXm8pwmokXgO2DJaK7bH89ZeE1WEmRpvjvVBZVa2KMOZT1FnD2h2ghUFe5s/Z9I+p1fVAS0KRnzCQ7oS3w01FOi9Js2uTyWtUD1x7EJOs/eyPPdc8R2Xe14POtFy3mX2Ka0EdP8UWdiFKFiqQikHfhI1JAt4sp2M1zE0uRBJnERRMxXFMhVm7ydcuMT4gg0T+BQD7UL55J9oylP5UY4JLsk4vH4txdpFTmJQLE5PJhI+jXjkfwdBVWH8yKdod+CsNrjTi1G0T+8yysllMzHf0bXw0RguQ6j2CkIHY16EwV/PAGoar3a6Dqij86UcQMJtAxdncu809xuPgxmCfe0cxJ0r7mWSt65XGEb1s2lzHBNwS46EpSn1hsiAU2Yy7IbZ3AnBRk2M3GyhnxyxAzwNowDMcG4LD/1nq17fRGxnQh2Dp6WbTTRnD6CTvuRzdvOvcjBm4yHMSSp9x3QnM/rQoWyNClGwWRCrNRDqjYXKlBThcS7r2ezavoYZpid625tVIuC6XmME4nkHzxiBU/fwNTaElWA8CmRbCwD3Alpaol2LJpaaycLG3kP0oVeD3aXd24D5HwKi6uXM6atwxh4p2tCfQlMnhsRFTqB6FnnSzFJv8NqtRlTe1TIh9gCDsbsxPN4oR67AAS9CoyQjQzyjE6HTC0VQ88nyzpqI2qzcfhDlanUjBppU3JuYwWFsTRtdEYcCX5Aca4mAfA3HMAl5dwiSGKtwFuWdTnJIWALabyViJWbk2ykNTOiJUz5ntE1plusrwaCGaVI60wkhw/jSYW4OCSPfQIGPtBX8CFVCayWr52dxgM9hysPn9Nmxnf68OqQvQX+A91vOTkhmoht8VOHaEUFijOV1Olsz1toCHp2Ca6sCUSYF9NIJwPIdk3mcSTZ3JWVyGCdUyWVsQ03Fgbz98g0apewELoeXHOT4YZUTA/s6huDnX2/qbycB0U1FrLxC4HNyagfotjHVjQ0VhdllMSicc3ijM2jaYHG+BVtCAYWhJJ7OVoy/2tg1Vny+Z1KVMei0YfKOXBtjDOQui3C/Hx0jcGdhu2xxmT0O6enO8AJPyHLZ7Ouqq9E+kbCnSPzbKAkOffsCUzAQtrEBix3Hs81wwuTLB0Eyi1LqGyU/A5PUgr57wZx8w9GH63s5j8lry+VGZLHE+GKUPztAvT7Vg0PlMdKU2bhCQaIJX1M2gzRUEDitBAXUlfor2BJpYVIsQ/zOc3hXemAYbM/m0KbweJnB6lBSvj9VfAwj4JbFfULyPYxuFXfa3TBQxcGkKzLsbiLSRSXAS5G9hWMRKnhsJRBYiEd0ClZUTpdIk/OfgjGsx6U086XvBZO420N+HMYu6N9F/Ks0igpx7va0UUSneh1flw0YtZQZ74bBOM222YEqOEdbW9daL9PS2Z1iqhyNthU3eQBCxCDu53WDkJ0Ebvc35hWBsVaLVS8m7HMaEjQpskxby4z3N92ZIub/W4xjO/2Ny93Ppc338To5PCsvN49jq4Z0fI0IqinQ0BsDXAMsWw25eTHRpM3UPmKcFhCg/MO9qGFYFph7B7GTAzAjqWoj7FUetM0kdfMyajcVRQvwIk36XOfYo0jybQOUL7O8KTJyG3wUYx6Ugkbh2HeT2uXfXUzWZTOJpsTebWoNrjCeeBNyzzH6DjsbzgL5ClIrOwqQUZzKSgHUHwcZbwbDfxOEYa1B8uJLvGcDREQjTUbPuWakCMO+P5DYyQS6h9XlBOpEnObaGgRFU+item0nC7OKVhbo7RlyJaaiDufkOOz7ePKzk16R8BFudeBUFXSwlAbYVc1eCySyLKTqDY6WMA16OJIc2S+UpowWGjfRWKIXoOMzeyCRkMQhFGdnAvneZPF1xVAwJLoFUH+X8TWYBS2EcaTmi2GNI504Ytx8Gd4C5tvCagWkoyjVC2yh8OkKFZeAJbOc4qWeTFiDc7BllVX8sykA954E49iLpTYwj042TRzELB2GI4uam2NIk7Liu3ctiUtbhtBajQeUJ5y8Ggfj7C6PRARDVc3E88jMq5cWj54uBFloi4aVNdi0bBu0ASaxi4B8RCCSTh+gMirFp268Z3Nvc437yyPuYmIpcpx/vtXHW/kMEDxE6v2SeP1qYfEV9HLnmugsxUXsxh3N5bZKTpLx6xn8B1PRHVLkU3zMxBzu9tGFlMHOHKA/Dfplw+AgBzkDs5WNm28ctpDdL0X4Akn4t9j+Exz8mohwfZWGkv1StLt9jPZ8vLsorRhcDW6cwiDUeYxOxzRdQ4LwqypMYv8MUTcYP/A2YtxSGr/bal8Ju6uaiB8gJl2ZCrovS33TC8BmYmAzzvI2SoKZrwfHPBPav55ry8l8rkpGqnjjBTURNjslnwOjQyn6lN5DiXUzaM1zzecxDrIzfnUxKhELCXZiYjmQOcyryHkJyC3KN/WzQzGnvTNz0a/w9iKYQr4+jbRao41lsYX4GdwsoootXKI5Fl8LkkubhgEtAFh35fn4O19jOhL8cZb3gCdOv+T8sNVFdl9dVCKWO5luc4lRvV9MEnOKPYNV4FrVbqoXZqQRa6GqeqKD73i8mMClnHt2zBvTz0a/1Hy6n6g9vCvLKQk19HFoHhtSEQdfm4gm8PlUhhavLCPqSncvN9rw8p7z8e5BYdAgvnxEF7F8Ck3V51okyWYCFLQwkqyXhh12dUvq9/LPQS3j9lFzuV4xGG/ERV5Jf/k2lWU6h6fivp1NlOv7r6X+MPkX0P0afIsorZ3gVwcDKwL+yuSRPJQKTpYThCexv8akG2DudWqR1YuVIup9Hv9dRrV7nXaOltx8ymyLE8kAIrxThvObko9NZwBN6VPMJUV4xuh3R17gAo12xtjFh+VKYPpysne+J61IT3EItThmti8b93V8P0d4+aLtzjBzHBPpjy09nUgds5rXtRcDUOS/+EzGvGK3PygjV57SoqquFDpJ7nsqKoHGmrSai7D7s1iYMn89C+SNg5TbmAd+6P1D7MBepTEAb2vIqR7R6yPSjFswfQeWlDrn2P3LPRnHuN49KvwWO1uChAKvq03TnkkfZRJO6uUh3O2Wb7/2R5gHkrb8xl5hnVoUKWH0+2tWenEpPmLydXImukX6Lqs8AJiynP9jJkX5LZ6hF3cHmeUk2Q5eN3T8LaXogEHg8SZ4i2TwQUcnfWPSVeZ6I7pHRzUmDA/+ntYx2g+P5L6yc6Ldk9FqqJtmkJEcE0qi6V+TrKIn6bFOxjqecpmH5aUyO2vwcVxqdLOUVo9UcxAp1/XxDItJyA3a7mzETeh1dZlsuxl826Z7seNZXaJ3wANqjq4wqxTgnTyivGK1PJPD3GSaZjTX+2mR9svlE4OG2QMH0E8xGGW8fpNJNZlntLO83v1BQyOyNnG9y4cK1T/Pal6ckdm0O/8sVF+UVo3VN3sU4nbqsOHoTadlv/nBBJTvJfF6IM1ptfovAZN0UOZCFipeYTUpjaTfS1PV0/19tsPE1aMt8dh58a1DM82jCOawqbU+/b+N7DxYM2ceFnhDlZVKpH5JRGMYm8tk5EreI0DHdkcuouc+uCuKS/NajO5vpfnPS5Qasvzmn55jlrufSrO64k1AH0Rw8c5UYTb86W6//Uqcbh1xfnPN1wY2DlHbZgFvi4IIjtxpJtyu7a7v2DsW4ykxwcXncJCL/Bo/W4YcmAX+kAAAAAElFTkSuQmCC</t>
-  </si>
-  <si>
-    <t>UNFPA</t>
-  </si>
-  <si>
-    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAFoAAABaCAYAAAA4qEECAAAXtUlEQVR4nO17ebRkVXnv7/v2PqemO/btie6WTtPMDTIqoGAH0IcDz6VRRCVBIoJJHpqHL9HEleeUlUmeQ1BQCY9REIzSgTCE5wvwAtgKNDRDGAI0NA3NbXq8t+pW1Tln7+97a5+6Q93bdW/DioJ/1G+tve6tU2dP3/72Nxe66KKLLrrooosuuuiiiy666KKLLrrooosuuuiiiy666KKLLrrooosuuviNBO1aV8Cun5UXRhF/VhydCELRkD6sCf+g94j6L3vfOzZt3Y1flFH7PxVQQVsPFHBFwEEPQ2rOU5IjSCmjSO/SJl1UObz54uB7qtPG2PLDRag91gOOpfWAFXGlDoI/VcCfBLACil1ksUZJfjB/XjUp9qaAdCChBzAE4J3TH2+7vhfZLgsuANIEtAZE/YpmnaEZAyoFS3SYgt6uSkflcwLzAZQntgpgBxk8rx4PAlirKuuYtE7EKGqKuhbyBVB4mwBLggXNXWDX+twOKzVeRc6uEcZ+E196pSOV6IxszHym8UJ0CU3RFNkIgwORo6mH4uijAF8K0gqFQQhQR8eKpzPU8Yelbu6bmDP0Mj0e8aIUHLUopw6kKb6uxH8yubYwhsdvq/IHvefTstRs60xoAqUKm1P8VWEVKZ0G8EdE6aA9dVCHY0A4vbUmfhbQGxS4DsiJ/6pBmy5Y8BgUqzpOohD1dDiUHs0fCBANedihqU1pQoekw2YdFPHMU1QFONYN0RJ/GDFqE5TWTMMGJk9dU/qE226vmNm/Ddcz46OtY5qBlFDYN8XQaSPTnk/j6ASQMawi8FdE+P35Wv9zEFa5TcBfIfgHWoewB46GYNVsGySAKdYzKdI/nXymAt05tWGX8EdUEVOHMcIzSWifbBu/g2K9deK57IygTZ5ajJXfJdOBiJPQU2NxiwEM7/aNI1RWNGbdAAhGm/x59fTnqtQ7x2G+FrAQvw/Qdyr4W6TytXFRMyvsniYm1jdzoY2Dm4xsdKqbMu3XichT/QFt6KHa1FsnOokI1Eyeesys++1hFRVHvA9BphNaCDxPER+cdewlGS3XJv9vSejkcaL/ikFBSP+ZEq8m6KcAPD47oefcXy5/q27UtK0+cOrUikkxNhehA9hRldsYVo0DrE5IAuc1GtsDFRSeaqo8/WFK6DlpDFze/TYQ0eF+1NzABit+9QTebbbjBHynwp9Oirs6SbiwXU+A6dQ9l7ENdyvruBZSgMqhTY2k3tzt0+hsos5XX5XUw9zlJ68AUOxLYONJzSZJ1d+TNe3Bsx2YAs/7SJ7OCaYTipJQLKco15vAvW0vMzC6s3Jkczi+hRiLf/1EboGgC73am3ZGvf/VFYr/DzM2Q9t+2PtXYxtLX+RoBqHCtezx9w8cVl9NNC5/goXxCiCbp45GlYpjzeKtzvGJMwkVDiouuIsKxey8do51DQt1Jr8O+VRKKzOlnwNYuNsONEzV+LjA/WhqbQCXgKEDMsSRnzL7CEi22WVbnx28Vy3tTTyX3P/1QEDbfLG02sR4vJ0ctv/l+l8kPZHzTXM+EXon9+dxsynrp8vHN6YL+f8A0AQQjX82aMordFp1tHQxgNPaJGFdge+VSumf9S0Ym0aM0eF+JC4KhwRtvf4sSN6rqhcT8FZMvqqblfUv5jeaP4rEtTEBMNzPeDFlUDIl/UjJRrt6rlLzxhAZuUug821a+xFR8nbNrfcWOSw5KCryZUrM1UR6pCoH5fSUEO4PhJi4qpNwM0bWvG03BX+6Or5APB/AJI5YH1Slp/MxBFOENsCYFFF1Pei3NVS4jkxipLDr1GTHG9YTJDXLQBix6tZmTK/kknlcbNSliHpkMFItAo+1EZMJEejLQnzi3BbMrxkEeM9v1kbh2zH8pybktZ3YABGeAfL2n9HOwaZ8YJJPZ8IA63auwpc3/TGq9QoWRcPYv7QBH+j7GQ6MXkbT+Cwycod3resSyC+saBLhipEP4yE+CCNj8/GVvX+AhaVX4HWcm3MzEoeLyBcwi654XWkdfDblswuV5LKo5IJIhJ2Tpp1MIp7xfE+HMvGuAR7ZdSD+xxN/jlHfCxLF9mQFHvYr8BM7gI/hRSzmGoqaIRMDNhJEAXam/biL+7C2sRoLC4xKAuwo9uG3ljwJL1NWSHN75YvJSCGaTSm/3giraPjCl1xm3h0+2aydahNaPYeCnAI7ZhAzhC3SNlGQhw3Q0WnLhwxjpMD66kE4/6kvouoqKJkEGRkU4FDhDI/IIC5rrMJQUoJvGGRFDxt7MCzSsQjDAy9ggMdQpgiEAh585igcVFyPxBfzOcTRoWjYD7xRcrkTcmetyaekYyF+RHfalyRCSSzUKAwLXEIQDxj2iHY44HszRlFMD+4Q4GIDsQaRdUglmLwMFoWSINrZALYDd4wdhy1uPga4uttwhhwq1ECZUXDWFCMjBUM+MTBZxFm9yE2ASvn7lh02jB4An8SI4IPFAhb7B54n1fNvDgKxo/g8Ib7TzskDOs697aCZnD87N09+51taNxyetosdBYP1LYvT/get8rKUlLSUZQw62Hk4Z9KnmQ0GaoNbXKO8PwaTlyOWbS9V34SfbTgFJ+91O5pSDAzyD8S6nEDvGx/5cYKem9stwOVBsqjQX+eHCj1KGRPBqxEVOj98T6wXQuk2UdxKuwvEiFj/UpW+o4qXJlbPpEUK4xGfBWjP5NssFwf/QhXEJH/EpPvM7RliXCZ3wmtRmCFo4gmFJPjbra7CfqGQ+3xW7VvfHxWqUSEb8ZmNEGWRhKuQ2V0wtIyLfkWlUVm/fazUowPNv1Wi7/soe+BHL38MldIIjhlci0Sj9UZpc5vHOqqge5Uo91wB3QzS64JvIIZ+StBghi7P4xOEy8fl+l+BsJaUrhPBNH9jXCT9MUN+LMovTHxJEBjIFQJ3o8DePO6Se9Mr38qq/AylHETDEUbcu3mCEBA6VoTOA+FzAE4FUHgNpAwwIvReAp1PwGcUeHs7oQeSBH2jjL4qoacaxs7+QNUMem4+1UgMvLOrYH3wYhK2PjGR38EGCxT+G6aUHLOgP9mENHq5VsC5LyxtLntmaYaf6DEhDg5tybJ2puHJiVv/20BMQx6xpJnx/vvjlzCcTe843cJ7xXAyCg3RvX0nWyu6GWRXmYKStvomMnq0Ue0RH0NV/i9Ur9HWofyHjtJG8gw7XxENZncrcAyr5or+UvVYK46/A+AbAP7ZE98joFWqE6Zy8OBm5dh9VOhO78wtAH0TigsBuoeUrxPiPg+Dlf1PYNuCEbw0r4nhoeQ9zugxPuP1huWFYq/f7orZFoHspcKBdg7sE2LZAMEPvKfVdfUelK1l1kEi+mSRFJv9Moz6PnDHQPXucFkRUjDgeXQ1EZJOsZ5wINbKvmzkETbyGBt5lFjXAfgtIPQJglf/CKr3O+K7o9jNI44gRLe2FI7eGw+5LOpzlGURshr/QokHbMnGF/qUdo9VEB2dsL1xmy0cTdBd+bNAdCII85RcJurzZNcA+uYOJ3D6SGEAzjQ/uty/iCW1VzDs58Gw7qdKDVNMnvZJIUHKfVmzOBwXmsvJ07vEcwyWE0h4ULy5jzzfUSwlTslvhNqXWXi/AjycRqhqBX2o7j71NCjygBRrUYVSJPISqawR8AdmkYB2nIPb0ezAYIc71bcAdDuBduU3w/O6ZFcBXPAnl4pjT3NVNqaINjI4PmfWgBDxymah/8x6cQB5Kw2gHvegwUU0TKs1bekMT/zmTgvO5xU6nfrkqIHFNQyaOtJGpQRwCE1tJR9vjSrpfqZQX1RgOcoyLqXIXcyEXQw+gxhfMNafFQxqIlquWUVFoq0CbSZJtO+22gC2pvNykTA3KOdUjtwq8fJe7wRRRb5BhJHdtVDubr1A0E8Q9Kzxv3/T5kGg/SaQ0NZxD3owfDb9/udqs8DJZzS22EMaiCFk1gbRMRcjgElOjm2G0CKboWAEBSIUCHmzoGP2pBdrtfLxzZECBiWFakUItFhZtjgVR063sNL+HKUnqLMXKfRWZRRAGjJ9iXjeQHG6LWPX8KpNgm5TMeUCqNwTMg7wcxo9M/ZjKabP2iGFY35ASW9SoNKBRcINvgrAlflfwvUzCL0RwH2AfslQtr6cJbAq7xDSLckOepwbJoThT4r63MHFRSniQX//HuPRKhS7ZMpEzbm/jQcUc9uvuSVIiL1VUH8Ca+qZb0RVJn+IpvEajfy5AM4iwhiMf79LbWyMnkrhmgMPquIyNOMdtphAjBQ0iRah1OzJvBn2TMg6R3hnW8yYJnxiupWPE+vWGphvG9GGN9OZmvM90V5thD1gcggN/gF9V1W/GxRnkywQySJSPsOI3Ab2LiN7EAvt7ZvRu8XrBY24udHuFjRqg+YBa3+f9TJpO2vE8BFPdvGe/j04OLMG/0OQJdF1khGSrUU0R8tke0bGiLjKheZ+0rS3sPV7I5KP+9QcT8BDTPq5PNShSA3hxEa5fktGfrTHlZar9UuMYnOvOCLOMD+uITaMVGbO2hFBn1sT82eKJV2LYX68oqPYUeqftmuF7gvQLyfFiuan6XLbLPBqUL+ieZhAVZaBzBUA5hHzzZRn5rxXRF8V57cltRrV+pKMxfO9s3kcpGhYkas4yLfgXQRudg5aTyH1JG+cNK8j1ZFZNhZ2vL4U+XuDyIkHG7AL657L2RpYt0yVT3JphITclwCcK8DjURQSEfo99bSRCPPVuJLx0YA0KwuV5GS2bj9y0dp62rulBw0sLOyElAoAc71tG3k2xjgXbF3b7lIRQaXB70m2x/NDwKoelXIFPwOBsCFkXBlvxaljCE0+Tqz/COA2Aj9IQicHZWnmZb/kAYEiCsHkr4D0u2yNlrQEO3hK7WOjd5SuU8HbpvEBBVloP9VMi89OTpIw+o/diQVHjbYva8Pok+5D1ft7roTB0jbGCDblekrN6VIvJSEC19i+Fxa7UKkQPVUrpvcm1i83leYHjUTXe3U3MalV0liha4hprYD2I+HrI+XBHuH/wuxWkpFn6nW5I8kynDu4BiXZBV5qUTL008YT8e+romysXBcXMqjTOEmjRQCea1tv8NoHLNwn1fqvN9m2xMF0Qk8EGnZz18bfPIoIH27nJoU+2txhnjc+eGS6LI8WkKFioWdHQWjElvdvbBq5o3IykZypoHcBWiLBA1zSK10Tz7k2U1OUof0MWjp98mi7+1cb+2NcZs4G4y1EmnJB/9XCX+WaphaWUZMSdjhG5sZCAjBJBZeTsX9LrAchlBKouVFEnzfiUmU2BH2IlNY6z4uJ/QfJ6OFq/UDU1G8WnL545sof43eW3I5qrbcgW5AseF/tznRjdCTVpeIcP1jnEJjC0UgplNdMy94GfnJkzmUxF5JoU2fzfmdHMvNUWOXfjIgKaDlA6ybMQ1H9R4ieZTXL2bhJpJdA6RJRhdEpmUttZ53/38E30FZC8CUovhbeYpZWFdJ4ksAg+MFFbB4oYExbAo+UNha8fJWUzgHpcvL8eybyj6pEwZipKfQdEKSRdUsVdKCobvPOXJbK2O1kGzi++DBcvQLLfKwh0p039/6bNvGUEsOEbIzyQt+Ivk0tHTQRsam1LXulkP8QiK6h1lWWNlu5hs6YMNinETpnaLI3UFFgC3KE22WGJuP8jBNtr1TmLjeYGambzQHrNMaMoBONHyCHaFs4MgLijJ60o4ULxualZxiWA4VwkrLew6Q3CeQoMnRmcGzI+H9PNy/6aXXrwEP9Bz6CQ6IXsIK3wCVBX+JZl2ItEV8D0buVOCMyhyOjc4ho3/G1hXKGswm6dNpqyX4x3OBxE7cP0N9uhdFoaYddGSUKJQVb0ZZuG99/Bpa3+SYdhMR8oD1WT9BFZU6G7JxGKCsobuPoPC3eocMcYwRzkEzrkBKJpi0//9dTqNX4FiuFOP8SMLY1tdAgSm4uCp5QYAORxhBONIvglXFczxMokMeYhvg0XlTR+5TxBRB9AS1Ha+YyjgBwaYeFHwzgH9oefGS8dUIwY/+m4zeKWD1d0IkWovqLao1etOmPLXyoPmpdgDzK4ozANoC+lTVUTto+NV7ISD8hwHdz42sSTSnAWwJxEBeEzAOx5zzYM2/vXTDGo4wRnPLCL3Hdlnei37YVTrYIL6lGaEi0acCM4rDCU3jOLcAr2dJniTyKaORXVQjotQ28demTkCLDTJRBePy9r+J3Zj/uNw4CuihFLFZeptyAaTentVVgCC4I7OCMbKwf94vaYnvSw8jLG8dd+TwQNZ7htrEDW0EJHl9deSlGXQU3Dp+AiByozrD1IhopcGTP03hTeTPeVbwXR5gnsUWG8NPmKdiYLsb6ZH/UXDlPax1hd2KJ24JkLAQpJ+tN7gbwc4Df9htFZcXjIL4pBP3tnLVKs4mECNP9wTmcs8lMugaXPcM3V16Itxz6BOrlAooZIcoISxduxAHrnse8eBT1pkW9WcIisxOfXXINkizCo6MH4hEchq1D83HY4C9g0wyuLV8YBKHC/DWIbv5NyRnmjlqsX5Vcceo0Mgfb7+jcOFc8BuTtNQ2cF0wqDqFgTinuB2ETzUjwFjnF76++BRho61sHhtcNYsyXkHo6ToEViUQ7Eh+tVaWRQ6LncPibnsmtmTQtwA9E6O1vzHBH01uSLfH1yWh8+hueO8ztPbmzMJj9ZEKn2Za+os8T5E8plHTn+o4zUdwA5Gmel6cN0qlqVDBPU/pfyHAGKCRRCL6JnRrxRc7ha+RywrfggWimNCKGeDrMN/nv1dPqPA8ZqiCr2EBW/2ei0bWJK07uwVQt3EgD3Gy0BPfEOrz/72B7LArBln3joI52FMj/IW2BtHJ3IVb59d6/a0jx8zOvXJDRUZ9/aPDo6glkMTZBZHmG4Z8wk4FCBUpVW7rdgU/oGO+w2SXUP/bpie+C/upbRojKU4fmEz5g5/ree+Awf6Yvlq9jgX7CLJCrpj13imKWwASrqC2Jn6l9a/XZ0h2hLOj1qrubti6BGzi8/v7ivOy2dtFLm/5ufjZbVam29hAia1digptUMFn02OLG3/PEV3Xck7biLwMLx1bZyD85oXF3bSojqUWTtXdkcTEX8YezLp50A8e6CqDmxMCSMcoHJRh63+5B/5239v5u7aHS1e2m6esBEUK5kn52/qEj38GMue1cpbvUyoGdaoxc2U48AU0xi9DqWfVPyzvi0VfKJxL0ycnHFSDudS0ZqzB+jFZPXLGOwyitiAvZ/mz0kUkuKQHyPNB8MkLxwOn10fGQ+yGZkIPGJRCUXyfOFkDPt7F8B1sUM3/psed4tFJ/6qfuM82oxyOgZ/YBxkOrRe1HceI3LwQfgvXj1yUPDFLUs4foPbmdtpdnvBTCB7U7GYWVo6C2atgQEjCxXkOxvOQa5loo9vo1E3s7inI21elG1XErbMZ8ew6nRPIwFT3yVhIY6xDpVGPI03P2D8TM+FGMherGVuMywQwBZp6ChzTTGE/PmV8VjHEFG9DDaG80SHB1i/S5DrmHoNQjvYtKeAex3vDq0zCvGT/z5E+C1Rvn6miV+BFS6ZBYbdXZ9wwkl5viFBUao0XUXQk8YUIpriVxf0KkxY5DkD7TYHfn5AMGysMh8GMnT92oXJ6RObljfwl5uOyfTH/95U6GfeDqdLt0ro1ocdczBv5DsPRB5034rckhr5mUnfE0Ef5Sha9GyFnu4SBtX1Y/s2qLN44XlEwtkOBI6XPZC5XHswmaCiEaSjG0pNqKeyB/74nmqPl0oxp9n2i3zPGwyeiscmrrk0MTYZ4bQUGm5KoQXTtcGTzOK/+3afI+ly66dujdY5+LV7hZ9/JqfBSKdI16/AuBPgJo+C3jcdhDGm4adLxiBvpAKG5VpWtDcvfVXhTbk9UfrtnCMQI6h4DAVUWK8CBn/gqouT8LQY2JH/mAUY7G0FOuTStyRFK6qlGz64lwzviPIzNWvcOxv8yo3RRlUxJK84z09KKrULNie/x51MTNktCZSrRPiHwixj8Z0attQetz/tbn1cjfFkWCl3OlQq8k8MEKOY6A1QAOBbCkg84KKm1Ygce4JPdQQveC9JHcE/VvgO3YRRdddNFFF1100UUXXXTRRRdddNFFF1100UUXXXTRRRdddNFFF1100cWvFgD+P9uuQwyBEy3mAAAAAElFTkSuQmCC</t>
-  </si>
-  <si>
-    <t>ONUM</t>
-  </si>
-  <si>
-    <t>OPS</t>
-  </si>
-  <si>
-    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAFoAAABaCAYAAAA4qEECAAAZHElEQVR4nM2dCXRUVdLH/2kSiGyRRRBZVJYBERAUFVBQkU0UBEFA3IDBBbdRh28QNxS3T3EURVAYBZQZVBTFDTfWQSKyiDKsolGQVYIsCYQ933l+v8upeb7uvO50gnVOTne6X79+r27Vv/5Vt+7tlBIvrtQfUEpJOl7SSZKqSaokKUNSRFIVLvcXSUck7ZK0TdJWSRsl7ZR04I92S6l/gGvw5ERJjSWdK+kMSfUlnSKpXJzn2S3pR0lrJH0r6UtJKxiUYyrH0qIbSGovqZOksyRVDThmN5bqWeyvkvZ718x7+Vi+Z+0nYOnlA86xWdJiSR9J+lxSVhHfV6AUt6IrSOoqqY+ktpJKmvc2SVouaYEk76JWSfpO0r6Q5/aUXRNv8AaxlaSGwI+TvZJmS3pd0ofATrFIcSn6ZEkDJF3PcydLJX0m6VOUvM285+FxF2BlGTDglxKSejBIXwS871n76ZIux3Mamvc8iBkv6VVJPxfZnSNFrWhPSbdLugGLE1DwtqQ3sd6DAZ/zLHOapNqS9kiqLul/JD3tO667pHewzDqStvve92AmXVIejy3xpu6+6xkn6XlJ2UWgg98kUkTn9SDhTklLJN3LTXlB6S5JTSXdJmleFCV70lnSmWB4DUl3ByghwvmyCZrnBJynt6TvCbD7gI2buIa/Ak1ebHiAa72lqAhCUSj6PElzJD0LPno36t3c2ZJGStoS4hwuYE3EYqvDHFLMMR0ktZY0CNdvG3CevpJKAxNWPKh5RlIzBmu9pFqSRkuaFWXQCiXJVLTnmg9LmomL5kp6CFwch/uGlc+x6oUE0J6whq583lP4fZIOSSrDY2vfub1B7kjg2x3lew8x+J4RPEmwbI2y702mdSdL0X+S9LGkB6Fcn2DZnuJvljQX5fUOeb6SYO4rki6SdDGvN+XRs97zJa2VNFxSZUn1iAlOOnGeyVG+ozK07y94yz2S2mAo3uA9JukD+HyhJRmKvgTsuxCL8ILWpTCFdwhgG7DMNwiMBUk+bMJjEl8xUOskvcXnPEj4AWWfAnxU5H8nVwFbQWzEkxEkST+Z15YwQPcTPzoBgxcVVkmFZR0e9o6SlCZptaSBkubzXgdo2xWS3sW6PKtvLuk0cDKWeMlHPyx7DZa5k+M9mDpsgmkZPMejgJmwlp+AjCfxsFUkPILuTePa7+C1CZzvRv5vJ+klvn8vg/laoooqjKL/xk0IhfYnC3NyjaRJJBDf8VpLFNEX7AwrJxAQy2Hth/jcYTLGLdBAJxEUdSUe5+H1I5KGca4lsJDmDEYPKOdzsCUnNVDuRdRVvHv+eyLKShTsnwDTBOHvF3DMMh69ARjKc8c40qOctxzB08P3RvydREGpbMDx+QTd3QzyUrLKTBKhzziuvfGGjlh8Jz7npe5jJP3HXGdzlDuCgZoI/36aQRwRr8ISUfQQo+SR0KML4LpLuIg8FP0qx3pc92si+U4w3UlpPt+Nm6sXx7WkMDjlsPjm5r01YPtbBGInLqmpCeSMQtldDTM6kUDenJhyFfDhZbdPcUxcyo4XOm6V9ALPnZI96jUFrlqbZGQ0x3gp8MvcxCFw8s8MyCnAy1W+1FjAgQc33xD01sEMdhmIKEOArUJaXwdWUpfAaMWz1n/ytwnI+ysWXYGE5VHfZzysHst19KBEMNZgeD8MKemK9pQ1FS8Yj8IuQcl/hzPPxiIf5Bgn9XG5VShhCNZR2RzzHZb3Kda/MeyF2fsBas4GGtoxAE42Qxk9IzkVdrTSsBkntYCdNOCuKfFlFTDSF+vvAh0s+MJCKtqzuH9joR/zBel88QkUbhpA37ZiVa+BeZZd3AGUVOP/gyQinmXMAG+dXARfnoayesAC8rFQf10jSDLA534ovgTHrMeKg1hEWZTXFLq4BEbzNl6VzjW35d5ahym9hlF0GbDuLEb/QqpsKZQi3+TLI7jfi0T3yxkQj8ueRcrbhnMehpGMwnqtNCFgXU5QPAjGZ4DnwvqncIMTQihcTCp4UNfLpPIzeG25UfJrFJ2uRLlBciL8vA6P7Qx1TFjRI8medqOob33vewWb96FC51GRExnifqxhhGENc4CZuQHflQEfP9H3+maC6GkBn/Ew8x8F3YSRdgS6Vrz0K0nWeODxPaDtqYDPDsKC+1IPmc3g/69hLIFSInLZrbHeb4/VpVDunI5CD5lkYSuK7gQHzSRZyCdwejflJSs53NAtBLcg2U817Vxf1loOPN9hLMlJU6AnbC0lC2/KQdkZeE9Z8Hs6EGilPGXUB8km0zjHHu67hcleAyVWCl4WJUcIgv8AI7Pgq23MsVkMynQSgfJkg7fw/jdYwihw8hxccxB/F0PPqvmSHispWM90Sq5OauJJ8chBvKw9cOjJYKx6ge88Z5Lt3ojl9qOg1Y0E51MIwnMG2n5/8TGgYzgBI5ui0ZXQm4ch7yVIKPzYVAr368j/Xr3jOkb/RhTb2AQmJ7l4QUETst8BL66SN44Auy/OCqGTqljypfz/Kfeag6E8TtDbgye3xGAGwVzSiDMZMSAnqkXXNano/VzMGJ4/hLVWDVDWcT4lvwxbqErgGYur+z8nPCiWkr8k8K4BWpxcgkVPRkHxylbqMS6odiQgRrjWDLLbS2BWU1HoXSQxWSZ5GYKHhVb0fdz0N1jMeRzbl5EciML3ms+kcKxV8o1w6Hmm1JmojMWTuvraB2oy8N1QdrcEzn+Ae3qZ/7sRX26kJj4aOtkb2MnHqh3FfB5Pq0g95HcSBB0eHCyCsnXDQgWejcHaf8H97Q3fZ7KrfzIRe4Q09sskFNE3kHVuJ8HwMxMn2QS5tQl8R4RzX8H/N2PBPzJrflWMz15jgmxTP7cOsujbUHImJ3fyORnXM4zcAmOl7bBwkdjchJIFhiVjpqIGycvcGEoW7GRkFHgqSI4AE4s4biSZ5pXEnqjBDl7/DUhwm/9Nv6JrmlF7jsTCyk5qBJ0JDsdz4jEocwtR2UKKh6lLErjpaBJmsqKjbxIgHvHyhWvxnHS8cyZWvjfgPBV4PIDOxOdPsAf5L7oP1GwN3DiafA7tmUqd11Xc7jAToSn8eVlhLV5byEB1hJMmwhJiyQ8E7HMDMs54ZA3VSAGRw6J89iQ83MlUuHRl/7SdVXQaIyEKJ7ZD6ALTXOjkIEocxP+v+4ozlZl38wLFAvD+PC7sMwbobiVPXoKfP4YH5RTyzK9BTQXDOJ3nKUBnOQLz9cymV4DqTuK4ayxk2mDYiqxrH/WG782XzqOWPM93Me/xZb+idDv/5i7Iw70dUW6mFCl9/UIoJJ/BvDPEsfFKfbywPIzmaoyzP+yiJpR2BxO9A6gNfUuMOOpZ1qK7o5w5KLkRFn4XePcXLNAR+5bm+bM+JTsFbI+hZGEBc5KgkIlJOEeQrCH+iLp7UwznFfRyHO8dhh5ugO0sxppdUnVU0WlMpspg8xbwybVh9SD6unz+dkZts7mYRGRrIZWR4muWTLY4vlySiQ8nlUjNuxAbyvD6EUOJOzgdO0U3wIIPmGmmbNzjG0YpH568nNTTjdYkoCNRqVZIxbzNNRaVbDITyVeY680GBT5kuut48/0z0VczdHVU0S14vsxH9M+g6NKSGZWWvN6dEdyXBLctE+KYaPI6eFnUHf7jqXNUNJnnx6b79T++btcVwE66Kxc4RTsFLjSJhuhpG4jrTCAtjZgvm8csS2FkEqMfr3xNxM8t5PeHkW/RjbDqlAI+s98c/5tuI0T+M3hxke8Dv/qqc1twBTfb/G4SbmKpaQWIJhuZflqPx83HdaN1oyZbjpCVCgpp4a4Symzs+87FPDb7re7PbLTrL1uugqUl0XZ/AN1LRH6JVTAnGDegVPsn+GwHKoJnR/lMQRaXiMyGXZT3VQ/vZxA+8JVIl/LoGWb1CFlbRfDG3/meGlCncDf3A3Xhwko+GVU0eRd42M/fQVJhV08YRtVwOkxoEUqpRQ2mchKuUcSq9TxvYV4vCyYvN5VLQfX2YBA1I6Z+usXX7H0VF72Q1NxJEx6XmtaswsozWEPfAKXbdtyBBMC2JFcZBkrGQzW/ZsLC1W2SlebvJegJhubEtZaVNY1FwlM3QYFrpBpFbzVFpFNJQR/gZiZQ38ihSUZJsmZ7E0PMBfYw7w3hu+tSk45gsbOYTOjCDbnClZu5voVKXw08NaggFK8sh9bWxdMPkYpnMnfov6dt1IFqppoahu2/qG4aZSoyUpWgK64LqKiWkWXyvb2wkgp4lSt7ZpuEQGBjkKzG1dtSa1kW5bh4xN2zW3K3meahaGVgl4ydmGowzEb+1YzGaHjuWqpyjU3amUgnURjJg7M/Tcn1Yhp4bLrbAMoZC7pm8bgpQfoYJG7iuCwGt9nASX1iiC1FOCguFzHF7O2+AzqTCGzFXQ4ScZ1lxaphJENWARstUHQvrLIqZYKg4n+VgHnHvUnEaWeMpXyZ4MlA1xzf9zsozkg1o+0f9cVUq6zYY4sjURBW+xN/86BSTbjRPCJ7adoFrocNedf3L9hIahKDtqWNaeZ5BwwvnVLwJ7zujLdsNGxJAYfSYvRZJMsd45EtWPbrWE86HDzFdDG5lbJtqC5WhjUV5aLN9gx2WSilU7RLqPIjUch9Y9aOzGYuzK2xtsfGmj8rSlmP1XTBgvdGaRUTkNeKzqPANoA4xZYnnJdUwqLHwXh6AS0y69vzIkbrtqc4A+W+TmnUFeb3Y8kpSUwEEpUv4dxhVru2IqE5OcSxsSSD9w6YJXWHCN4PkDANNnHMGebOiGkZyDBfcBBQH4BFO8683fBR/9TWsZBKcSy+bMQERWHEBeC9hgzsY8APEbemGB1V4jE31ViEjeIlGY0+vvLfZrruyyTBOgor6cwP+rv7Y0kXvHQ5DS+ZcdJUd887DEeehnK/AJubmvlKp9OtqeTkoiIVAYd+YKrG36KbA0aeFAMXi0pOwz1fonekIf0j8Uiqr5zwC27/YchzuHvOMjXwigTduijWwUUp03KwIWIIdlVj6huZntoL86hkcMcR9KZFVCWLJjl02rtiezK+uwrzf9VDHJtqSqG2yrmH4NzTl+ZXQqdeTNsYQak5vOjfBeYcrGeWKfa7mkJ9N01TTLIBbuwmGvKSNLNSJeQsfAPTl23r9tWYV7wOguAMoCblg2xn0T8CBxHTu+CkJ5nZy+CZzPYPZRLoS06mbA8xYRBG1oacc2wNHOT5eqifoE9lPXOsrh/GrTTzXl8XIVK6gos/gr9A5W4Y/FBcmHOdRDo3kyW/MC9XGNmGJYaZXHb3+rVvW4rXyKI3077rZqRczdobxINuztDNb/mXNJwByyjFlIywZhc8Lk5SIpCI5MdYzBNGsllS4e/wD5K6pi7+gUlc7iMwLvOVSUuY6b7fzu+U6ihcM+q3TnKJpM+y/sTJFPAxwxfFi1te9S2zCCv5NAMF7dMUJNdQPcwzbWLn034xlEmQsabCWI/AeYQM+6iil0Hp3HJhJ7OZpXjQt7HUctP/cVMC+9MlS3aRufq7pAqSrIBFnNEkAwooeLJrx3CNnW9STaxsWicuhK0td8meU3QesxWKA3fdUuU61ByOlaxKYLYnJY7+6YHGy0eb1+dD7SbTG55pssUuPM50JQ6Lx651oG2M7qFypg77iXG9wb76bHFKWWbH45EFIWvUVQ1kzjCTCSKzvJTU+0PmOw9DeR0qHJ0Jsoqej0sdb5vzfNLbsI9Dpm/4ZLpNj4U0imM7noNg7B2+Slw0ecgkHcNNabgLxjgX1jLUQGsPIGSlDbRW0bkmivc376Vz0gr0mF3G/6cyylM47nbT8VSc0i3EKoDVTIudiSLCrCPvaLYletXXw/JIlBJESQOjk23zkX+xUEMiaEkK2DNR8L0kL66ospskZih1j8UEgxXQoKKe5nJSlkAeK0M9wr3MjnGMX6pQJKoHP25mdkMoBZzMYADnGgPtZvpQmli+7beElWZW+S4ed6Doz8xyiffB5YPMcLjO/dOpkRRXDaRXAUrOhjXFo+QSFPEdq7iNSt0KEhu3wqEdOYTl4bfz+LZ/r70glxsFFnU0JP0wozwc7ni8b4p9klmj1wfXKmopGbT6CVlJObSNgbawMoJERiz+cbw5h3zie0jAPiDFVT87QusO+9jJ/49ewKL7dWSI9YGKSbCNnZDy2WDcdl/knmm2R2uD+4RNCBKRzgFrYHZhVbei4Hj3Gh1KL51gVQN9K9OaUxbtQ2rdhKJbCVLxmkwCPOc/cbS14OcA/iVhGmGtojzKdQWVvyWy0VNI+cTX6zaL70t0qd0DeKyIOe0Ctj0+zmdcZeDS/Wn6yUN3v2sWjRatF5oG88fj4Mgnw0pcAvEUf8neA7UhbupkGxliIkpOZbGRU/JS7qE2m7zYe/dz7z1AqoPKsdE6cmMp4GGm9+uYi4gl91KnbUKBxbWtehF6im/D7MJKJzPTLBptElne4bZPdkFsIefeymDezG4HtWKc42kmDn7GKAMllqI3UZ0SQadzjGNvYv6uFDRvHXg9nfd70IdxaYxzxCN2Z90RcWz3Y6U7FM5d07sE/21Awr9I3BwONw84x5VmbebdvnrQf0lBLj0BcE/BjWoEHNObebz5WNUMsPrPYJfD6HqkquMKsJAw4qaeFhC8UtliLcxawzpmu+RaMKxHWDJxNYX6jbQSf0A6nYqh2OSoNgxNBMKYJduCFJ3P+sJ1XNQEs9QshRF/g9fHcYFbsIaRWLcXoLqbCtsNQMz9BSyejyXOUzLh8qcQH2KVTKuj0AUme1vLPYxgh53RVPXeIo+YDJy04VgHgelQu6q+5cxRpaA9lQR//BbiXw/lfQRMTOHmemLBB3DrPtQDMk32Np7nZ0EX23LOKsyWxLPecC50021d/DnKCWolbsJgvwD8lSY1Ho3rr2ALn1tR7qNYcho91q4Z/z28dpHZNHEPsPhdwPf+l8SzwaDdxXEYAbIemWM2tK4BUbq32dLYe74fd32IKZ7BWLnzKLce5j14+uqAnRWiSbpv3XoaGWobs6WbC5xHuK4noXAX8F3p0MNc9tv71ezWMNXX1vCYKaD1D7v8L559NEbjooNhJNvAbeG2Z2Jdt2Dp76BMt3vLPXy+Hx5wNhZ0GRbejr99WMgS8zMh6+C0h3jfrZZNZWBrUyptyEDW9XV77sJKnzcz2BXwzKlAydV44CQCZAWs33Lpe42Sh8ezxjLevUkjYNkA8Ps2ahvluOAFzMa4bYIHm22AB9BDcToWU5LAUxc37ArZPy7Kd+dg+blcR2ksMWgXXuHWSxjwqaTKNVHodOBsCLBxDgNwA7FmPJXII+yl9LNvhx2773QoSWT/6AgY1Z//gzZQnYzr1jJ1315M+zSi+WYcUGPbaevSkHguHnKKaR+OJQfwmvVAwr+Zq3PL6jIYoOFYZC4wOAKo2mESoFEY0FsofpcPLibwelho+00S3ag7lSxoAP+PhfS7ztQxKLYW3TtuQU05cP12cNL9GsUTQMAg3/dUglK6n2c6AU86wGMOQTELpbpBdVaeC/+dTrCeb/B/m9nJvRtwNpXPtje7uI81+2OPgYXF3dgehnUEyREwrzTBpjmuNo8bX8sgXE4RZiSzwtdyY+3B0+G48jMwh7kE1doUqfJgI1lg9WLgYD2KXUg5sjUs5kcC33K+182DDmVQ3maQunEtm3k8juufSK19NXz7HVPJexQoDDMz8zspTA0iH9p0KwGqHYq6nGDmJgC8FDwF3Hb9IFXAzGbw0Qm4Zn3wMtYMSFcUtBDrq0F9fAyDt5M/l/FtIna05X5fhNM/CitqzvfPMR7Zk6yxNV4xEIhMWJJR7BnDTWUBFdMoE26A53rWeYap68oEszewYLe1ZnsePwn4Hie7cenqYHk14OmIWZkwHfx3M0IzzBLnA2SQLaBtWXjfdVj2S2a7t1VUCF8prJKSVVWbxei7cuodtE71xWX9610qwj5SsB7Hgzvj/rH2rMtFsd/DCE4nO8sxzfGzqBG77io3cG7V70fECLfkOALF+8pwZvcjCplKgiSzfLmJ5KQ/1lyPVNyrfrX3HbuQbLOnyQgrwjhmFdAlmkswmgOutuN8eWZrtCXQu7tQrtuxy26IeA97bnSAeUxkWuxH4sb1Sdgd56gUxW9lTSRAjgPzvBv5DKu6BEt7BopnV7O2oGo2Pca5hQJLkMykEdi+wiucRW+nltKCmZBr4cFu/6Y0Ysmn/LVhoJ5jsKP9GlHCUlS//rYeFzzfYHNHlJgJT/U3f68muM4POJ8Vt64whSBXBizN9u1mM5KWgCZg9ePw8jv53DSMIB9MPp/3wvxoWtxSXD8ceR7spLv5DZadwMT7RPgfQp4rFb69iGphU6hgVc7pb3WoDuPoQfer49h74MqjQ3aUFkqK+6dQTyNA9oQVONkD9/0CfF0NT94dZ3JQztQ8zgQGGvvS+hUE7TfCVN2SJcfqx31d12oXrC1oacN2lL2JILYHeLA/7lsZC60Cn65h1uFYWQ0Wf0hSFfOHD4pC/gi/C54ORWtF8GpEVpbo7mF7oHurzI+UrTwWyrXyR/wBdi8Z8azSo1peEPOw17Nct1+I4+SeZXtMw6tZeNbvZYueB3iBuDg3tipYJP0fhbCpNiDQQ0AAAAAASUVORK5CYII=</t>
-  </si>
-  <si>
-    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAFsAAABaCAYAAADXaio8AAAR8UlEQVR4nO1da7AcxXX+TvfM7O59SOiNhMRDoWwUbIMLPzAkMqZszCOxY1KQYJMixo5d2BUHlwuIIRQJ5djB+RPywAbbcUwVwcQBbAKOnMQJgeBH8IPwMmAhCSReAklX97m7M90ndXp69s7u3fvYuau9EtyvarS7d2Z6ur85ffr0OadbdMq3nvnDoyvBp0saKyzDYGZEAL4E4DJNwN66xf/ujyHfDUO/ZWn476si9baEUZ+lnFaQ//0eAD+RLyERHhiqY/tEgohILijXgJtrzGcTOi4/9PW+vM05DeA+AG8EkMyhrAoBPzUXH/trHdYBgSb0VTQdHilUDE+2ejpYoN/VkIBQpVdn90RES8uK+hNOr+kUNm24Q0kRFABmgNMHMDOWMKOfUaj86e6R0pcCGJxrQQpYU6R9wf6E73ihZgY2lPQVihAK4TOBHSfu0xGRBwOJlQtmKWM6cFqswzRl2GIlO8zUa2fr0Q0EwE8Coi9VC1RA1S3/8pW6vXp3bH9vLOFtIrGzSfdrFBwS3RQR/SYBf1+EAqcIhOA6822PjSanDcX26wCqapHxBgLg4YDoA4rwcQAvFuy4Ti02vlhgZ51x8Yt1+1ujhv+D8he8BqGIdoVEV0aKTifgO0VJbry0siZUFDkdKTpYyK1Z/l69zveNKTp7IKBPVRSdrAgRc7NefRWhqU0E7NSEr2vgayA8y83nEBTs9YHyT5KBcXlE8jahwPK3iYRx+ws1c8fSgM6JlLqgougDJYWBTPXoQ1TVqEx/eiTsrBExhe5TRHco4DYLfrH1Hva2YVTwuQF8IWLXLokIY4ZRtQyReK9GuM64eyy2d9uA3v7shI0mDJMmcNU2V/pQgTNbiTJxlp9fI+BnCvgfAwy3NsM6ic66dfEGB5zrQ6JK6pZR0YS8xNOkJPx4JGHIITWUl5LX6UTod9cdnIqmnH0xyBn0QI2AzzW1wx/SDOL0R6sqKQJVIvrdJZquArCWcwWleonRp1N9nv2d/Be5VsiWl2FS29qOGb59zPBDFhgnf23WZRVNNqLHncEQYaciPJLVAzMY7A2SRZZbJxLpfefXmNvNRGdFoBV+ZWWk/wTgi8cTXGeZ/4mBoezGSAZPL/X7YuvI157IfbnJrfSwxOKakYQ/P5LY9QMBnRAQbSLiN2jQUQFhdUBYTkSDgbxLyjWOUxIY1BgGpJtT81uRX6XpGkTAGIBhAl4iwm4wHlNET4aEn8bMT1lgpLWw/Hfy+lgIVql7oAkMnMTApQnzhQbYBuCLHZNNjIQZ1YqmjWGIGxWpi6rMXzHWkT7OucqMGsa6SGOwMtmvto6bxkDpP2oMPI30wO6ak6GoRLRuMKQ1GjhsX2w3RBqrZXpvgRUDmlaPG+5n0LDhVCuGyqupScaZiH8egJRl3qPJ2bv7CCSCsZOFZPBeBezSRPuSdJCfFnmzln0PpPam1kmG+aOGcb7YEL6do0U0ZVBnDDEQZ7p7SUinDDKdUmP+9HDMMlP6jmXsyMi0Xo+LNL6uL0TdAs9WE9ftKKfbMop8t60rwg4FcuXsjS1KFqgohZgZAelgX8zaguuxJ1vUmLynnITVAFypU17qAWCt72FSlyT3zFYiWqU08AdPcz2Awxh4uwUuTpjPaeOLmSjANdTzNXPnrlpya+CrZP3bLRG9aXVJ/dWSgO4f1PR3AM6yQJSvoBxlLV0+PTL7UytnqzuJz6u9/AvQNPlJQKIJNbFwMr2q2rsNxNtXnd510tI4yiR4siRCkyXSihMt8FnD/N068xYDJ81NRGtgZ5+mv50zwzkEI4nd/YvR5PNrS/o3BjVtTHwtMkdTWdF6ED5R1vSRAU1bGfgCgFukISJZ9Zz0yfXad8k6pyN+n1aoWevIH7XWTaCCHJmZ4yobsELKPlOLKD+oKm9JtB9guTEQSHnG+1XbwTZLs2iPi2uWP2iAEzNVMR3Kiq6NgFuLkK1EJ44bfunxkfgqZopbG5IRoYDSgKbjBzSdVlaEfi33Weyqis6e2vy8FGfqJ3EDIWF1SWOJ1u6+ccMYMcaVJS9nrSjzMD0GZNpKjBKJ+xbOrrRg59q1XmLT+nHTM2eCs6KYMWEbR1C1/NkEOH02oktE90TAP1AHXsI8gmw2+EzVfGtlKXn36/qCj9TadFKePGpo0XP+nAiluGlHFOFnlvEEAyM2Heea+v1MKiD3nI7RQrbrWAysE0sCwD4A/zrNI0dne5YCnqsoXK5TmSmEILvJAOaxkfoVywL11uWRelMyR6d0RowFbCWgC1aE6leXuBrxS4axvV+L+UU7Y4untKKXLGO/BV5mYMyyE2z5tGYap0uriZb7dMIuhMqABmCVTLsZOJqBjQCOqTFvAuMIBioAvjIN2a2PaQdTUXSZAh4vyLNDg2zn9WPas208uWQwCL8dEFbNFkhoBTNGswExJFoTKaypACeLZc6pHmXLPNzHtEfMSgDj/VqPRor2DgY8wsC1DOzIdLTxuj9IfwcJcIlhnFoDly1juYGYi45IIXllDTyT26KIv9+houj6PsKtrZZWpwhWRRrDsRV/ttOvE5Z/sHUs+aPj+oNviJFRtMu0i+QogBTR0pBSx4/UWiZJzuSE08NfZW9mymRKqdQmpVTvBzWLcy1wWtFIUBFEhLvKhKtb1WYRBNqNsIDmtNEyS3y5Zm+1wJHHDYR/IX9tM2sthCl2bZuwWtOp5vMy9yhk3xYFAT8IiT7me6GDnavd2QYqa1PexJIBc1fVXDdh+HOv1eBBSHioRLhQuZlpykudZzI9Z0dDZ2eEZy9Np7PBq+G6Pq7iV2nUoB1CokcGNc4PgO3Z6WEjeR6UOvMLQmVuVHGQZCZa9j0FXT2S8LUGDXfqq5pzDfwwBN4XAL/MGiq2a5WnWEMdI4gUzlkZKQPQFplYyIAlM7G6V9Qyfr1QN9eERM8fVdbXK0KF55BfcoiBPNF3B4SPAXgh6+nVzHE02fOPiYETAdzZMdmDAZ18bF944XDCH99VTf5tXUlhSaDxTDVxgQRxMIlED9XtjUsDGu3XtFGnzk+eTxLHQkLl/PLCsWGUJE1BAZ8BeDQjdsICcbMkl8YtfyNmrCpENjOGCFgzoOlmIpwXM+6PvVS/Ujdp1IYImpxquWV/zKG8XzETZUZyKEp44KbeDX1IMfCJkPD9etZjxTluU4nOuY/7asw3Afh1BTxWRJc6NSyzuIEAazZW9DeJ6NTJ04ThxCL2oRr/3DjT28/XTKuD/5CA+CgGSQY7Qj9RlYDv5+stsla1TYIkIbUbAHzI/+4013CSbGFVJvyDWq1bG6nbDeOsfFxSnE79uciufBOpHortISnZE5yacZhhtM+1a1kC3MLARfN9bpMZ7XWwqJRb+jV9MPOmCc+RnnRfyu+dVeM8Mk2+C3kn863RgUMjpCatGuNmTyERplBPwMa65TtjxrndqNUUbjjtZsvWl/TNy0N1rfVuYc6iNN6PLdNp8v5sH/A1Q7G9YdzyVpUNQgvAaDtIuFQBj+YnblUf80sFrCWonX5srjN/1wDv7FY92gqil3C9KlRXD2r6pmVsyL9zIXdtSeHYvgBLgkkzsWpxw/M1+459CV8yYfm/eYFJV8AODVwfEp2hCX+TJRZJZpL4g0WdjEzRIwTn8AK+bYHXd7M+wXQnMtfpoKZzQ6U2DcX8xxa4KzsvhItqeceyCD8eqru4IlKV88q4sV+2TLeMJnxSWdN5EdFZocJ6SUmmnJPqQMyOJEefgB9qwj8T6D+B5vQxtAmT5VI41hrGFxLwvPVzO0xLdgahsEy0aU1Ed44k/NejzH/JwPPwhEvU5viB0FkmUm3DjbDXSMy4d9zyva8YO7giVJstYzMBJ5U0NoVE67L05Ix8n//uIGW0sXSm1JfS9IWtivAogPsV6L8M89Ott06qiPZRpYRxfgL8qQFvKszmLJiVbDTSr6CWhHRpyeLM/TGL3/k2CRhYnwG/MlJOf0vaWlVmor5RXkeOEOGeccP3jCZcPiyko5jtMQnw+rKiTWVFR4utX7Vcy6RQYpB1O5nDQc5HwzsU8CMCbSfwU+LMZzetpl0R4WWZH+QTazgXRTc+aZSncn1cwnxlDFwwVz4OKNnISV+J6LhVEf3jfsMf2h/zdQzcD2+lkA+yaq3SBE3ipgwo71GsKuDJCcaT44a32CAldl9sg4dGYmtz1wrZ0SQ5tQD0yQTsxmOVCwC3htEa8U+k8Umd6uFWHMnAR6uWPzlb7LFb6PhNZmQcFtA5g4repQh3APgygAdsi/dwQKeJmnWfpsbMTcQrahpAk/z9bVwB7CdU08L1AUqj7FmyT5tyDjeMiyzz71vguF6QnKFwt/H2dh8YF66K9Hk15i1DMX+VgQd8cLUhbUkW8CX4pBwFm5HhB8osP9zmXtZcB1ACN3RxO8vH/+2NFvidhPkiBtYXbfd8MC8d1YjJEUoVovf3len9E4Z/FDPuNox/AeHh2WZoE4bRr9mlNawqqUbWLPmlf2MJNyVDpikMqbvXUvvkxxxWWuCMOvP7DHAmw4fjFghdGxByST0nl4GTDeMzIH6kanFXpOheANstsLc1pJRJcUkBy0LlfOlZ+tlIPCnpmEXS/TVlTrNx32YYZyfgd1rgqIUkOI+uj74ZIYqwjECblwe0eVkAG1v+P030kAZ+zsAvLLDNAs9xmojZyCHMr8WcgxpZC2C9pB3W2amJEy3jrczckwGvUxxQUycX+lclRW8ugd68VOPDCWOiT6tXDGOvsbyDifZY4h0R4aYs5hc4a6apONEc4qM4zcKlWaxl5iN8EqSkNRzIpnQFB5TsDK2DnayZ0qANRNhAik6wlKYyrI6UuDpfgve97IktdtcSp8/FF2bY5Y2c3os6Hwj0hOxWtEtp4JZUhiwtOQf2acOHLF7Lyxx7jkWye4hFsnuIRbJ7iEWye4hFsnuIRbJ7iEWye4iuTmpoGhfnXJFf9jiNFOjOSjy40O0ZpI1Tn2chzvNpKIqn5o1TmkmBTveK8ssx1ULng3aFbPE9G8vJo6PJpWsivU18SAXdQk9kX0KwS3vTkzHIWBGu0cCNNLct4RpQcAukzkyATxWrVnfQHbLTf+zOuvnensRuPaE/crG/+fjh2uxjItL8YJGy4tTPsmKhs4a6qkYiwqCkNGiq4w39YeG1J+hiYo8ENn01+rpUZGF03esnkfLnapJwGWNTX1h4hSa1CR5Qh4NwfJAtTTkgkRq3Hwmn/uiijRU1kvDkhgLw5UZzpJp8beoHEdtdtbPTBEvG+pLC4SU1L6marxrhdLtSF4ToUpHzRjcDvjygabxfB1gVqeILvLsIznZ5kMWrFmMLXaWukJ0uaCK9oRz8ds3ydr/VSCfIVPQWWV2C9mIoWkTSd4+c427ADUREhhVvjheY7e6QnQpPcHQ5+PP5DEkMnJqRLd1/d93ihRpnueBhjXFFnfmMbtR5IdDVAXJ+lnWb5dRTTs/LmlxwHGqOqEN6weui16+HWCS7h+i6i/UAl3VIC0eXB0jnirDdcLFmO161bFuU0Cw52tMV7TdjW1B/eNe8fgaIHxyO/yC29gkiBB0OZeRXYDT2YHLr5eN0E95sZbEiXB6BvtjJ/1HgkRjGe8cs/1mH93UVXfNnM7Mdis2DhvG4LNcrtHvZ1J118pAeU2hDLD9j31Dk3m6ia2okXWCE0r6EXW61SGTc4X5H+YhDy5K5xt860U/Z/X7tzbSb5vYKXff6ScP2JBZHaI3j+yOX3F4EkjL8+GjsNioIfLQmBjp6gSW/O+bBgq5bI+KAWhoQ3jIYYVmgOgoW5q8VoraNJ84nne16GecW+M8FoqgHA1qYVN026Go9ZFdgWSH27uUlDMgerB1Kdf7qfMA3Q6dCKi9PdrGXMeRgEPCukS0SfUwlGN5YDtyWGZ3q6wMFR7gsklI0ttB16abXTx1RUh8eCOjphGfcOXImyFZAu6c5LzayePyO7XRzFVmKOWFxartQWy/RNX92QBQsD+mqogOix8MzkC2Lhy8D8K4iBR8MPa3rYbH5FjHDucVlHj3Goot1EYtkH3RYJLuHWCS7h1gku4dYJLuHWCS7h1C542DAbP6ig6WehcJrgXcTy57+A52mdXURmdtiphmk22jS+5YWciYp/3tI5/8zCID/B3xOaPjes1bpAAAAAElFTkSuQmCC</t>
-  </si>
-  <si>
-    <t>ACNUR</t>
-  </si>
-  <si>
-    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAFoAAABaCAYAAAA4qEECAAAS6UlEQVR4nO2dCZRU1ZnH/13VTdOI0ALNoigoDEkmIi6Jg4iGGJEYSdwXdHCJYkYTMw5GT/TERBMNRhMzMRmDZhSjRMWIEhFjTDSCRAxqZBqxUREURNmkoZutm17mPM7vmq9vXtW7rxfomVP/c+rQVfXeq3u/++3fdy8qoIACCiiggAIKKOD/E4o0+U+dfTrFks6TNEnSU5Juk/QFSTdJekLSryR92AnGmRfFnXhsESok3QyRI5RK+qWk4yUdwWuMpKskvbaHx5oXmU48tsGSZhgiR3hPUr2kd81nn+e6z+2BMQajsxJ6qKRHIaLF05K2SfL13T9JekjSibt/qGFoD0J3l3R7O05ymKRZqAWLNyQ9K6lZ0gpJD3jfD5D0oKTT22EMWUkTJX0HddVmpCF0Zpfx/Duiv4+RNF/SFZLq2mE8kbqYKenT3ucNkn4AgcVvTZG02ruuXNK97bDojZJqJH1P0vOS/iVm7tk0DwwldAWWv5z3XSX9ByI8QtI0SQvT/HAMhqEuDva+ckSe4X1eJelSSbXe5z0k/UbSyW0cz1xJv5c0UtIfJX1dUgnflWE7eoY+LITQvZjkcZJ2QOTIxfqJpC4Q+BZJW1o/p12TiVMXjfzWD1EZPiJ372JJH3mf7wOxL0nLeQabJE2W9JakvSX9XNKNELsBqbmHhU1EVkedn++a6KE3wM2R31oJd03m+2WSvippSSsnE+FUJGKI93kdvxWJb1Oe+yPdvVTSaI/DIiYYz98RM+xsxdg2SvqrpLFIc6Qqt0qaB1dfC/PNTXpQUsAyiqAgMgiHS+rPj0R4XNL1ELmYVU6Ly/GTy737Ig69Bn0biogI/8k4ffyK521KOb4MizwCRhuPZB2B97OUYGmcpMVJD8qFiCNOk9Sbh2xGjNdjkU9jVc/JIdZJuBlvxSfyy5LOjiFyFq49HZ/Z9wZeYCzTY353El7KvinHGKmFC5CuL/OcGiStWtIavJ0JSQ/KR+j9jUF5B191g6QTJP0FQjyIemlMMfiuqIprY4h1L0R+1vt8IH5y9PpvfjfyTg70rnsbKbkqRlWMRwqHpRjrNhjuOUlT8eOjRe6LW/s2132OMeZEPkIfTOAQYZ2k5ZIug/gRoS9C9z2SYuCRdPxW0oWeu7Rd0jex7Cti7ot+60wmUw5nnoTn46MWSTkJG2JxpKQ5kj4TON56JOFFSV+TtIA8y0WoN+defjaHyvoYPqEj8bwVIlg3axEq4zb08gBE/MoU/vMAFmW89/lSiHIXhI68j37m+y55JnG4cbnEfKaiq1+GKE94qi1insckHRs47h3o94Us9I8kfQOjOJ9rSviuOzFFN/8hPqHPhBClBA8iv/CmpJ8i1tFirIQDNwQOdjA+8nHe53P5vbks4o+RmLPNNb14xaE7Yuwwknv/HWKu4/3PPfW2P4seGtgsR9WtxPBH3P1dPJJ6rtkXpovocpT/AJ/Q38DAZc3knmPyl/B+Lav2UuAg98NAjfI+/xtGNdL/X8SFdDjI/F2XxzVrhuMcDjAZydG4oTuQvPs9zu6HH/yFwHk8x/M2IPGR2voSQY1wLUv5jSv8my2hPyHpU3BJMSIrRO08jFgVfvMTgYMbAJGP9j6vYaCrELtz0N9ioDb4qcZXjsPbXrBSY3zu6LlnoNObUXm+CxaN7z5SrSGYSTS6HDpdZhY2S6CUMX53LKGPIwIqgZur+TzyTwdJmo2L81zgoHriXcRN4n7jj3/KW4imGCN2T0xeIxrfz7zP3vT8+WFGPaxGv/rSMRA/e3jgvJ5Gwp8hrjiJzzfxvgwd3UKCLaGPhMhZxH2t+e5H+IrjEc8kZHHwx8VcV01CyGGksQdCLP/i3fM/JPydmmjAFfSvW45edtjLS7VGqYRXY8Y0FKboF/Odj09AxHMZk8M6GLSM9y2k2BLa+ZcRkfqg+IVeighzJyv5QcBgvoxYxWGOeUY3BmTHUZXDxVtgVEp9jrC3mWybxeGGOSKD+HAOvz+K9q5GRebDmwQuUf7l26gkESH2MYRu4Sm5CZajNoTOKcfY3cjAogDhfEQ4KXnUlftyJXNmm78PQjVZPJYjnD8DHeh+I1c0NtO7/xDSnPb362PuE87A0BzfOWxnjJei3yPJ+hbM0dvo7BbBlCN0P+P7NfN6hQzYr7GuGwhzk1DB5HJhqfl8uKc2miGUQ6RGDkMKJpnFi8Z9Ftw7ypOIebikDiWoJ4cV+MBxiLyGQwPm+AhSESXE7sbgv8I4nLTsZaXDDbDOXBD9+z4icDMWVKzeWiWjIuGKbfwbLexXvAhxPnpWcMbVBB5fiikkZwl952MPnJdUjxRaHG84tTkmh21R4Y0pDquIcIUxvI3xrDLS0mRdT0foTSbC24kOvYIARnDztMAo8B+iIg+DeHsUiSmLB41qGosRTsonFxFMnGUI9HCM+nB5m9IEZigLIHQ9wZUb60Tc3tWoFvnejSN0jSFiA9bzWt43khPO5cvGDTQfosDnFAxsF3PdVlRBM8Q4JfD3HE4ydmY5kmBxNcS4MsHg7RVAaJGWuNW8/xYRZw3vba9JeTEPbTJu0Q44zSXRH0RPhyIpZXoOLx9zzRi6psyyCcPawzDNbC8UdpFge6GR5NUoItuhuMhOAl0sENFxQsYo/7cgeD3ZNZGuvN4LczsK801ivihAMnwUG05sNAFRRyGL9F9MzkMQvAI6OqMfGfOvZkj5CY9iK2FpL1ZkIjmDy1MMNkTs4lDplazSFhP8698nMZ8Wobn1rtDlYIKXZVTvu/OMP3NNpK4GZ/hjFIXOzejHWpLnW3DKR6fob8jlOuXDBxCmPVFjOC0NtgcuchYO/g42YYqR/PeJQI8me7gyg/K/hgvm8O8zJI7OZcUaPcOVD60pglZ2QKPiZnzbtNgRSOgirhuNqv21iUqnY5hvgG7LnddxMj7pVMTthwQSX+f76hQJ/tZw9GIvR9EeaCJHkhZ1gYRuhC5FeFKRIb4D+k3Hdx/NtVUZQ8BLiOOnkCs+1WS0VuQJW33Up9SvzSlcx7RY1YoF3B5wjeD8N/n7aPz4p9EOaygOiN+flyFZI6KvgaxKb+OCRQvxeoqB1qQ0iB+aAbc3VrVCfYQ2AjV4xY8T4GpXbXcFhcjfnp+hQtBIROfSmv1NAfPFlIPdlrIqXtmBHP1RK1rVagKucVhk1NMYk0hyxec6bN2ODEl412k0EX/0UJMgmWnKNyFoNvmM0MFuTnF9WryaQh0oIQ/iY40JgnqZBNkZ/LvE9ZlkuPgBdOsRRFgu+7aQDN6EmA7PXGhOYRA3xOSP2xuvYHNCEUrogaSOHzASP5RM4UC8r184JnJex1R8zixGcD+I9VOitUlxld08hA5tvVq0Gwi9JkX5TYFRcBG5mDOYq6u0OOKXEFX/xt2QofqwhWLpWqKdvujOx/h+EDo7xJcO5ehauKE9+qqT8IiXB8+HkB7CLtizQRD9UaT/UBh1DUWEeph2/wx1wP7ossmUY8YaIzmCiz9JcJOEpHyvw6KYrv2OQuQ1PZnQlSrEPMSQF6NeK6je1JDCGEMIfgFtFAfSQbDLGI6G+iJTN5nVd9Z6GOH3AYGJnuYAy91AFNqa5sjWYk6AT705BUcfQGltBJ+9Tih+kdljcxEqd32GbWPXmO6gu3C+XbXYFTb7pVAdSV7E1j2wXW0J/c75sCmQ0K4r1aZz5+NLP8r7C2HaKJ2xS0c/gU6ZajbaLMYjyJqCaFlA9USIZ9KE6r263u7A+oBg5KNAQu9n/u7Dv8tQFxH+FXqud81GGaKyZ6h834XVdCjz9HLINoKmgARRY8x2iN2BpITX2sBUg+1C8tXpJOhYyt6XXY0/zr27G+r3piFwIp8XeYFKqI5OSnk2BUy6tXntfEgKpD4MzD7mShlfSidrNxjp41KXI/RCCprNcO1PaILZ4kVVoRFfUpNNc8KE/ObFEDQFGNcktRDK0fYaN84JlLa6MY5f2tY22w9xvYnbK9hpNciU/wXhQ3Y5heSW87la22j3agxwyZq47q8BbcRJUrImYbFKmb8NyJYSNU8xavYl6PcxLKE3w/qu/PPPkr7PvuutJocR+Y3/ljDgbQmBSFGCB7OTbqcDicBybcRZgbc0hIpQkhQkeU1Jpa/vQhe3F30V99xk2ig+oI7YImjz+6Nf9vbtnQNhl/KA7VQObiSAyYX6gEEn7XGsZyIv5JGQjdTm3gsU+SRC5/P/jyHe6MG4diJBQ0xrxDpUSJV/s51sH0Lvp3BPlhGzn49TXmk4tS9VmFwD35nQ1ZQJdBXdtblEPm3Ak0917MgjERFzXee1M1RS5ruSa95CuuaRmGvRO2IJHbks/4W4Po1P/Tv0UjFu4DZj6MZiMOPQgBeTb8J74mSFfOeTVOeRirPpH29EJTQSAJXAMDPIcTwPh9/j7a1pMdnlNIDcQ+RTSUvYBRD+b4aAzcT0F+fwrRv2kJ/cFmzKwdH9ifK6oBqct/QSG5smUMR+A06+j3taBEeW0E2szOdJ7w3jofejPtx2ijoT1Y0h7PTRlDLZ3hlQl8P9O8GkiJeZec0gl/Ew8x1OJXw0zNpCrfnieyeZtzF0Szoirjf5C1srK8vR1d+U4LMWm60bScinZvLp7zgkuYq+zu9BT5/7/VeMwdxo3Lzx0Gs0kvyQ/2B/0/0mdM6xJJG+gu6227waiSCdft7Kw0cQEdYxofdwg6LPapCOzSSrfhzThJgLDaQkBxDOrudVyzMeDSCgwzuovBLG9BZezUx25L7B/HqiEnriyrqQ+3bP1dwHf/kHJv9xHaF3C8Rtut+H3Icrzrqm9MtMRm8Ig+qCdzEO12cAsb5zx9wBIlkTzjemaF1wKEEKfI5rauWzsqa5s8kLjPZDBbyGWnBlqnfpTHIV+yPNJiMnVX8g//wP9ilOJKtZRXdxEVtw5xhVssYcVNKP1zSjcvrzXTMcWYeh2d4Kwghp2G5cMPdq7bPcWNweRkvkx1AB93r7u2eZ7NyJ0OMQQ+SVpJtjnYBcuu9VVsYGHf0g4mmoi3tN9DeQtoQ1NJPcZ9KH/1ewL2roSDywKlPVrmXuDbh6M735rcJhqMw12Xy+7B8IXBaYz3pQPj8L3eZKUa444FTLOPYABh+Fs4fRD8Zxe11mo6rcvO6EkVyPnc1iPk8EnfdwlKSg4Vl86e+b+L6MktdN5v6B6L1Zxts4l9xAZz5bT0R9t3re0+NEdi5/0Yek0TSTIq2i0/ZMFiEv0hyZeRhtY+Nitqz9iVVtwJK7jfBuE/rdrSZDxyJLuekWwxDvkDjaG6m25zw1EGLP4bvgI45Cj8wsxwq/xqr2x3AMh+i9IG4VedjvcV8p6deFVL07Gw6jv9lK3RSMbHfmPQv1+Tre1IfGdvUOjYBDCT2ccHs63PsBIfls9HZ3kwu+He/DHWHpmkr8jv49jW6khW0KYYY56GU1UXJ1TK3xFPzsb4cSOlR/LsCy/g6Ddz1Jpf6Ik80B1OCxzDf3fy1G3expjGS3g8OTnPPhelJc7bMZ6T2RwKQKg/hCmgJzKEc3QNwymtPdPudmjnJw/W0vsiDVhK63QPQebKd7vZMkmyowgFnGOg11V4SnMZjtJocRuNnzQ7bgCPwizQ+25vzoS6lm5Nqe9j6uzlOEq1EYfyENgD9DJ7blMMK2ohwinUd0O42xfoacxbF5TjlYggeW5hypXWjtQd3D4OwTOT0sFxqx0H0R1Y3c09bjNduCsQQfPfGBt5ozN3JhManiO1q7qamtJ6IfzsBHwhE2ZN2GgYws9Bt4LJWomLiSUZbJl5g8xJbAynsp6ilrwv7aHCF6bxJghzD+T2JrKryqyHuoxJfQ36FNkrFor6Pne3JgiDspayuZOndkme1525eq8YHovgqqx3ubY4YEwep41noW60W46yBC/eEksvaG2M64N7JAtWbBV/Ba4h303Zdx92GxyljgVRC3XdTc7jrj/xj032fhnl4sTtIhJEIi3oXw9uSBjSSHBrMHOwkuTVvNwi9Crf0+4N42o6MIXUJV4mQiSUfcpCS9Kyr8Ef25Ei/gOrh2Jt9/muRWOZ7NIjjzWDKMxwR2VW2C6HPJ2s1LuS0kGO1F6NPxLEpd4zXcWpJwn0tZLqIq8SRqYgcLc5U53PUZiOCCnr2wC9dioG5ATZWQU/8imbajGUtSq0EDOn01C7wDb+TO9iBQexE6A/eeSm6gnIkVe3qzEb1bi679M+K70nveOHOM8tUJ3aml+MCnET4/5BnBCnI0x+MX9zSV/YwxvK4gUcvvPkmk2C4HDnSU6qgg89ULA9cEN26G+/yj1RzcSevfhGh3pPjNM9lzM4vgKldNsq9pIi9DAraiRlYGHs6VGh31/7CsT+jriMM+EPd0gqLHU97/WxZxOoS8PIfPu64DtkMnorPkiodAoLMpNqQlssMCEj7DMZwjwm7reHQWQhchvueT520LFrujGwKMcQEFFFBAAQUUUEABBaSGpP8Fdc8BzQQn6S4AAAAASUVORK5CYII=</t>
-  </si>
-  <si>
-    <t>WFP</t>
-  </si>
-  <si>
-    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAFoAAABaCAYAAAA4qEECAAAgAElEQVR4nLS8B3hcxdU+/s6t24tWvVfLsuXewMYNF1ogdAIJCQSSfKlAGpACoSQkoSdfCB/p9ITQmwGDMTY27k0u6r2tpNX2vX3+z9yVjQ22gf8vmcfzyNLeveXcM6e85z1Dlj/dhP/WIACfsKx/C5pVdcOymqvzQ+5dhgUE9CQkS4fIEfxh5+hv13brq781O3TfyrqCR9M64PcCLhFwAnju4NgFD2wZulXi9H/OKs27yy8LV21s771epByh1MFZnAWAZp+AEEpB3nQL+OG3agSMEO7cZwe0Ozr6YqRzPM5TVSOh3Fzrwnp/cm6e43vTppRv8ztF8B+e4b8y7twQhXDN/OL/2gWcArEeePNAzoZDwzPqgqRxekFgl0WBnJAPFsdDhOV740DPF1oHkmUvSNGz0lrm0bRmwuUQIIkcnAKHl5r6L2na2z/j+vPqnqwt8uL1nQNlWw8Nz4AMgDPAQ8hKiRBbXJRw3UGnhNyF07G7NVy9dlPrDMHvQnnAY/l5SxlKqa4/vduCf3jcmy4ejP7hynkN1+uEA/0vSrqtowtCgcj91y7gFjlaGwqs28BHlwRFTPqf2aVIWRTvd4wgmtKwfywzqyNByojbib6oOXtRgdsjylKS6joEGEgpuudX4dRpzhx/+vRJhc8MGU5kJMkCDFwytfTJg7p2Z0ufwrlFIauRFJxFSDTfLaBtaBzDSc2E4MIZlYHnL14244cxKqvNQwlPgzR+yh1vdNz75PsD1+VwroEr6qp+q+jGf00Oo4O9ELoT+n/tAiLPoSTPvYVzEGwZSK56qmv8Dt0iWm1+Hkokgi3rD61wUguzywPY3BadNAhh9vQC/3sHB1OIpDUMxbV5/dF02dyy0IYkkTv7xjWIxAJME0G3K/zzOVMO3vjcHvREUhA4Yl/T5ATUl3CIa0kkTAUgKgK8OXZZMdcxoFGc4nJhftDbXOyUzYv/vuextzsiX71uQcV9hBOYVfuvjGllORBqfe6Tnju7IAl4noBjS/Mz3AnHEVS75Pef8nu6dw9m5sb7wiWFMt85buhISQK2DyQWhHxyuCTPu1ZvHrmifVSdvKiCvueTCESdw9ahTIOlUkzzcuvL0nEcNL3giArwJhImFapznPjZuTOwe2jcFrRAgNRoHAErDZ3yABEILAEWlXlKeeSIlPg9oHtHFHCcud7jkc0xleaOunm/2yGPmf8l81FZXgoh4xBPehB7y5JG0R9WEFcJCCGf6SICz8d9Hs+e9tHeCtHnmto4ubCTd4pQU+nS7rHowqWTil5cWJ3/yFOb2684GI6cErUKHuFcEnJcMsZ0ZQVHBNSX5W48mJagqwJEy2kx4QkwqUKBkmInqkqctgJIAORhAVv3pmEpBLJODBDK5M0JhLOt+ahlYlhXMKAbgm5QIjl1mitwBlM381M+GruW/hleSmlBPgQpJJz0ICZoV4aiJ6agIseJfInAxKcXtksClgxJe3Z1kPM+GEjMFh3OVzpHkuhPKotH06qnLuTetKSI+6A4KA9v7hhZvr29yGWltfRYKp33RtvIqop8V8eS+uCGAdOF7T0WUiJE23MRS6AiFSwLompmH94CqGCaap4TdCSFI3dJYFimqWNNTxKnlQexqjiAbTvHLleTGa4wP9AWGUslxijBpzEd7Do8R9DoMpgz/1ThSoXbB+GTjmOfUwuwCNCbSsM7loBmHf4WAf0Ed60KHApk6w2I0s/7I4m5cxaXo1QEHtkan0M4grpS394xXdLKg4GmrT1jK/IFq37qlLxd65qH5iTipnfWZNerLeN6ujcVhcBJ4IhCiSTj5QNjX9zcs+5My+QooRxldypwDv6qBuFrIZ6sJYd9PEeQVqnjG682OzZFTPrUGVzlA63DN9zzbt83nC7d+O5pZTfHRdnSrBOL+ehnNEBQoyXgyqgg3KcLJMpzcnBydT5q8BToNHmYDj8KKWybDWJBFrKnOJG4DQLU+ANNVU2xgf3D8aX7o2LxKZN8A/2be5aX+JxdVS66nfe4UFfg2vtB6/CKV/uSs+WQb9euSHoudA1LCsS3q3kNcYgY0TmIJixKLARFnp/klrt10BkcBW+wt2Zx/fXFOfE8tw+79vdnb0Dg8Ern2MW6NXK6JAvWyr/1FcVjFJUFvvAV8xq/Wy0Z79Jo2DY7RwaBvWiYgJmplCTR/qNFKUpkoNJlAhY3EVJ+8vA7uU8vaPueQRHP9aFiMIWKHBlOMQbBkYPUWBJOQQRM4GMBKQGcPBerDzrfX9MSuWSgd7g+7s1RWgYj05bUFz7easnK5PEY5uXK6x8T6A2DA9GagsYA2gdH53q8kllcXrFxgHJIpAG3JsKhOU3oBk6vDzx+62l1/8NRLQhQzuB5oiRiSZ/AKx0ZAvPwfVgWKvK93VUFuQeUDHHW5Bqv1HrkTaHysnfLoHelRnsh8uRDRSHsKxacLieC+bngCAe37JyQKUVxchhg8cmn1OaJU342QbMvaKaFtG5CMUzwxEQsY6A7rqKAT6FfF5EiHLiPyFoWOfiDcjM0AodbKH6vO5GXHFfFpVXOd+bkS2iOAXJx/m6/ryczllYWdWZQuqkrvmpykX/LzPJAs0aB1lgUOosmBIUAHHRTUPslFzyKNe62NGjs3iyCeEbHgZ6UbTIou2GTosYrr51XX/PNuCJiVQOQr8SxTxOgZ1QITIIToSHTYKa1bqeMYI4XbpaiZvOiiUFhEWJnkp9ldA4mP5ugDwv76AXD7pEtL5Ez0RAUkZZlEOtYSbslHh4r9Na/t/f9bHtPbJ5uEs3l4lGbk7/TVERMdWrwevie6SHf1gOR+Jxt3UPXjKWpa7pb3PbmgX6qGxSqJUHkhaPug9rJd5i4UUBYxGHamtk5EMdonMIjkCM3mFFUkQ93AI4qpDUJad2CQZnzzPoYpvxMwLLkgFMW4HZL9jOaTHE/q4COM/qHEp9d0CcalHCQUmnkyA6IDjGbFbNJgQPhFAsNtwV8Yt+BsdTn3SKXaiyQN5ZLyUNqRkNTUgABR90+x4Fo9+jSd9tjPxc4wbxiUs7a6VVBDCUtvNeX+ZgfsIUBgmGOCTuNhAIcHDUgEP5YbSCEylSDJ9UJS6+2X4groyCfaIDTCZ4DErITMmTkejhkzMx/NCV3y8J/TtCYcIguNw+HUz6S2rBlFuIpzJSemVfo27a2LXoBBx1nTiu8bdNA2kqbaRRXlyDgkLCg0rXrjb3Aps5xvtgnd8WSytub93UjxTlg8d7j+h72J7ach00HDnXFoZgsuaLMNB8jLEp4EFNBZ0snaqoLMJOkmCEAdbnsc2TcblhJHRb9z+eHz7VE/rOCBiaWY/YRJn4HqfXI1JU0UCzzO4yMcgFzDasmFe2YN6kIigkkx0ZBElFUubk3nR7eSEcUYW69b9uCKSWZjGmhK0IRHtAAiYBqlghdhW5YDiZMNtkLUIysdrudov0Hh8CBjyoyVBOmockwdVDLAK/pkCwR4DRYLGY9LNj/Iqq0c2D8Py/oZCwFh0Oy7faEVts+qdlUUVThefN0rWSWIHBqY8C/2ZM0IVILOw2KpEkgu5z95zSW/W/3sFpdWeh9itk2O761HKgKOCFxBEphoGnyzMo3SotC2xjsIUzIyCXwOH1u9RGbypA/2hpufT/tfGNSEbYWBESkDRH1ObmQBR6aaoHjOHs12OviM2a8n2XMyyX/WUEz4SZjSfueQ/nBI8I2QVFamAtXbu42ly99MYNADZlHWDftt9BQkWd/nwcMwcq9oboEMDw81qrZtHiyB6h3ZW0TDbmfm1Oc91yVn4csAGQiBGAClgXJxmPYP4Z1FxXmvjp7fvGrk5xJ5HEZhGQXCgUHOJ5geCTjtdxBp9vvD/MwAE6f0OqswMkE8kr+A4peVpT//+ZUyUTUIYu8/ZOzszOC1HgCkXDkmOXIPLimm1AnJvuMm1AkFgEwDJFNzTCg6gaomcUuWOqqM2DUzJ5DNy3ougHTzBqnbGKRnVY6A2qYE3+n9jG6bsIwLSiKgb7eCHZ1DaArPO54uyc65c2R9DzC6bAi3RPQ2YSQJ5Sc5WTqUc/w/1fnq4qK/t80mmmGRTjX2qb+6z150lBpjvevpg2BUehDCla4NdR6ZFujP2kc7wjVAnwCxRx3Bhp1QKecrRkM0DEmvnBYB93JOIiSgSHw4AN+9vbtzzXwttfwqGOIqGk0jWrYPKhVnlpbNGnfcGxWFZfSpnm0t3TdzKegSUIFVnvAe52jV7buDFdetqDi3ik+dzptGllE8OjxKe16g1f+dIImE7GyRT88t8chYutAes4/tm59cFtrdNGDF8y8eG5BLpQJVJcdKxs44hSPN5jGDCc1ODQN/kInMhxvJ10UnP3z1FwTq4MplCGOg4ob4waPEjeHoJuHSKittTwo3MkUHKoCymyupsEYHYNckGfb3+kYwTR9FPmShoJ8EbUFOejRYq5O1br47f2D563ZbX3lnEm593++uretoKTytQSVsGMM2DeuG39at/P2Pf3jn7/9zPqf1BY63xxWnShmr5VlhRwPnft0RbACz6ew0WQiktB1fY5HkveYPDEcPMGGttGz73mv9+/DYSOvqMAzVunW12ujgziSq1CKCMeEUgSXeKwmsGPYyxPcPPSYBadqIWAY4CQes3ItvDeeQGMogLPzDMjMGarEBvwljkLiBczz8TCpCYNa4HUDkpIBncjuQLLCTo6MoUoS0RiMgiMiDMgsnIZqCnNWNhQtu+rZvedZBo8ZRQ53Zb5DEgTH290jo3He74WUK2GR27nu1d3OsfdaInO+NLzvme+fU3/Zikb3mmHqQ2pcwYGx5PSGKUV7Pdwno36yDbl8gvrLhGBN0+DVe/pGLrtmdcPZXS4RhzrGFj+0ZvdTEYv3sSV6eYP0q1w/RjO69SE0aWMGOgw9A1H0HpY9DJPC6+Tg8IkQxA8PtiZeaqWHYpMeQ5HTa+uKQbNntCasKJuarfX0iNGkH4kYbFRN16AkFbzUZWRTZvZiCUFXNLpgUyx5D8MzJAlYVhU0l+TJzeVF/qQEG+pGkc8JL3EOfWVR1T13vdF+V19K893+8t6nq2XnyuI65/ZDqSH8ZfvgbUsV/tUr5pT8OWNYJ7XgskggbG8Z+dgHHDmcWnPgTTX3obVND8yuKdyYL4pWrab6ztne9mjE5HyspLSyIfTK5Uum/oGjFqSjXhq1KHSTIqLySFEDliRCEgimlThQFBAhMCDnOCWNw6bDpMcuSiYE5gzTGcWT4/MnBZ7LOj3dArWD6ax5OzzZ716Rw64RA1vDGmQ++3fdtMz+eAbgJYTcBibleJWSgCOVY0Yz7OURTgZHAmC56pdPrf79pq7RpesPjZ8ZTcN/08t7H3vmG7MXl3vcoxbnzNz1Rvt9NXmeV0uDnkHNsI5B/Y4eWtqCMC1wbCmLOZv+FEXCABw8jzf2Dn5/LKr6SpzWaCFP8dimzm929ccr2Unn1uZv+Ok5077gMTlVNays5lCAEzhs74kgRpyoziEYjxuoKxWR5+TAOyUb5LNwLI7AhMBN/MRHMRVKUSBRGO4Adh7qXNkT1yNVlcXv2Z9bCqCq9qoglIpUzTCWQpx95OCAFTVumDkBODgK9nKiKSU5sHsUPEzUFvpfyxiZW3TRuyMb/YjQNRmpWBbNc/Bc6pbl9Rf9WGl+fUf36JJDY8nJj23pv+bSutBvXJw4Gk2MeNfu7/32pUvqf5YmFjjLQqFLADOtR5uTne06hFn5ro8JujgDdMcMcJS6dvdHLocoocDBdXeMpvDgluHvEoHikqkl931xQfUdA6Px0wQirOMJ0Xies7XWFJwIx1VYMm+D9QJ3uPbIgHMcI0hWwJV5C8TSfczc8tRIywKXJoSJglUxbINOnNBpHk+Q5JzFT2+Pn/Uly/nejEoPVI8bcVmGxHPo7BicYUXNmM/liJsWs+fAaY2FWOx02ohiCsALH7QXr3fIWy9qzNn8wzOnXz/YP2aHfgmnC7BEEJ0iaRgwCI+4Zbp6w6Pzf3XulPN+v6H9njX7Bq99ctfAj+YU5/+uWzFTLJB/6cDo178wr/jeYqc4bqUVCJwfpnRsedAhEQjacZZvQASopGF39+i0vmiinBnTPNPYzGWSlaW58ug3l025YWGJ78BvXm16YnqZd3Dx6VPfZOFW83AccDhR4pZgMjjxI7bzGA2eCA97o/El/2geuDIejayKpXU55HOOU9H7IidwrwamlWyskRmElqFRg0Nb2kBXVOeV5FDJLIcLAvHwskBMxu3QNSpFR1Pz5sysfVyQstUuFmpSnmP1CTgFYGvz4Jlu1bIuWFC/oLHUCZnjYLgd+NeWfnx9VgG8EstbVBTycYjeIDwCn3mpKXPFE7v2fP8rq6Z8b35VwatPb26+7Zmm3soppcGWXQNJDCYyeeGUvnBGnufVYUOHSj9urR/timSR2A+XKUsiiO00hsBjw1Dy85oCjsVh9ZPKY1VFoYHbzp46V0iYmase37dlc1969SklJbc5eIHKmQR2NXcirllZE/ARoVqmhVhKQTyt2lNRNKw71HPJz9bseue1pvC1G/tpxb6oUPhuT6ZhIJq5qb1vbP0H+wd+ELVc6NHd6EkKsBQVa9v6VjocngVRg/t3NJUpZWETW0V7ukdW9KhiWaFHSrjVJLzpKHI4C4JJbYGva0uUbWgbO2vOsro/XDArFw6Ox94RHQYvIaFb4thIZHIikShkAuBMA0kthWZDp9OnlN39zmDm3O//a89Oh2WR319+6vyvT/M3ryzzHRA4y6Cmia0tI9PDiaRdJGB++KOqu3ssBW5Es3B4xiygZSQ65c87exe/vq8Pb/dETmVmI8ibSm6Op6s5bXke3dj24O3rel8Oj6vuyxbV/poTvb2tXaNIxyK2bGVRsFPjo4cdgbAEpDUKZfsw1J1haHtG8Nzbw99SEjzPwjowLEjgQCiBYqgI+Fzc9v7w3ftah5cOD6noT5iBv73fdvfmA4nzynN8ueF48qLWlB5IUyBkaEJz98DZc6blPLa9fwSd23ch1dUDSUujyEXgkai8t6f7B186rfr3IYEonGKiyOtB92h66nt7O242qPbrlvHYip6OTtvSiwRoiuv4+4COA3C0Xjaz6s6xMSX44xe3Pffwxq6HQ+UlfpfT2OOTuAjL0fcMJJYJLg+axxLn9o+lZ/uRpbMdnktCLgjRjHlE6ySBw+83tv/6g6i8+aHT8ja838J5OzQdcyrz3h2JJN03vXno+QMDifnMlk0tduz9xqLyu3mRg3dUB7FkEjX5VXtaeiq0qpJ1ssC12cuW4R2sxihw8BV5oHtViAJBMpUp7kklp0DmwDPciJqgeho5Pi/8DgEPrmnB5CIXuXhy7leHFDT9cF33My3h+HLCW1hZ6cW2vrBVksM7EgR469DIBTGTCg35gYPrd7X7CzMaxACNhRUVYR+wYUvH+X4ZBzxBV9sUAN2G5fv37uYf9/SOrl40qfzpG5ZW3uLKcaYi23fbabvGcajIdeEKSQYTeiZYdu/e7q6LDw6Syc9s77qqbXBg2sXz679SHvIeGI3p+R0Jrb49JXEHh5UFW/sGGm9Y0XhBWp+oKDCfV5QLzmKhFzUAYiCaThevb4+fVWgoRlGuBxmD5jFWii/krL3htb3vHxjIzAcnwOXRlO+unHG1yPFxU7HAEQbLCNaqmdXb+mLJBdc+sWnPmr19D0YT6SUsCLOxEApoHhfE4hBQkIOk31MyrsfzGbjJ8IirZhXijlU1KPc4MCXHgYKggOV1IXz72b0XPd4+sr5lJLkcBo/V9QVozHPjhf1Dap2DD/fFMs6NzUMXn7+o4Z7hgWhN/7j6rYqGRlcmEMQ+hweb+hMNTcPRi8+bO+mvu9rH8ETzwLQHX9u9JZmMn/rg+ZPPuWZm/n0iR1K6/iE5iMXllOdtM8CQ1IBLjv70jBlXuV1EYWZ0V78y5//WHVhf7ZdreVFGOGMEP+hNeeIK0f7dFP781q6xqvG4gvDErC1wgSsQTbBZLlvY39G7OjKeFpYXUynHaQgxw5KZYF/Z2V3bPkLyIGssy6F3ntVw9akNwZ0a8zISZ6e+TBPyfY7xG86ade05DcW3vtUb/d697zStf+DtQ8+3D8aWGpZlA04smNQVMHiYxRyUoWNEALb0x+AkDoRTOv61P4KoSrA/nESSc7uf2TM0lZmUopCIO5dX49fv9UDRhW6k9O61e4cvr3XyO9M8lL9ubf/lGQ0F/8otKxykJRUocjvw3r7ury2eWvmPZMoytjeHl//w+b0bS8qDm//8hTkrTg3pI42eMTQ6YnCLhwu6zIHartq277xJwbCPmpr8LT85o+YqF0cNiBQ9SRJ6vnmwlPI6kqoldMaizm6V5jIgZlAzVksBNxi5ks1pHkB4X3FkKyMSwZu9mYsZ7jiQRtFAmnPrlg0lQLcr3DochqXecs7k6y+fWf50CjrcjiykY8WzyBtDyVTVwpWL6u+pDEipu9a0PLTm4ND561uHzz+tI+/P1y5pvK0hz9HnlgBTI4rT5My0SQQqcjg4lMCa0Bg0qHA6GE5CUZvjhJKh2JrmIfAWfrGyFi+2RPDElg7Mq8lvS0LkM7H4otMbK+5+6fX9d9ROK/zraFGonSQsW0Bd/eOnk5RRWFea+8pL73cvem5n6+tXzK5/8LrVtTeqiobhUQqdQYNQIMoRuDgJ1LRANIr8DHcMRM0S1Ksb6v7ppm7fz9/Y93BCVW3Px5IrVjtoGozygqEXgYjY0jJ6+kKZe9jOsADkzaiGsKNl2D4hJRAOhPUaFjJEDVplQXIQ5q45Zjt5hPxS+NKawLXnBqyX453dHyJyDNhhoDAv2hgGi1gCIsWXF9T+cUjlnI+va7snQy3y1u6Ra7sGtp7+05VV3zi3oWztEDU1OAilKmXxOojgxNqmhB0DLi0P4NLGEjQNRLB1MAKIAs6sD8FpmbhzfRsgyyjMd7e3hFMNhmUl3use/bxX9LYucATfpGO6ncBIFsX2tpErFjdW/DUZHin909aetcvqy/553Vn1NxZGRxFOmKR3VPdZmhJjfiTHbaLU54WpG+B0E8nUIFjoe7SwWRa0vFD6013nTIrf/k7nA+ERWgiXxnIFOjAUZkIIMuEPx5LTBXeZWxZ5Rp4FC6uFy6pcdryrGqZrzVbDxbxoUskU+512Hi1A1zGlxPfaJafU3N8xElm1J4WmAlnsNA9XgEBtR1fggk0y9IoEISkLIt25vPq+oJUuvH9994+IJKE1nK7+7nP71sQupF+ZLgjPujg6BIuUwbaJKng70QZ2DMfQPhaFavIgDgeIrqEy6MI9W3sBUwInKVhRFXxhUFHn9o+kVuuZxKGvX3LaF5sH45if1hA2OTzTFl4cT2bcC0pc27/x942b6vMcB25fNfUamtTJ9l6tVnRYBgl5HW5nXiypqhCdFpy6NoG5UCgaQcxwQDgK+WdCTyT0vI54pv6ahVWXb24dum5Du3K+yVFHpSyhK5kRmGKOpPTSpMuf5/c6UgyKYOcU3tvTauMOhgV3xmCCJogpVFZNQibnS4fOmVP1ZHnI9eSLW9peY7JvXN7wM+3jHBkIY2M27OmYCOUwgZl8c0XjTfsGUpPfahs5l5NcSOhp/sfPNj362xW1BV63oIKFDbwOi9XxWBpLCZIGQZIVBzgKQnk7Stk1EMd+lhAJIqpCvn6nw7/5rR1Nn9vVFWu44+zp9y3gSKZX0eUkB7EuJ5gMR/ounlrEbXnw9Z23HRzWG577zrQpOW7TiI5poRcGkhfm+Ylzcb7QRSLGQTh0cJyYpR5MAFch2cS4mUa3ZqcRR4YkkZG3myPnZZLWWTecM+O8U8rSL712cP/180tzrHjXKNdvqVDhltb1DrtdDtHmmvjyJAiVfjc6R6OwwEkmtWy6kWpRR8+4lrl0aeOynIDD8+NHd7zdNZyceed50y/ym0TPfJRJzNA3Xs4CUUdlgOx9RBVYX1s6+2ud0Q82tEXG63giQ7Us7hcbBu9lDtRmclHGaBNBj3ogzuYyZhN3jYjY2peAyehnGlDjc2+cIelqgKIuGHQlGqtzn1rfPTpl4972a/Jqiu4P5yRcY4p2mc8TyDz7dkfllQvqf+32BQ7G44m8rkji0VcODS4YiqW9Dzuc6s1zCjomlzsGLRMDoOYRaiSzmgVOGWZuwZHiAibwk2vnq3d+9997nr/rjQPv3Hvx9MXU0/BEIdWp2SV4GUwLA/zgKBUEkaIWYcSoB9zpU6pQW5ALWRQPI/xQwcs9qmAGMhb91b92vNk1MDazPCT0rKoNvpmABZXHMVPjKDRZRlyhiCSNY+bgmAGnyA/fvHzS1zyCoJhUAMdbiKYzSGgmZEJR4pVxmJSVLShRZHtTbCQcDBnUCVuVgu0TdLfUpftk0pdQ5i8sC7zePzQy/663Wh8pKCz+I3X4+t47MHo2eKXg8R2RyknFoaYbVk66laZT4stNQ7+97q3eMwciatAyTME0LbciKa9oY4laZZxwacWFdMZhz1TGCSvNg8+kwWtpcFrGnoaSwZTC4Kt1+d6Wnt5I483P71xfw+eIJZJDN3RdsEsdnEFFg6MFvIA5YhyCKICzdB25LomxJDWBBQ+UPSixeEslf9va+tfdfdE5zNFds6D6bofbmUyxzA3HzgwIVFFAdDyFwf4IhibmQH8E7kwErtQoZuU61l85t+w3MNK2mbBJLpSDLFKsmloCzqbAkgkLiSPoMwsdiV24NbOFUkvHGTWBA0nRERhXFG/nWHraXzf1PHL5KXU/qpbEbuYfNnTHz9s3mEJT3xC+OLPkdx5e0HZ1GzV3b+69qicSAxFNBFzO8RlFngMey9xlqKbCS3Jal1wwJOfEdIFKDswKxXBK7jgW5EbsOS83guUFSf3r8yuegCyhbSg2/cWDzY811Plkpyhq9n0LxCjPk7TzqjkEJeBvnUkI7xzs+VKZKD5+ak1Z/G+tB5IAyahvabsAACAASURBVPVLRqant+fmN5ozX4KooSYnp+OM6sJHecWAy/o4CEVte0zhd7PalfkxEJx9zmocX24svnNvT/z093tjiy2JaauAtEbw9PsdIKyjgJiwwCrZZhbTpVkNNlm8zkpXhMLlEC05OrZ/S7cjzxI4YX93uOHKJZN+nomOSZYlnjHocx/a2TN45njMwpQK775z51Q9IUsWPEZieixp44VoyHdGP1cuPZzj5B5fPLPh4HjfEDhZpYJgHYMl8zZ0qsIyjn1miyM4dZLrt1V53OWdY8bkV/eFL5hTIWySZaEGFg+HAX1ZVSjFOcG1dEjnNY1nXhCe7ld/8vU5Oa//s6UvEtfNDAOVR5J6zaN7h26GyHJjGd9aUXeTw03iMZZpHGfYbHuOIK+o8AgcerxRAxjXr6q5ddfju9coFpGYfWY+WREZEqfC0jmAVxgn2L6uxaLzD9M1my3jdMnKSFqL9hopf8YQ5YJC13hNwKPs6Q9f9ZNzZ1/7+o6hK8ZicILyWF2X/8yQzqc3xNPBF5tHvl0acvYurM39R0ND3f9V+yyjnKepkIOnjuJc6Bkle42jbp7lBs163jG+48hwCMoPFtf/5PqX9z1nSDzu3dg3WxZZOich6MF4sUcbf7lHk3aMuX+2OKS/IHwwFC9amKqrXTrZv6V3bP/w1ni8YSjJcZSY9jK9qLH8LwvynM+nurtETuD141W+2H3oloW4lotgXu4JBZ0BsKKqcN3Fs0sef/T93q+y+9IFCsEwbJLh/FIJPTGCsSSFLBhI2hwNMuEcs9EMz3FaQU4o0zau5DIqQI1Ldq9tH779gsaSS1MZau4cjq1gqyCQI4+f3Vj1h41dkRlrt7Xdcd7k4N3fm82t788pTShEhORgQQ1bQcev+Nm8vngMYlj9GO5pK5NlCYurKp8/a0b5Uy9vbb88pQrQGMLFZ1DmyW0iqplcnM9Nf/SdRPG8hZUQkinTJcbH5n95Tu2W1i7X7q2dsWWMp0oV1k3k23Xt6ZN/tHFf07dn+R2PSITXTyRFux4Yy0D3nLwwHCPABbNrb33z4MiZQ8l0MTElgJkMi6LW7cbCShGdIwpyXTL+smMQRBQ/JJfBxmk4VVU5i3JUEij2945IjYXu1jNqfW+NZkbkHX3hRSw0OWNS0QEjmZ65bmvzjd8/s/FnDbnStubWHptbwuqC9HDd8QRC1sFhQPCBeuhxqoGEcajFDVvav3XejPLvtA2OVB8c0BZQIbsC3S5Py6jhwCst4YvCqXRufVEBhAK3bPyreej6ryys+n2pL+ctkP7rLd1Abb63+5cXzT3n1YO9X42b7qKCkuqMbpgnFCATtCjycFrAccz4MSOQ7+y7cG7xYw+92XYji5dM3rTDvCf3R7CkRkaB5IDCbD21jlC1sudkNT9DDo+Puh2eMkOkPDKUh8YLByIZU81o4vyeqFrFOxzwctypd73T/NSXTqs9c36Jd1cslbZXzacZNg/cUuHy8kdINR95Wrg4LpM2leCeQ/Ervjpv8ln3vb1/42BancJM1sq6wNqqPBEbXxo6P8/jII2sED0536muPzhQ/cetA1+ZWlb4QoGnVSt2SQduvXT+52Eo1tMbe275wfzA+YGhVqgn6Q9j2iHwPKY11EE8ooXHHxIBiuZX3//GnsFL2iNaNeEECJYKXaRIKxR1ZU6s6czY1WxCs5V123xyJpKqIZeXVpYW8EWdr1vdzKA7unWd3rJjAGW8Y5Kp6bwginj+wLD1zSVTvh4sydu1OQZwqmhTEcgn8DAOU4Ef79TQl1SyRPXjDNYwNE69W7c1tb30l4sbX7zp89NW/e7tg88NjKoLZgSMrY9u67p6d294+srJBa2sLCucmi/Q9Yck/G7dgYf++EVx/zeXV3zxtLryt4NucfwXL7X8cyxt+ipyQj0hxsH4BFW1CS2qCdcE7nGSt4IalzR8+bTCv935TvsdlGdsJglEpNgfSWLfZsVOvxkfgFr0CB+Jo04YahpD1Fk7r1TezYspFYLlyLHyMM/pQX8kkmfxPFQzg9U1xU9fMsX3Ym8yOtEaR5GSRXxyLyGFzgk4c2rZSY9iEUk6YzVt3NWHp3c333XD2bO/JJzTuLx1KHZhP/FW/WXDznvBiXDIrmcZrUVYUlOBX28NI5UxXf/4oPOuW8+ds6rAK2IwkqxY39r/OaeX0/7SQw3WRvFJ98jaLr7AGzilLEujPdGwU3YTWDat6v8e3TfwPz1Ro8Qu1RsCMswUG1o28tAOU6OyyYudxHAUb7b0Niyv9iVzRYmG9QxqglzepZOcuH+zUU4zOpwuh/HNaWX3eEFQN1HuYWTzAdODIQqM0xO7EfZe/W7Zxm5O9sBM0BnZGs13Oweebkp98YqF2q9OrwgdmBLwP3Hb8zteG0ppQfACLpkWepcZXGF2oRPlbjd6jBTe6cisvDocW1bjy3v3te19X48nNVdBMBgpEv0aPgX5SSMUsSSPkYSFk7VWM/fCDELA6Rg5rbzwxSeHO75lSQIk3lKLA/7e2YVoLZZo1Od2mE6nk/KEEMPUo5lYZtcY5VbUu4XdgaSqnjqlenW6LZObpGqsOZLGKXnyXmVa4MWQWz7oErGH1dBVPUtjYKFaSJKwgBfQbUy8w49YBbYiRVmC7JIx4RJO8gwAFVn4wvPWMKuuRy+/drnn513D48s2dUZWMjPl85C0LFj7u1nCUiBLOKXCj55dCVBLwR82ddzplcjil1v6zoAlwQVLnVbMKbB3ADi5qBmAsjSUxBRpPAvlnWCY4BA1JIyoLiwpz/nb1s6RxefNr3ykwet4w+d38y4/59rQoRfsHxoJCrrNnWWNdtSiDkuQnWv2muPcKztGvsZTXyIvD+AtM/iPA8rkQo/TdBd7X4rrhKxNe868ICiskQT+CF/Q5mpQYAoPe+UYrGBhsSSFO1KgjkfjGB2LfCJfmsuyTdMCrBh4vWR7T8fnrjLyfvGnTd0/02CILA9YXeZ/saggr7/jEGP88yL+Z1YxnjswANMANnfHF3WHo/9ULL4GREdxjtV7VqM3ziLZk3lt2w5SE5ONRDadPukwEUAGCYcb02tytn9XmHZNZHxw+X0f9P5OU6zpkXQ6L23xonGYj0sO7xSRBdkJAww4Vh7jsggfwxcshkDaoK2NbwtEQ8/Uqnt+e/6UHynHuR0nMJHu8xAEN4hHZl0EODichqrTk8p5Io7GUMI0dIooIzwOKOrU7S1D/9w5OLwYnASeWFg5veavIdWg+50mhHAqiaVlHswpLcSWjmEQS8Xd73ddMs56HijBnNLcF3N4mKzvWjWPH+xgwor6GAZ4BLM42aBg+HQ4pXme2tZ5x5v7R7/QN64U2mRomxrL2yk3IyUeRs6ordgTTFX2ue0kTRaCgx6dj7KYnDOgagRrOnu/e9FQ7f953XKbeVLvzArIkg3Q1zaWfsK9T4xoEv6EhTMssv6h4bGFUUMSf/V+50WKxtsZ7JSi0O6llYENmb6wZAKa8MaBDufFUypxy+JSnNczajeE9o5nnY7s5Mz5tQXP7eyOVMdGIyhwkI4TeW3biUgEhUVidkuHEyU27LEcEp4ZILNvfGHfXzrDkZlgxVtRACGGnalRm8bPTJV15DvAR98fOeazIwaVMFPgAMMcJE6PQaAJlv+Zn0TdZ6glz4H7FL1C7PGSqlFf4rD0M6blPPzUB+7rxzOaM6zq4CwXLBLFJY0FN4UVU/3X7p7zp0wuf0EIK9xf3x/Wvn12bRBnVwfwcssIRJ5C1yycVh9cV1rgO/THNXseKpSEgStPrb4zdZIbYablUCptl+iP+1gUNi9te7829Xuv9zw/NJ4sh6jb7b4Wze4bwvEcnISC4YmcAJuUgpP7paOlZWs0ZxhwBcWBLy+bdmuRQxpOm9axLcjHu3fTROvAOJRP0VsoCxzWtI5/UxatwPnzKq6qKfNu2N42sJojEiySxoqa/DeWTS95szcSPUPLKZ3MviO8NGA++U5v17dPr5qBX585CRsHYoim2UNSXDiv5vbEkIBN7dpZ+TlW/Czqu4sSah7PVNsInUgRC7iPK+RsGwaBZVjeW5/d+uRQOFaeFxIxKbcMM0M6JuUEEfL4wMlMKS0YumrTfo/QnvHJYY+dbDCTY3HQJPkWqSD0l4CbQ4jjTvpVpuxpmHC4nJ8oZDLRqv3nTSMzhuOZ+m/OKpbPbij4SVN3aplipCSn6FC/u6rxhyU+gd70QttPvza79F4GgQhfWlXXdfOfNkR+sq4r59crK5p/cVrdlute3v3lz80sfXZ6ee5GIaOWxjU1T41oHjra73VwXPS4TpFasPw+RJzejwmETpgWkRDs2Nl2wcIid/6dq2oZdwb7ogQ9Q0N4q2sEI+oYxlQTaVWHZlC7iEyPssCfRqvtoy0RvKD9ZsWkuH/Rqsb7ONCTdkHYcKgBbIpkE62TXcemBVPL058yqofjRtFrnYnqaTVFO5ZPHn3h9R2pS7+xsOym8bFM0y07em/Z1Rtd7Jhb/OW0yUE43ccNTC7y7/vNW91LNUN9/etLptxwWW/c+Nyi8t9JMmhTOD0tpuluFyHCuKLmF/td0ePtuGBaHHJkAeUif0xWyDQkyahmER0xy4S3qPKDcqvvuUe39Hxry0AKgwmGlZvZzk87ikCWc8pMBhE+osaf7GTtE1gqkDFDm1uHf35gVs0/Jaej3zqJM2TpdFzRsbGphRWpj6yi4wvabl4KRNNGjmERCMnBnFrRi+8trf5JiZNPnDmv7oG/rNn2/WcOjNy2uNqzyZ8b7IsMJyB8MGJiVV3w0ffbx5Y++H7P93jR2fPTs6de43VxeLaLVSmSFUwjMhpk3Zeb7yoJtLCs75iuVNaswwGFNvR4rDw42+4CbsbmPNj+tZf3RH/QNpSqh5W2U2zG7TsMgrIlT7M00ywmQT/KpP+klIl1iDPcjZkoASoEUfFC5F0EJ9mOw6YSu10cfjTda0c2H+0gOHow3L07oXvfPTgus7Zsj2QVjA+2IVQ2qf3qRdXX/v1g9w3Pt8bvZRDzaTXVj7gt3k7dBFMzUVmY/2Rpbv8v+iJa2YPvtd1X7HWOrp5c9NhAdwRj4bjL4mF74w/6aE53xrLb144mMrKCdWMRD5+Ds/fnOHoI2dTc8ft1Bx59a2f3JXaLg0OGQb2Axfq2DfCEMwnHUwjUhjY0y7I3sOMJz7jdR7nWT+7W4wyH/VN2aOZZ1cFf1nucXZxAToq9MI0eHEpga/NAFsg6/ju01ZltqhZWkW9RiOz3lnAq5JA8WDzFg1e39F7517ea7jENHsV5eSMrGgpedbkEYAQQ5lf54AKUq+ZX/fHOV/b/ShcF3PHmnofiAjc4rcqztjkxwiqIdg9h63jUO6BpOKfWj1kFMg7vL8aegXUGW+aH2C2zZQxfyGiW85HXt/+mqTNVdsmi+vtqg3yXltJ6fYbWi5ycoCkLnkGV848liSemKHJK1URVM1Ho5Mwyv8PwuHmNm4CO6YfNACccE/kNqQ45OlZXBF9XFJ11NJ/kS1mqMts5obC4DIxMf9xhWTBjGSTSCjKplJdV8FnK4LQ82vzqSdjeOrTsD+80P2RaIsdW65WTy39dwpmjmYSNXkCQJgR19byK+1/e3XfFnsFk47hheB5Zt/epu7+4YNH0mryWNTtHYAocoomYUO7nMbfYAc/EPiiHn9zQDOjR9JFeEiWTgaEqMBSFP3dq2T+kkHZzo5c07E/R057pGFs0Q1a9wpgyI5xWcuI6daUNzqFZECmlrGeeDhNi7OOJJvMwuInOIJuo9wnmI9vMSbgcyRwam1btznGK/04o+glw5Sy+IYk8lswqRWOe/4Q5Leu34cdSyA+58HJTT4m5tylbf6wMdiQ1UnXHi/ueGlUMD9OG+pKclsmNlX8+YHI23GALOou/2r3Typ3nTrn2S3/f825MkxwDMTX3lpf2PPfz02r/6HURK6rrnFP1mTNZD0om7SOiK360ekmCALffY/+fsTATDhlDlGBP+/DstTsGPtc0HD//f4cydbZ6iRKGGE1zIgm046vDdvGIQnETIPThDaI+ulPICcRMstBch2EUDybbH/ztxfPWFznEkRNlhmwFyEJ29Z1w5y87K6XQNMVB4VIUFTzRDYguiXr9cv2P1xz6XW/EKoSs2/S461ZM+3phiTseVybueJTtlpbKFlyZxV5YHNzy9aWVP7r7jQO/J7KA9t701Ife6/pfQnjKYlufnzP+uvsgnjlIf/XoZUtvDcj8kb3i0qoB1aBH2szShuV/bOOhn7T2ja8iHues6fkhLKon8BEBxBQRU5JoHx7D/lELaZVk7+BwRskYS2SCcHDM3hufIm2zwy/2PRGKoef5JdHnczlGzBMUh7IkeYpo/MQbLdogfyyT++62g3d/9dxTrk4oignBAQkCufvdtj/t61fBicTeLeF7yyZ/31PkW2+mKBxHnUOI7O8+8mr7RYIvL6z834SZqnn43a7rwcvYOhizUw12otIATV1QVYtb3ms+/dW9vbu/ML/yzxkje7NpJQON2XOQbOPOaNxTku9ef31j4QODSvL7W0dSNTuHk1MHoulJfqcHFSE/ptSGcPk0N8t00JtIvP9Wl5rpHY3XE0Mpi6a1rFaTie7UTxtIT1C6YGpYMqXy71N8UidD6Kzj7M9DJrLZQUWFRo9XG8wOtpHK5tahy1/tVs66XBcQ9Hm6OU5A0lSxr5+3u9AsI4PvnVb36y/Orbg/MTSEGYUlR1bIv5mgrYp8+xfm7Fpa+1atINy6HyxquIFLcvGHt3ffYjGGUBauQn2hLzFT4BCggvXAlrafrmosedoji0mGmnm9XhAhDarHIQsi3HGjP8/j65dlAV5P8EeNFVVA86jTbZqrHtvTf/nLm1q+AFNAjs+BOaUelIe846unFj0WosF1hYW++oSmF3fFLDelDLOzddSGMz8hnQAlJrEsk9T7+MGZpcHXqMTZaN7xXBw7U4ytQom3u1txuP3uKKHbAL9q+J7YNXCTQAhpHrUkK0m7HSKMjGYKliDYGezXFtb+5vpTJ928leNI63BiZYCPrKWEHCkxCP2BoP0fdqE9XHTmwXda535xbtVdNyyrudXpkUce3tx5XypjiA6eM71IRsJsoxGeN9rCicp1ndFls6pyX2HwYgnHurBCoAwYoqqtVbYm0exuMIZhshbjzMK6gpeWzy5+6Z19Ay/d89qBB8IxLf+tVIQZss/5Be5zgWBgx+RqZcdkhxVldHt7l4JPo8hH6n2U6BbP91OhqL40b1dL1Bw8uqP36HG4uu6RKFSNUcCpDbXajbe8aB/hFAh2to0v6htPFFcWeHqTaZ1vjQzHAKpahiB4ZYNeML/0B1fOr75f9Aloer/j+n6DwxZJfMs6ImYVQjKW/W+aA6ZXlf/rxqfW79EJN/qdpZP/dPOy2v/1iFbzI+913j9qiVPbDwxGPY18tpve4PHc3p6vLqj0vyLYzZiMsy6ACIVsSylQOv6xtJddWDcMeCiPy6YXP1XkFDt++ebBhw71xmfDISNGdMQiI3O6hyJz3kB2X73PNrJEAVawYOHY5o6xRd8/a97nBYl8lABrD6bM1R4JhU5i9yDqioGxhA7OzWGoL4xR0wlFFrlNXUP/w7JXnnAk7SDcroyo66bhLA4E2392ZtX3FlX4XuM4GY9s6bzm4fc7fvnIBVNmlAo6DpNgdjONruMTRy4sO7nuhaXeF+99p+WRmCI0fmGa96d51HzrwcvnLj/UH7n6VKcS9fsESDShscLj1t6RM/pievnMXHcPa4S0rGw/LMfnwyGl2Y1NFAuO1SfmQBkKOL8qtOV3F804/YmdXT/99+7+G1IZTmB+gZMP02c/68ZnsEMuwrpkFRE7+8dXRw2tJsfjOvjRqIP96uEJgk5il7UMtoHLxOoxCQelvRmVxeVIc4GSTb3x1awr1WspmXl+Wa9YUJ0s5TI/XLpg6lOnlnmHhnoijn8d7LjjkY3tP7x4atWji6pzW/WjNs/YPapBCHg+7Jxl8N9Ny+tve6d9/JI/b2r53nut8tL5FXn3XTc38OhplaHfdnS24u4DcYRZQCuYiKaoq3NsfE69l+uRJBmmyEFhUiQ8qitqUMpw4EgUpmUcN/pNaQbK/O7YL8+e8eNzp5W++I9NPV/Z0zV4aU+aZANaYh1G/LPYxxFw/yMnso6N/ljMy5hTBS5Pa71LHGSwr/WRzfgY89gtcSDHKdSKPG933Xb0dGBfaMritGo42PWDDq8SMJPGpHxJK1s86X4t4MGTm3u/9NKerhua+hKzJQdnXD6/4K6+hAn1I2GOYB21kwSLIEpy/B3XzKu6574NzT9vGVNntCX7/jGazJx94fJJP1lUVddRlx5F/2h3z/DA4HwWbnzQHDvP0MUXt3UO33/2aTV/nFngPpSZsPl54KDlBcApCkYtDqr5cVPABMIe9NSy0Pv5p8vvHxwu/9225v5T45y1ZNcoTilw6bWUiBFTUQ6x+k3MtDjVyCYwNr3GhCBLcHOESyqWYZqEEk2lUkPINfSFGUW/GDalKDU+XFV0QrBVbsAv4mP0A6fI49BovPytsOuaS+u9t77YFllpsc4m3kJNMPiBoVhWOCBBc/I1t/x7+y/f7Ri9zO58skR8ZWHdg5PKcg6xl+igxzZbCsbRmxuwJU2AK6fX3rGpa3zpB12jS6gpYE3zyGVNieSpdyyd8pXrpha9G4qNv7upaehihqZvG4ws/PaKKuu1fW2Nv3hq0zM/vXDOOXOLfT0C29yENWhyHPJcLkxjAF2u094W4qMaRO2XbNmmR3Q6m1ZUeJuKJ5X+aW9nfFHnYM9GjpMGRMN8ZljnzN0RCxnTpF6HSHlJxtICT9NXp/E773o7fMWGuCqJvAOzqn3dV88qf6nSA+xJ4xgSDDMZ5S4gIH1cyGxnsb398bw73tz6nNOVkz63vPqXPVs2LGcxMzHT8DrJFjXHg3faR09/+I1DD7eHx+qIzT2RMKfave2aBVW3UbY7u/HxVSf0qh9TMkgmp/940bTLf5rZ/s7B0US9JMjo66fl33m2ac2NCf36uWV5a1yennRa0V3DaqY8mUoV1hSG/rb2UOyxu189+OzvL5z6ubyCwPDh87HrBnlgeXkQPdoxFb5jBU6z+4ImdQspYsFR6dv2+g7rXwcPdV8KJ+5nHU/Z7M+0a5MM+izOeP6u1lauH9QyVwz2JpY4HSp0iW4Yi+svDcU5uzfmyH2w410EU3zyx4TMsPKRlO6/7Y2WF1p7tTn3XFL0xYMd6fy2mMUsIAJut7l0RlH7y3v7vvbAO81/zGQUnsgOu5GqOkdsv/nMWV8AkRKR2HEejHkuR4GOj04upKOk2jFw5yUzLphSkLNb0zRANpHik/KtL+//4yM7en5WEnTG7BWQMhxPHLIaF9aWri3P5yMHu1Nz73h5/2NJRctj1t8xMQ+XkqpYXZEHXOTEETEDeVJUgMaJ2gPnNP6gptTVxrwUz2lgm03ZkDMv2O6yoqxkR8pViAunlz3M9g/JcQk4pTbYOWqOIKoPIar0YTTTj5F0H6LKAKqC5EhMfdisM4pa3DRd339t52PNfbGFfr+cKBJcL5byyRqN9XNYBCV+J7f2QOczd7+y95EMS8FFJmQTk3OFvXdcNPv8uaWeDta0n+f++GSDv/qWW2yC4UcnM4PFftfoqsqC5wb0RG37YLoBdpeUgEP9sZlJU/OyEr/FKuUBYcOFk3Le2zakLOwcj03uHtdrdFXxFlQXvLrDImg3gbaJ2WoCXSbQw1iXlgW2j6JT4sGiglhaw7hKoGoKZlcFUCpQBL1ivDDXvWtz+/CFaYU4CC/YNAP2kGVBd+93ltV9w+uT1cpiT3PveHzmrpaR+jlVoX8uqQltDMgySt0SZvkJJnl5TArIkN1+JFjpamKy6j6LNv7w5v6Hnt85fDnjhM8o8O888/Sqh/f0xy/d0DK8ihNNRBWVbO5SXITPbp/IIvZVdUUv/vS08kuKy/K6ggLDM+zc52OzNZwA/80bb4RgmcednG4ghzfT88qC/8zP8Q+PJNKVo3Etn0UDbD8imx5gmFhYkTO8oCLn5UhU828YCH+O50Ts7IrNjcpcrKE08AHbPo2ZhMOTJTKsGUcaj9jOhzok23jGkypSpgBf0AmfV4Zq99MAdTnunplFzv2b20fPSSqag+d5WCaH5dML/igU5b42ZlAEnZI1pyBn49a+8Pnbh7Q5p1aWPZTWBatc4HBqwECpzKGIsQQGouDGY+CjMQjjMThNHf88NPbVe99uuY0TJBs8+vzsynuHIvqWV1vC3x5OxKexSk+WSKvbuUJdgavpyqmFN960qvamAGfakCVjD5qM532c2R5RwP/wuu/AoavHnaKusq1+yPtb9lUun1G39tw5VY/6pPSQpjo9qbRSobLKtQp4JcqtnlnyfxUhqWNde+yKiJLyU0HGYO/4ksvKA+/O9nt7RZVDLit3WRyCFocCluKMDED1ODDkdGJYIzZcyZsaqnKcyBU5eNje06zWSIG6kLdlRnnOxtah4emDKa3Y7yLa7SumfXumVxgpl3n4JQ7FPjE+q7Rw3cam3ss8AT41pSq0Y64zCSfNhlos4hpnjWesMUoQIDtF7B+Mzvzx663PqIRKTFMLvZ6R2y6c/D/q+Hh63cHwDdGEWc5MjUeG2lDg++CiaaX3fX/ZpG+vmlG8dXh4dBLb4UA0NWiqCuMEsztFIYwL8gksZXbIAqFmXtnc+9899J2l08pu/ercmt/PKBd+ny9llv52c3ilF8rMPMlMDxm8WJrvH/98Y9nfH3gn8XNOMhFV4br9jQN/+ME5c1c6vK6x7J54JIuIZgwENAOOiQIdSxpMhwjn+DCsmIKw4bOJjkUu0bapcZbFFfk3rp5ad2HHWM9BzopL+V6i5AdlG7yZ2EYJFX7H3ttXzj5ry3D/6kluS8xRTT3LYaf2NhU9BQVgO1D73lfpywAADGpJREFU2M4Vmum95ZX9j8UV6uZEGZaRxBVTC/5SLjhG/aEgt70q1T2jyBgNC979PztFfinF+bfOK/LgraYu6akt4/dVVoT2zy0OtejGifDViREehxAO5pz8IAJMmRd84V8HN97469f27+6eWnn76tmh9ZW5Oeuvk93r2a5eEckBB9WQGE/hnFL3vS/mui7uHNMaiATsGEzOfK2p486fLa3/ZlrPAu1sb6M9w2Nw6iZcH15mAqQjkDmCdZ1hvDtIcWljCEOxGP6/3q49OKryip/73rvvzW52lyTkseRFJIigEA3IxBoRVECs2gqOj/HVqQ+sb4eZttYKhbbaKozFDlasxcdYqyiPUUFBoCIESCAhD8ImS9jdJJvs6+7d+/w6392NWi0YW6bfzJ38sZndvWfv/e455/c7v1/XqAgt4SSIqkYonEJTGYJJU4QJ5+yYnsfkW9tY22kCS3c1eKxdrCpQuBmWpTmj7pFxXo+rP0SAQAK8tbPzmbb+0SmkyQq6okGpxx26c2r5b1BSAtpt12+9un6ZOhyHjiSCBGeFClpyv3loYOGLe4KPeMyMtLy56kkKj2d8U5n8G+s0Tu/KxtF6xFDgA/PPW3bPX1r2r95xbOP7nexI1cRJGxdVsfue3q+1XjazNDydSiU4GUFggiXx+LzKFT/f3PlGRJRpgubg9c/775nutm5rnlz2blpSjQfoF6EUzHOdufeJ2U7Dog5YXFcTVChlOagM+CAja6Zf9aW5KYWW9wkhO5AwmHhgBKqAQYBoHvAcH1a8YShKS1JWSFEsTgyRBCQU6gTYCAR7j4UWbNzbey9B2A3yTCFPKCuaKu7nLXp8SEoBzbuIthjpeO+TkH9ROV258bjeFDwZXdwRFgNuJ596YemMiwst5qz4tcL0zCsJ9Hi8R9LYHcfn6nzuxguuW76p5a/tYdnXHm1f/u4hdrmV55Se0MnTJWY0WMCbNTNDI6y94+AREclQQFIaqCoBLx4MPntBpe+fbhsfxT32Uawq9h2MTfxyIYd50gpQLhvYGQqSspK5d2bREw1F9lXxaBwEJ8Ab3TGYBBIsnlwAipcBZSIPvNUDKWDARGGKO6CEokMfYiDMAKQSkmv19u5nMc8PC3HhAsPKEURLcOjhA72Dj6YlmRwWjzPhjO7uS+pF27ukHOFD1sHtNSfXLKy/tspuPhbOYv8CFdxMjth5tuuaPruvUP6E839nlPAfrVw8ufmVvf1/2BOMN+FIpKUs0xpRyloRVwZkHIxvjWEqmjLyYWNbpgG6+pMVz398/Le/XzDttgGRUAX1K/SK+FKW89uFDP4xeqJJkBkrPDTTg/U+TtX67avah1NG+8NR6obeY6NQjiWh8wg2BikohwVGFA2E0ThYaAae3peGmxuKoZlT6Qd3dj0XjGWq8a2KQAKCZeBkUqNfPDDQmIPQ8pk2keeZ4JOgTDCnnNl97zXnP1HpdewJJXNBnmiNgcnIRs7eJ/9OHxb4GksIq+DOri5sm+K1Nm88FH7k47b+20IpqjqL2fnYl8rw7slNWeHBTgwImzHvjXSM+Cqgv9auHo4Juk5asEwbCRaaAJMhp4RYGhCJWw9YnhSbmRmCgCQJDE0Znz2kIvh4SIDw6QxcUeOEbZ0kTNIlqKZykm4mmsAmaJgMTzHIIPMRHKlpGRkL+pMojWkSHAkDQ0mt2q0P1U50HQmPpopFGXkMJEQfAzDV3IFyBGiezoLXZeu6tMK17o6Ly9a6C2xqXMJB1mCSLQYcqYI+DhrE91bbzeAZFZbS7ru8dtWFXstzpNU0d8UnJ5tr2YLJhCaWIw3pHGfGM95dXSIVXNpYcrhEh22tGWro6loz7IuInFfVzh9OCXWv9kiBSNvh5uGM5FAURHAUaDaGlMvcLi2iwgcKYes5PRg7Luuox8EzceyWsaFtEObXu4E3MZAZVT2nBuPVqigG9owInlMJYX5fIu1PSwqlafj9SM1p5jSv3XUinjFtGRmJdSgqefhHl057WHIkYDIjFEQZ05UbPuudXqqnXSzF1aU1ZMNFkcdMjwazzP67GvwfRkXpkxJOzuIGmKTgCwegzDqcD/I46Zcd32MkTBRTgIfmaU0FlbfB8Z4wFFf4YOX2DnimKQA2G0+ksioy6yp4TQT8rl0DsyTA7Bqra+OuroBby171aq92UyqVqsnoas40xnhI6Pn9g8p9ktHlU4EiaSBpHUwMGphR5OktsjIbj0qmtmVFes3fQ+IdrX3JqqyS9evGrT6mg6Z9tRfhKxTl3otgkVGFFlq9PdfWMe8nVMum62aVhJAE4d3DOtxkSYLqdoLMs+DkKPACAX86MgozsFBWMAJuKguVHie4nC7wmpLgBOFLKsEYhftMsftbGwDR8z0CLSgZUFUSCFkFiuchcjoGDoaARCLJ2gPFKMlwxDtHBFt2IGhdPMkU2DpsatzVemq6IiUvCWbAhytE3ACmDO01wBW9AeaSOh6pzyuSYwVdEoGTZTOslTxRYjETipSdcjgUN5r6bgcPMYzjazpUl/EwCRMr05reO5omE4IGsiE5Rhv3KlZGIBBr5CX6mHcdBicUAJajYKKFTrMm2+65db691/jVfZuCZA9f4kpfP9me9OHCN6uSqWFRGlI0yCgC+JwWsDsd4OPiYIXsuK9mI9Cbj3aNO9CJ0QRImSyMqZ0SeTBTQHDjlqj4eCihemIKxY9IulmWgddUMifpjq9UTHYmtPycH2644zpCywUFk1MYoziJlDqY/SUV/m1LAwVbT6Ql5xuHQo8KCXGJ107vnje9fFvDBHNby0C2bGvb4A29idicBZN8XFOV7zWwcatfaonOGQkGm0MiNSuSAL+mpwAYDgiVxm5l+Yct/mGx21PuOWI8uLEzHEliOyrRZpYFL4WyATs71FziXmNRTJsA5SYPUJ4DM7fBChNcFIzXatII9KpX3hnnv+fkgv9N0AnltPKqLmtkj/WlGt9sCf2yPSLMwfPrwKi5XgjCGSx8jdwypoDAgdPCqn6e6vIXOQ9f7yM3CK6Sgwsq7fEP+wYdu4+GV+w9Eb17cpnz4H2zqh+r9tj3k7hE50gQMzjtQ9DaFZ3y/OHgmp29yYbZFZ5X60sLViys8SZ3RVJOdzbW+HaPsmxgKDE1IstViXSWMWAV/OA2qlEuT87RctkFbidoKrAcD1WFln23XFSyYtpE9+72jzoUXASNidNiWeZFVxZCmZ+HM85r/4dA0wx7dj/Dsy1c5ZEUhVMwub5swk6P07pTyMoz2k+fuv0fPdk5ekb1UpTmVVX8ACFRBikhzmRJ/cBrC1Z6XB9lCgo+vXsKd2x7hFIu9TMgigjebhm654Udx9aYTYrw1FVTl805r/g9jGgJKcm49U0cC6KigkRREPDYj274ccP87d3RRb/Y3La2tT92c1QmHllS7/vz5YXOD0Zg9IPGxgnMDtFWx0bDszoGo9fsOy2XKrJm0QmySEGIpwgOQxFRkjUNLQrYPi/0F7/s1MW9NeWFQBnnRxqGbGOBNtDM/8Lh4py5VuDUTwICSj3mg031Fx7sZIapWzyyu1RLFCGnnfDaLOjlAyd7dwh85r6FtapPFGHDAL5SKJjpoSGS1Xx/3NK2bnNL35IlDcWvP3nltAcLzGwkjrcV9dvj8cgwXtBBVBDMqvS+u37Z7E/X72xd/9qHB15KxALzaprKfnJTrWk4jjjFpDBHll5YfmSAD6xPb+unFrrSTMBKTBxMZqxOiwlkxnZqbZQaeaCpWNvbm4LooACyqmFZ43MVnnPsw4KQcWtl8O6raZrVRA9aJGKQd1rBbeGBo0hDGw/3PCQdQUU6CYPdBHyhQ+XaHd1vd0ajU3+2oO6xO2dXraZpGjIYWSdy5JczFesoT0crMDPxdTdcdENNkX3l01u6H+8eFqqevGLaD6cUsz1VvGJkS4KMvQN0jCFrFoboxqKC+MBiARitEVAOhTnXixgX4fh/WLiZr6Gc8CA+xs4Bb9FSXIQ6VgdJ1vh1W7ve6xxKTH1q/rTbH5pbudqBCxmQwUarYCN1YDHofpZvivLy7tg84f45tU+sXFj/087+0fN/vfnAW1pGNZ/n5AzjAy2PX+koV+x9dZz74H59mZhz7JU1nmVUmDjD8juAmOAAFxDSJZHErsWU95W7Lip6WSfwXswYaR9N6EZPGjcrFIqAQdzBOcMy9KIBGQ6at15cti4lZv0xIVPCAJVNijmGiJbX5/p/rIEgS54o93g/60gXacPhun8BqMRVmFFA8HgAAAAASUVORK5CYII=</t>
-  </si>
-  <si>
-    <t>UNICEF</t>
-  </si>
-  <si>
-    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAFoAAABaCAYAAAA4qEECAAAWnElEQVR4nNWdCZhVxZXH/wVNI5vIoiCIIoK4xSgkIS6BKHEDNUqMDoiRiUSjcRIVHJwYFzSJG4mSSFxQ0TGOiaIEt8jiEtQ44gbioKK4IK20gNBAQ8vSN1/d+6vu6tv3vXfv627oOd/3vn7vLnWrzj11zv8sVW1k6dE1ap4UlEimr6R9Je0uqZuknehqlaQvJH0maYmkDyRtzT2MQJKJ/XZkkm9pLBrRSSXNkL9tJR0n6STJHCSpWlKppENzXL9IUqWkFpIWS3pC0tMcazbUohn1ZR9Jv5b0rqT7JJVJukrS3xC/uZLWSvoSSa6QNAcpfkrSNZKWSbpL0nuSrqPNZkHNQaK7SLpU0g8k/S/MPhemneedP1rSBkkfS9oiqZekTyU9DpO/KWmGpA8lTeP3LEmPSLpJ0qodOcgdLdEnSnpJ0tcknSrpLEl3og7s376okXWSfizpJ5I2SdrGyxhJO8eiw+9BX98q6WxJp9D2S5I5aUcOdEcy+mZJt0u6QtJwSW9j6P4i6RBJJ2Dg/inp75KmIpWt0dnrJd0maSYzwaqT4yX1seadtmybwyT9UtItSPYOocZGHQdK+r8C11hGTZfUWdIoSZ9wvJ2kh1Fno7yp/qCk73GdQXItfc7fHpJelXQyv3eR9BBG9QReSFv0+OGomjOloKput+ohj4OwF3mQTEoa0alRJXoKUzsfWSmbLekrSUfAvA7ANsuM8agBx+S+MMceG4q6eJnPTzl2lKQBkg7gnrVI8VJmxw8lLUS394ejcz2YmIusKntAUsvGYE5jMdpO/wskvZbnmpZM6RWSTkN/WkO1AJ1smTcRBnbkngmS5kvBm6CM1zF2S5HitUidZdzl3rOsFN4Nwx+k3TGSPpJ0hqQ1kpkpmZKI74k42qqs0yX9oTEY1Bio43Ssvp2i8+qcCXAKTDiQyUjRqUCwc2Lt7Aocsy/hF5KuxqitjDEiQTiCiyRjX9RgST0l/QhdPRH938G7eAtS/o9QbwfBhTVnjHymzwfVXABcbBDDG8poO+Un8f0ZIFktmZpOnwbCOAgDOKZAu/sx7a+UdK2kndHF69DlAQztGsE804drZmIAZ0UoJfhcMtZ5eUwKXoxmTtinKvT+xzLmeWwGzToPMlgvmSeZYRNp871iGdVQY2iZ8Cu+j4Q5lvaKmB6KdFfJvBEZoFCynsz4jBuRpicRjO5wYwXooxKV8AnSOyDBK/wtjP0Wv63BvBidb+3FQEmrccv3kUwl7Q9FLSmahQE2KKPLXqQx7AjDWqFnhRQ9jIRbPTw6Ykao/6wKsCrlhZgeTUv/CfOGgKlnRhKqY2DcQCmwzs4l6PHjE9q9Bhsxhhdu1cIg2nROEgw0XVArxzJL59CGDQl0ZkZ1zTqIYhhtO/rvSFZ/jtlB7i/pRZj/EMdtMOj7ksbRuQPytJuPxsHEssiQhUZwBccCT8KexwbEx7gLRnca+v8SXsgSDO4pobqKbMqrtPt37MilOEhWiPpJxkLGn2cdQDGMPhWd2x2pvplBPwscu1/S+0zDX9DhclzptkU8TxjJdnxvmaffD6EGfONXzbHNqJcbCDw5+oTfF/O+AhyhFhjtQ5hVAvufmPAyC1JWRreJ3mromJRiCG9AbeyKe4z3ZXqgM3/nDbg6awehbd69Br0ap47Av+O55tvMvtHMAvvSD4teehBXspOi+8ye/LaQ8C2+/wmo9xsQyzck9UZwUlNW1NENFdAOg2On1fWeCpmqQG8jGSfjvTlLvRbUUMhRSKJFvERLGyN9GfalA592MOJZpO3HxDh8WkbQaXIsGC36WBYKRqDbZEJUcgMOS1svTLA3hr4931enHUBWie7uTeEuMO1Mfi9REKIQN4zja2FTSKsjlZKZtnqzwu/zaiT4YV74+3idNycw2dKeSPXrkrkg4fyM0ADWyvr/YHiFYexH+KA9x3pmGUhWRrfzvndBf+0BM8bKaBWOVicMoQ/lqjFWWem22H2tQB3jiTnfhTQ+hcNSiDoRLpgam11P0OfOHm9+RrDKzvwjPY9Vse8FKSujfR3bGeMnJKUV8WNLBzPV4xLcKePztuDgRJA8QgW/QV052g8m98vY9ljadjx4H0fmYH7/G3p+NL97x2DdtiwPix4SpPhEtIrBC6aVMuhnmGYusrYvuTy/MyOAhVmolaf/oaAtaa3Tkcr5GOdiyMas/4MBbqXP/fndHhRj7cqFoBZfUMqzPC+rMfw4ij2E7rCV6D/yil6mY+9wXU8vjGmh2Y0wOivNURBafN+d/28ido1F10pmBsZyRTS28FnvIojTQRobvPhMJecT7GoyRRJtUnwiF7sTTBX3biCv9zWm3QLO2euW4wjY64thskIjaIJymTqDKUbP56MOXnh3FTBVxNXLsUE3xtz6BUj42LTMy6KjB4Ep7+D3l3RqLL8XRuHLUA9VMy2nex3PR3FcvJlgzuxYGHMwurOx6Yc8ZA2+gh3DatxzEVrt78G5W3Hrj0vbjyyMrgRLlgB9PmTQTm89Hem5kDEBYco0QfM/YICG4GpfT2bkjoTii8Nw9Rub9lYQ7MYL9ulpvrcmTrKMKJ5LHG9I248sOto5DNfgMGzDGAmGPOVdW5Vwfy56nZjDknrx7Lo0mrBpU1CpjNkdaWZ2hUZhFg5SW2bTJBjuxh1/MTkpi0Sv4O83sPor8Y5EtKscD0p4gWnpyBTXGQZabKwkDe2EgXfq4b8QxBn87o1q6U68Q57BL0hZGL0wwtHhbJ4A9HKqYQoRrZ/xe3mGdg9JEeA9xrMFEfmQNE5BwnX+72TaDBPLODsSzO6kt4QXPc67e0HO1mKUhdGLI5wZ8uQ7hDzL0dUfEETfien3YYZ2e3veWC7qX+94XaNe/1z8uqRztbQJvNzLc7JKiVJuZcauAda6yF1FgRxpHcpqDJ/hewsqi+Yh3cPA0QbXdLGnagpRFwYYozpe1Ax0eFPREvremZm7EzPWINkTcdGP9sIQr2SZuVld8MlencMY4gzT68Zng5ZIxysZ+rBH/cN1RHE5qah8xrIhdB9ZnHIvtuHoRJIBVzFrHd2c5XlZGf0maXwhhf2QApc52SIZ56LPztDubrlP1TD8UyKCd2bscyGqgNGjvBm7zcP2ewJV7d+vc2ymB/1SURZGtyCmcDGBcIFre3pooLIWWwZPA43SUNpg0ybS/y9kYmV+uoT4zaFEBW3fN3kY2RD7HgQP3iVms18WeJyF0QHI4o/orecwij7kWomuHiKZD72seCE6OgezewMZB+M0CGmbkqHf+eg6CiMnoB4WR5VRYXZopXdfCZVVC/AhJnBv6oxRFofFOSV/w/qehV5bh6S18cqu/sy5SRSzFHrOMCz4y+jIlVj5X6KilvOc0whclRVorxBt4gX+Tgo6SmYM8Zg2BK0upYTB0Xps0UQy5mcT0WsSRssrkrEu8l+jv2GhyXvg4Y/QZ3tE4cfQk7PXnZmi7T58ksgZyzZRTNpUyISSnbUurpoy4QnRSw3bugqkYcOt5xNt7OcVX37K+Y04LyfhkD2S5cFZjeEGppqYSrMk05bYh+iQY9aZwCRby5HFU8xF74QRtShcuiwlfCwjZjKV2XEYaogIpDkU1/5idLGroNqfPKVgaKXHZCE8aeFrSMWUG0z28ONhJDDvRlJe8HJpfUjQWsm4LKGdfPGQKtSQu2ZN5JEFERIwIVJ4NUVf50RRwOBcdOr82lNBK/p+Ezj6CMIL8kqBXwbG3eoxuYLKp0yE6kgXvIbWSuZSUvIi5ryUyF4FHpWjUWQp7iRYfwbHV6N+BjK4UiTkfbzM5cQRemLxl8F4n9J0Go/TcwfdXcbcjxD8niMjPcErITZ9HOHa8702r61XY5iCiixyDP4imaM8AG/9/zdQIV94F36bKqG1BNf3poxrDhLzav1laXXovejjrjEdydsdw6cQDUbnLq25LnrULRjrQaCYUpCPI4c4vsVMcPSY92K2B6NDuoggjKu0n0yg3Pf/u9HZuVjuERjUKLdYI105n2EiZpjjYcr+JBLSRvF2oV8/8ByQSZSpDUElGdr1V3C9wgud6hncl6hQzTT9HTWE0ZswJNMYSFck5XxUiEvH24r9fljtadRI2LjBvdG0NEm6uhc6cRR2oCEF88MxXteiBqyUf5fpfypO2CpiG0LCZwHjXBj4OfqSumAmTgwgTd6rfh4MKXWF41/AnMO9mmnhtgaglZuAS4eH0m40Tya09Mdy77m4wwtxSo5opFUJ32em9WCGfUK8+VGE7evetXcTEjgP7H41amVFQ3jV0EH0QUo/541PoVO3oLPdNe/A7PE4PC2k4AQcoDuRoMeAYj8qov6jEFUAM4czs+7xkMN8Lz32kRRcjv6/F+P9Bi8/18rdVNRQRn9ENO8hOlNFNekGJPQN1MYyz9M6mRq53kjLwUhWsQWQ+aiatg+HsV14ua6+5EtiF/sQQx+OGnmUmTcFAeji4eqiqKGMDgD7bwPFxmH4pmFEBpFjLENPOhoomWcVhJL0Ljr+SKQ9S74xF1XBoMG0vRi1MZdwq6OnUCO3I7HlkpmMwb6C2ViGGmnQMrhIgTzSwHWGJsTCz7COxNEaAlA2PlBNFebbXpGgkPSTvBJZUeU0DIQyIFbvl48qCePOoObPX2+yN8f8DHoAhncq7mJiHLt712ylf5lCovVoRKdGYrRCZp9CQKZD7IyNeF3uTdl7YueX4hgsVX3qQzhyn2jG2JIA46DdRgxwGdP+nRwptN0ohh8QO/4rcoJHgpXjSeKtoJS71VCqYXRDV87W+hzfAXvGc3zbKL2dQFnV72PS/xoGqEBMJK9zk0St0bfDvHNfEey6kf5cmYDLy4Cpj2d5WE5qtP06asf+Ao7AeFxaF/doyfKE/rjs/wCDD8ABKcU4ps4qp6RutP8KGHghhnsBCOfcWDOrCCLdEAuTNpiacgearjDdYtROIJFyUEkVEt0TRrSH2dtwhNYDyVahHjYVeFZrVEQXntWB2HIJ2ZNK3GoX1zbAyB44VhXYj3lFx7rzTbYm3oHGSYfNr/VD17o9NfoS8GldoI013hrCZzG4rmK1Lx7eUL7vlaLObzPq6UNc6vm0934joZ2ctD32VLJSfR2udBZajfFcRuTvBGbHWzBlELBtFrCtA7Byr4zPWRjp6eCx2kNF7LFUQKKTGZ3Z5hSkEmIKxyCBByLRcei2lZkwm1iDv2JgIDjbZVsqwMjPeNf0AOGc5C3P82kTs+RdZshsHJGqBm9mVTSji3xeSmqPDt8VSSxFSlejR/0OtSIgNIGa5Z8A7f6Ex3cXmez13j0780K6oqu3YiNW8iLXJXPKUeMzOr+ObnzJdrTB2x8p34P7AReHEBOZ4EHA7wHNLkP3n0NlqmDk4ibpeZFU2AUvKvraEKp54CB07xAYfF4MZ28iAjcW3T07xzrwZkHNaTs2KAwtDsaT7EnC9MY8N9yNTi4F4WRePrw9qIGMbhJxH4hT0RnUcV+Ke55g9UE1NSVDm6JjDaFmKNGhiuhGkOf+3EXQ9ehJlia35d5mNbbmuGXmZYRUgW2ZrPGDJCGWFB/fbhrr3xwZ/WUMG2elIpfHNe1GsE3L6KLxeNPhyu1ALqzbGqGxLn75DpbovLr3NALz1ejbhz2c3PzIhPHsX5P8beP1zyYNTtjBjDb5mH2aV9mkMDEQBMmMNmmkP0j8mu7egjQQY7xzwoVhkX1z1NGO4qHRLYlXNQ8N89sYk93G4cZljpoBo3NKdXV8I7pkpu5wTu+KRDu6j9rpOqtqm4lEJzL7agU1uycYGRuTjjN1u8cHkigehZyStHS5GamOesz+lM//Byr4xpuZZ2i8pYVuf8JmivRys7ZF3WuiC7e3RPfis43cXJalzIWolCVqHcl0fwaOzUJdqesoJSZelmPrN5/i23NGK9FiL8Ix+kJKBQLyaIVqgK+M1haG2Oi5mn2PIpB+EwaiRbTxVPC8ZIazTvxwr8p0LWmpR9mgKtopoBZuHUFAv5rBXJSjHOFAlsR9l0KZNrzIcvKCt9HHfHQWWfsBXt83kkabR4TQWy0Qpssm8r1jrPj+ehLKhnZs5dPrLsPyiLdLzOwUG37MJ9gu4guj+N6eZKrb5Gksx24p0N5zrHmJdguIzN9ZFOQozJAEobRG52tVyXmUBuTbsWtrVCwT3FBzpFbausiYu7w9VnPRJkrb3KZZ34wxPh+N1ohODziJ9jFrodS+Ygs1/exxgMV1jD6VwsHNSO5rTMU+DM7VHx/FWpFRoQRHjPRx8waZelrxTG8mifjII6ijXmxuNYRZe71kyhSEIVT2bbFSaB7whKqCUogX6e8BXllaGxLMX9HPlYRyA/DzsV7B+lzSZS0QCYunm1xHD2fgIxmATzcRR3alWmcwzV7O3VwN9YxtnH0ri039lzGVtYFuRcK1MmGpQyVTYrzH5HKu86V0Bky9l62ARO7ycZjnvNY9SfY6t3s8mfU61NSo4ysqkuJMFmrg0tiWbZE6SgpB1z02ztt64hNSXfE7tsTWn/RG74t493jv3PgcqmAjL9Cty2nn7e3nqE3sd+KWoE3N6AWUf9WniHH/jJVeRcxLgnS1x3aObWD15zxrzheTOa8gYetqAv0l0WXe1phJtCJWg3d0MXxratVRbwrVUMS0KvQdO0IilG4zXJ/ZtZHT/rHS2uQXGdG6kDFBiAqsd7mOhvwa6ddipQpJ5NcE9lAQGt81WfB9UzM6I05O1XN/GXN1ihWsX9T9GeLHg7wD/UAuuZY7b/MWeipUHyasRclU3tXUjE6DYDxKlSno5n3fnLpmrrbJ1rG9nw/IuFN7hxhuTkVNzeigvo3Kx0QT20k+8TZ/kEHh3KBrr6aBlrFxr6T0LK3ercouQMUzulAVaFOSHxlrVURftsRmwcwU/xGpLhWRonNv0SQcy0UlrEhN16P4Tr5pRpAL3kXk6+SSFPs4t+RltObFbI7tlBtfClKYigh0OYn2sWwhJnaPWf08ZBTbwDX9QHIf+8DLI4pysDxOjplGeZnw5q5gUZHb1PtA+JBv1dXJnh5fSXlwpnIG19nPvGPRhlSJ/AkPDs26G3hmyu+wfBBbWDQyT/NdKRfbl4/7pzZzvGv29zbnTqJWBNmu4zOmmJoRx+g3vWPdo61skjhtdqGwsIko1Xys8nb8FVHHqN6ufpfP9mboRgWaAUaf51WytqS2Lxe8GxFbkH9XMWN3jJ7rbW2jMARozDme/tqJIvK5OAwJ2DWXEk5cQ95Qut37v4mGeMTPyTiXAAHHEZtwdIc3xvW4/46GsgD0MG9zwR6EX/2Nsuy2F38tJoXm/wcI/8EdeHOL2FfjLcKnA7luXv02ahjpS0YazvrG13hN+fe2rGk+ep+VqAzHuJ3DgJQJ+7mQfk/y4hDTw61+6r7r6Wwa6GgYq8oWMd5FMNlh7jdx/eO43cTQW+KY/UE+TPzYl9a98Irceu6fMoBqYNKWhK19N3FsS2RgCsKOr+peX9PPrR5m3VBzc+0wFjHL7vdwbTeMlls0tDxaahGMzuHYXEPQy7nYLQkH7OcFrT6v/Yc4iQtGt3m7mq3JZVSTllb0YpvIvkyhddE0DexGVS411NNTK/zfqpAPLSTTu2ZfzyD4ol46qd77Dv+bj1tQaeO47r9z2oTB7grCMgM7GPuiI3RUv2LMqjObvbFttZYCGwq1tRU2obAqRYlZqRQMloxbqmcvtoEo68jYLI3nxtdrq0QKXFbGeke2/3WFb0Qn/QvcZelNrG4ztAAAAABJRU5ErkJggg==</t>
   </si>
 </sst>
 </file>
@@ -433,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D23" sqref="D23:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,7 +465,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
@@ -467,90 +473,98 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>